<commit_message>
added initial date input and changes in UI
</commit_message>
<xml_diff>
--- a/COVID Simulator v 1.1/Input/Input_Simulador.xlsx
+++ b/COVID Simulator v 1.1/Input/Input_Simulador.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignacio.brottier\Documents\COVID 19\COVID-19-Simulation-Argentina\COVID Contagio Argentina Monte Carlo\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignacio.brottier\Documents\COVID 19\COVID-19-Simulation-Argentina\COVID Simulator v 1.1\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{442AFCD7-AA7C-4EDE-811B-B126B37AB8E1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF8274AA-8A1E-43AD-B5B6-2300EE290271}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29040" windowHeight="15750" activeTab="5" xr2:uid="{55AC4C4C-7526-4060-9BB2-10E89010456B}"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="29040" windowHeight="15750" firstSheet="6" activeTab="8" xr2:uid="{55AC4C4C-7526-4060-9BB2-10E89010456B}"/>
   </bookViews>
   <sheets>
     <sheet name="Información" sheetId="28" r:id="rId1"/>
@@ -22,14 +22,15 @@
     <sheet name="Tipos de Movimiento" sheetId="14" r:id="rId7"/>
     <sheet name="Capacidad Sanitaria" sheetId="30" r:id="rId8"/>
     <sheet name="Estado Inicial" sheetId="31" r:id="rId9"/>
-    <sheet name="Enfermedad" sheetId="4" r:id="rId10"/>
-    <sheet name="ProbabilidadadecontraerVirus" sheetId="11" r:id="rId11"/>
-    <sheet name="Efecto Severidad en Letalidad" sheetId="16" r:id="rId12"/>
-    <sheet name="Tasa de Letalidad Moderada" sheetId="17" r:id="rId13"/>
-    <sheet name="Tasa de Letalidad Grave" sheetId="18" r:id="rId14"/>
-    <sheet name="Agravamiento" sheetId="19" r:id="rId15"/>
-    <sheet name="Tasa de Enfermedad Moderada" sheetId="20" r:id="rId16"/>
-    <sheet name="Tasa de Enfermedad Grave" sheetId="21" r:id="rId17"/>
+    <sheet name="Estimación Efecto Politicas" sheetId="33" r:id="rId10"/>
+    <sheet name="Enfermedad" sheetId="4" r:id="rId11"/>
+    <sheet name="ProbabilidadadecontraerVirus" sheetId="11" r:id="rId12"/>
+    <sheet name="Efecto Severidad en Letalidad" sheetId="16" r:id="rId13"/>
+    <sheet name="Tasa de Letalidad Moderada" sheetId="17" r:id="rId14"/>
+    <sheet name="Tasa de Letalidad Grave" sheetId="18" r:id="rId15"/>
+    <sheet name="Agravamiento" sheetId="19" r:id="rId16"/>
+    <sheet name="Tasa de Enfermedad Moderada" sheetId="20" r:id="rId17"/>
+    <sheet name="Tasa de Enfermedad Grave" sheetId="21" r:id="rId18"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Perfil Etário'!$A$1:$F$2725</definedName>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="233">
   <si>
     <t>Santa Fe</t>
   </si>
@@ -1594,6 +1595,45 @@
   <si>
     <t>Probabilidad de Ingreso Infectado</t>
   </si>
+  <si>
+    <t>Cierre de escuelas</t>
+  </si>
+  <si>
+    <t>Cierre de espectáculos</t>
+  </si>
+  <si>
+    <t>Cierre de fronteras</t>
+  </si>
+  <si>
+    <t>Licencias y home office</t>
+  </si>
+  <si>
+    <t>Limitaciones drásticas al transporte</t>
+  </si>
+  <si>
+    <t>Recomendación de aislamiento</t>
+  </si>
+  <si>
+    <t>Restricciones al transporte público</t>
+  </si>
+  <si>
+    <t>Supervisión de ingreso de pasajeros</t>
+  </si>
+  <si>
+    <t>1. Política Aplicada</t>
+  </si>
+  <si>
+    <t>2. Reducción de R0</t>
+  </si>
+  <si>
+    <t>7. Capacidad de Testeo por Dia</t>
+  </si>
+  <si>
+    <t>5. Fecha Inicial [dd/mm/aaaa]</t>
+  </si>
+  <si>
+    <t>03/03/2020</t>
+  </si>
 </sst>
 </file>
 
@@ -1607,7 +1647,7 @@
     <numFmt numFmtId="167" formatCode="0.0000"/>
     <numFmt numFmtId="168" formatCode="0.000"/>
   </numFmts>
-  <fonts count="31">
+  <fonts count="32">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1819,8 +1859,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1866,6 +1911,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2020,7 +2071,7 @@
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2252,32 +2303,11 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2288,10 +2318,16 @@
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2303,9 +2339,35 @@
     <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Comma" xfId="7" builtinId="3"/>
@@ -2758,22 +2820,22 @@
   <sheetData>
     <row r="1" spans="2:45" s="9" customFormat="1"/>
     <row r="2" spans="2:45" s="9" customFormat="1" ht="33.75" customHeight="1" thickBot="1">
-      <c r="B2" s="110" t="s">
+      <c r="B2" s="103" t="s">
         <v>105</v>
       </c>
-      <c r="C2" s="110"/>
-      <c r="D2" s="110"/>
-      <c r="E2" s="110"/>
-      <c r="F2" s="110"/>
-      <c r="G2" s="110"/>
-      <c r="H2" s="110"/>
-      <c r="I2" s="110"/>
-      <c r="J2" s="110"/>
-      <c r="K2" s="110"/>
-      <c r="L2" s="110"/>
-      <c r="M2" s="110"/>
-      <c r="N2" s="110"/>
-      <c r="O2" s="110"/>
+      <c r="C2" s="103"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="103"/>
+      <c r="F2" s="103"/>
+      <c r="G2" s="103"/>
+      <c r="H2" s="103"/>
+      <c r="I2" s="103"/>
+      <c r="J2" s="103"/>
+      <c r="K2" s="103"/>
+      <c r="L2" s="103"/>
+      <c r="M2" s="103"/>
+      <c r="N2" s="103"/>
+      <c r="O2" s="103"/>
       <c r="Q2" s="57"/>
       <c r="R2" s="57"/>
       <c r="S2" s="57"/>
@@ -2791,248 +2853,248 @@
     </row>
     <row r="3" spans="2:45" ht="15.75" thickTop="1"/>
     <row r="4" spans="2:45" ht="15" customHeight="1">
-      <c r="B4" s="106" t="s">
+      <c r="B4" s="101" t="s">
         <v>99</v>
       </c>
-      <c r="C4" s="106"/>
-      <c r="D4" s="106"/>
-      <c r="E4" s="106"/>
-      <c r="F4" s="106"/>
-      <c r="G4" s="106"/>
-      <c r="H4" s="106"/>
-      <c r="I4" s="106"/>
-      <c r="J4" s="106"/>
-      <c r="K4" s="106"/>
-      <c r="L4" s="106"/>
-      <c r="M4" s="106"/>
-      <c r="N4" s="106"/>
-      <c r="O4" s="106"/>
+      <c r="C4" s="101"/>
+      <c r="D4" s="101"/>
+      <c r="E4" s="101"/>
+      <c r="F4" s="101"/>
+      <c r="G4" s="101"/>
+      <c r="H4" s="101"/>
+      <c r="I4" s="101"/>
+      <c r="J4" s="101"/>
+      <c r="K4" s="101"/>
+      <c r="L4" s="101"/>
+      <c r="M4" s="101"/>
+      <c r="N4" s="101"/>
+      <c r="O4" s="101"/>
     </row>
     <row r="5" spans="2:45" ht="22.5" customHeight="1">
-      <c r="B5" s="106"/>
-      <c r="C5" s="106"/>
-      <c r="D5" s="106"/>
-      <c r="E5" s="106"/>
-      <c r="F5" s="106"/>
-      <c r="G5" s="106"/>
-      <c r="H5" s="106"/>
-      <c r="I5" s="106"/>
-      <c r="J5" s="106"/>
-      <c r="K5" s="106"/>
-      <c r="L5" s="106"/>
-      <c r="M5" s="106"/>
-      <c r="N5" s="106"/>
-      <c r="O5" s="106"/>
-      <c r="Q5" s="114" t="s">
+      <c r="B5" s="101"/>
+      <c r="C5" s="101"/>
+      <c r="D5" s="101"/>
+      <c r="E5" s="101"/>
+      <c r="F5" s="101"/>
+      <c r="G5" s="101"/>
+      <c r="H5" s="101"/>
+      <c r="I5" s="101"/>
+      <c r="J5" s="101"/>
+      <c r="K5" s="101"/>
+      <c r="L5" s="101"/>
+      <c r="M5" s="101"/>
+      <c r="N5" s="101"/>
+      <c r="O5" s="101"/>
+      <c r="Q5" s="108" t="s">
         <v>173</v>
       </c>
-      <c r="R5" s="114"/>
-      <c r="S5" s="114"/>
-      <c r="T5" s="114"/>
-      <c r="U5" s="114"/>
-      <c r="V5" s="114"/>
-      <c r="W5" s="114"/>
-      <c r="X5" s="114"/>
-      <c r="Y5" s="114"/>
-      <c r="Z5" s="114"/>
-      <c r="AA5" s="114"/>
-      <c r="AB5" s="114"/>
-      <c r="AC5" s="114"/>
-      <c r="AD5" s="114"/>
+      <c r="R5" s="108"/>
+      <c r="S5" s="108"/>
+      <c r="T5" s="108"/>
+      <c r="U5" s="108"/>
+      <c r="V5" s="108"/>
+      <c r="W5" s="108"/>
+      <c r="X5" s="108"/>
+      <c r="Y5" s="108"/>
+      <c r="Z5" s="108"/>
+      <c r="AA5" s="108"/>
+      <c r="AB5" s="108"/>
+      <c r="AC5" s="108"/>
+      <c r="AD5" s="108"/>
       <c r="AQ5" s="9"/>
       <c r="AR5" s="9"/>
       <c r="AS5" s="9"/>
     </row>
     <row r="6" spans="2:45">
-      <c r="Q6" s="113" t="s">
+      <c r="Q6" s="107" t="s">
         <v>174</v>
       </c>
-      <c r="R6" s="113"/>
-      <c r="S6" s="113"/>
-      <c r="T6" s="113"/>
-      <c r="U6" s="113"/>
-      <c r="V6" s="113"/>
-      <c r="W6" s="113"/>
-      <c r="X6" s="113"/>
-      <c r="Y6" s="113"/>
-      <c r="Z6" s="113"/>
-      <c r="AA6" s="113"/>
-      <c r="AB6" s="113"/>
-      <c r="AC6" s="113"/>
-      <c r="AD6" s="113"/>
+      <c r="R6" s="107"/>
+      <c r="S6" s="107"/>
+      <c r="T6" s="107"/>
+      <c r="U6" s="107"/>
+      <c r="V6" s="107"/>
+      <c r="W6" s="107"/>
+      <c r="X6" s="107"/>
+      <c r="Y6" s="107"/>
+      <c r="Z6" s="107"/>
+      <c r="AA6" s="107"/>
+      <c r="AB6" s="107"/>
+      <c r="AC6" s="107"/>
+      <c r="AD6" s="107"/>
     </row>
     <row r="7" spans="2:45">
-      <c r="Q7" s="113"/>
-      <c r="R7" s="113"/>
-      <c r="S7" s="113"/>
-      <c r="T7" s="113"/>
-      <c r="U7" s="113"/>
-      <c r="V7" s="113"/>
-      <c r="W7" s="113"/>
-      <c r="X7" s="113"/>
-      <c r="Y7" s="113"/>
-      <c r="Z7" s="113"/>
-      <c r="AA7" s="113"/>
-      <c r="AB7" s="113"/>
-      <c r="AC7" s="113"/>
-      <c r="AD7" s="113"/>
+      <c r="Q7" s="107"/>
+      <c r="R7" s="107"/>
+      <c r="S7" s="107"/>
+      <c r="T7" s="107"/>
+      <c r="U7" s="107"/>
+      <c r="V7" s="107"/>
+      <c r="W7" s="107"/>
+      <c r="X7" s="107"/>
+      <c r="Y7" s="107"/>
+      <c r="Z7" s="107"/>
+      <c r="AA7" s="107"/>
+      <c r="AB7" s="107"/>
+      <c r="AC7" s="107"/>
+      <c r="AD7" s="107"/>
     </row>
     <row r="8" spans="2:45" ht="15" customHeight="1">
-      <c r="B8" s="106" t="s">
+      <c r="B8" s="101" t="s">
         <v>103</v>
       </c>
-      <c r="C8" s="106"/>
-      <c r="D8" s="106"/>
-      <c r="E8" s="106"/>
-      <c r="F8" s="106"/>
-      <c r="G8" s="106"/>
-      <c r="H8" s="106"/>
-      <c r="I8" s="106"/>
-      <c r="J8" s="106"/>
-      <c r="K8" s="106"/>
-      <c r="L8" s="106"/>
-      <c r="M8" s="106"/>
-      <c r="N8" s="106"/>
-      <c r="O8" s="106"/>
-      <c r="Q8" s="113"/>
-      <c r="R8" s="113"/>
-      <c r="S8" s="113"/>
-      <c r="T8" s="113"/>
-      <c r="U8" s="113"/>
-      <c r="V8" s="113"/>
-      <c r="W8" s="113"/>
-      <c r="X8" s="113"/>
-      <c r="Y8" s="113"/>
-      <c r="Z8" s="113"/>
-      <c r="AA8" s="113"/>
-      <c r="AB8" s="113"/>
-      <c r="AC8" s="113"/>
-      <c r="AD8" s="113"/>
+      <c r="C8" s="101"/>
+      <c r="D8" s="101"/>
+      <c r="E8" s="101"/>
+      <c r="F8" s="101"/>
+      <c r="G8" s="101"/>
+      <c r="H8" s="101"/>
+      <c r="I8" s="101"/>
+      <c r="J8" s="101"/>
+      <c r="K8" s="101"/>
+      <c r="L8" s="101"/>
+      <c r="M8" s="101"/>
+      <c r="N8" s="101"/>
+      <c r="O8" s="101"/>
+      <c r="Q8" s="107"/>
+      <c r="R8" s="107"/>
+      <c r="S8" s="107"/>
+      <c r="T8" s="107"/>
+      <c r="U8" s="107"/>
+      <c r="V8" s="107"/>
+      <c r="W8" s="107"/>
+      <c r="X8" s="107"/>
+      <c r="Y8" s="107"/>
+      <c r="Z8" s="107"/>
+      <c r="AA8" s="107"/>
+      <c r="AB8" s="107"/>
+      <c r="AC8" s="107"/>
+      <c r="AD8" s="107"/>
     </row>
     <row r="9" spans="2:45" ht="17.25" customHeight="1">
-      <c r="B9" s="106"/>
-      <c r="C9" s="106"/>
-      <c r="D9" s="106"/>
-      <c r="E9" s="106"/>
-      <c r="F9" s="106"/>
-      <c r="G9" s="106"/>
-      <c r="H9" s="106"/>
-      <c r="I9" s="106"/>
-      <c r="J9" s="106"/>
-      <c r="K9" s="106"/>
-      <c r="L9" s="106"/>
-      <c r="M9" s="106"/>
-      <c r="N9" s="106"/>
-      <c r="O9" s="106"/>
+      <c r="B9" s="101"/>
+      <c r="C9" s="101"/>
+      <c r="D9" s="101"/>
+      <c r="E9" s="101"/>
+      <c r="F9" s="101"/>
+      <c r="G9" s="101"/>
+      <c r="H9" s="101"/>
+      <c r="I9" s="101"/>
+      <c r="J9" s="101"/>
+      <c r="K9" s="101"/>
+      <c r="L9" s="101"/>
+      <c r="M9" s="101"/>
+      <c r="N9" s="101"/>
+      <c r="O9" s="101"/>
     </row>
     <row r="12" spans="2:45" ht="17.25" customHeight="1">
       <c r="D12" s="15" t="s">
         <v>96</v>
       </c>
       <c r="H12" s="17"/>
-      <c r="I12" s="111" t="s">
+      <c r="I12" s="104" t="s">
         <v>100</v>
       </c>
-      <c r="J12" s="112"/>
-      <c r="K12" s="112"/>
-      <c r="L12" s="112"/>
-      <c r="M12" s="112"/>
+      <c r="J12" s="105"/>
+      <c r="K12" s="105"/>
+      <c r="L12" s="105"/>
+      <c r="M12" s="105"/>
     </row>
     <row r="13" spans="2:45" ht="17.25">
       <c r="D13" s="11" t="s">
         <v>104</v>
       </c>
       <c r="H13" s="17"/>
-      <c r="I13" s="111"/>
-      <c r="J13" s="112"/>
-      <c r="K13" s="112"/>
-      <c r="L13" s="112"/>
-      <c r="M13" s="112"/>
+      <c r="I13" s="104"/>
+      <c r="J13" s="105"/>
+      <c r="K13" s="105"/>
+      <c r="L13" s="105"/>
+      <c r="M13" s="105"/>
     </row>
     <row r="14" spans="2:45" ht="17.25">
       <c r="D14" s="13" t="s">
         <v>97</v>
       </c>
       <c r="H14" s="17"/>
-      <c r="I14" s="111"/>
-      <c r="J14" s="112"/>
-      <c r="K14" s="112"/>
-      <c r="L14" s="112"/>
-      <c r="M14" s="112"/>
+      <c r="I14" s="104"/>
+      <c r="J14" s="105"/>
+      <c r="K14" s="105"/>
+      <c r="L14" s="105"/>
+      <c r="M14" s="105"/>
     </row>
     <row r="15" spans="2:45" ht="17.25" customHeight="1">
       <c r="D15" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="I15" s="111"/>
-      <c r="J15" s="112"/>
-      <c r="K15" s="112"/>
-      <c r="L15" s="112"/>
-      <c r="M15" s="112"/>
+      <c r="I15" s="104"/>
+      <c r="J15" s="105"/>
+      <c r="K15" s="105"/>
+      <c r="L15" s="105"/>
+      <c r="M15" s="105"/>
     </row>
     <row r="17" spans="2:43" ht="17.25" customHeight="1">
       <c r="G17" s="18"/>
-      <c r="I17" s="111" t="s">
+      <c r="I17" s="104" t="s">
         <v>102</v>
       </c>
-      <c r="J17" s="112"/>
-      <c r="K17" s="112"/>
-      <c r="L17" s="112"/>
-      <c r="M17" s="112"/>
+      <c r="J17" s="105"/>
+      <c r="K17" s="105"/>
+      <c r="L17" s="105"/>
+      <c r="M17" s="105"/>
     </row>
     <row r="18" spans="2:43" ht="17.25">
       <c r="D18" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="I18" s="111"/>
-      <c r="J18" s="112"/>
-      <c r="K18" s="112"/>
-      <c r="L18" s="112"/>
-      <c r="M18" s="112"/>
+      <c r="I18" s="104"/>
+      <c r="J18" s="105"/>
+      <c r="K18" s="105"/>
+      <c r="L18" s="105"/>
+      <c r="M18" s="105"/>
     </row>
     <row r="19" spans="2:43" ht="15" customHeight="1">
-      <c r="I19" s="111"/>
-      <c r="J19" s="112"/>
-      <c r="K19" s="112"/>
-      <c r="L19" s="112"/>
-      <c r="M19" s="112"/>
+      <c r="I19" s="104"/>
+      <c r="J19" s="105"/>
+      <c r="K19" s="105"/>
+      <c r="L19" s="105"/>
+      <c r="M19" s="105"/>
     </row>
     <row r="22" spans="2:43">
-      <c r="B22" s="115" t="s">
+      <c r="B22" s="110" t="s">
         <v>139</v>
       </c>
-      <c r="C22" s="115"/>
-      <c r="D22" s="115"/>
-      <c r="E22" s="115"/>
-      <c r="F22" s="115"/>
-      <c r="G22" s="115"/>
-      <c r="H22" s="115"/>
-      <c r="I22" s="115"/>
-      <c r="J22" s="115"/>
-      <c r="K22" s="115"/>
-      <c r="L22" s="115"/>
-      <c r="M22" s="115"/>
-      <c r="N22" s="115"/>
-      <c r="O22" s="115"/>
+      <c r="C22" s="110"/>
+      <c r="D22" s="110"/>
+      <c r="E22" s="110"/>
+      <c r="F22" s="110"/>
+      <c r="G22" s="110"/>
+      <c r="H22" s="110"/>
+      <c r="I22" s="110"/>
+      <c r="J22" s="110"/>
+      <c r="K22" s="110"/>
+      <c r="L22" s="110"/>
+      <c r="M22" s="110"/>
+      <c r="N22" s="110"/>
+      <c r="O22" s="110"/>
     </row>
     <row r="23" spans="2:43" ht="15" customHeight="1"/>
     <row r="24" spans="2:43" ht="17.25">
-      <c r="B24" s="101" t="s">
+      <c r="B24" s="109" t="s">
         <v>96</v>
       </c>
-      <c r="C24" s="101"/>
-      <c r="D24" s="101"/>
-      <c r="E24" s="101"/>
-      <c r="F24" s="101"/>
-      <c r="G24" s="101"/>
-      <c r="H24" s="101"/>
-      <c r="I24" s="101"/>
-      <c r="J24" s="101"/>
-      <c r="K24" s="101"/>
-      <c r="L24" s="101"/>
-      <c r="M24" s="101"/>
-      <c r="N24" s="101"/>
-      <c r="O24" s="101"/>
+      <c r="C24" s="109"/>
+      <c r="D24" s="109"/>
+      <c r="E24" s="109"/>
+      <c r="F24" s="109"/>
+      <c r="G24" s="109"/>
+      <c r="H24" s="109"/>
+      <c r="I24" s="109"/>
+      <c r="J24" s="109"/>
+      <c r="K24" s="109"/>
+      <c r="L24" s="109"/>
+      <c r="M24" s="109"/>
+      <c r="N24" s="109"/>
+      <c r="O24" s="109"/>
     </row>
     <row r="25" spans="2:43">
       <c r="R25" s="23"/>
@@ -3053,37 +3115,37 @@
         <v>96</v>
       </c>
       <c r="R26" s="26"/>
-      <c r="S26" s="118" t="s">
+      <c r="S26" s="114" t="s">
         <v>106</v>
       </c>
-      <c r="T26" s="118"/>
-      <c r="U26" s="118"/>
-      <c r="V26" s="118"/>
-      <c r="W26" s="118"/>
-      <c r="X26" s="118"/>
-      <c r="Y26" s="118"/>
-      <c r="Z26" s="118"/>
-      <c r="AA26" s="118"/>
-      <c r="AB26" s="118"/>
+      <c r="T26" s="114"/>
+      <c r="U26" s="114"/>
+      <c r="V26" s="114"/>
+      <c r="W26" s="114"/>
+      <c r="X26" s="114"/>
+      <c r="Y26" s="114"/>
+      <c r="Z26" s="114"/>
+      <c r="AA26" s="114"/>
+      <c r="AB26" s="114"/>
       <c r="AC26" s="27"/>
     </row>
     <row r="27" spans="2:43" ht="15" customHeight="1">
-      <c r="B27" s="106" t="s">
+      <c r="B27" s="101" t="s">
         <v>117</v>
       </c>
-      <c r="C27" s="106"/>
-      <c r="D27" s="106"/>
-      <c r="E27" s="106"/>
-      <c r="F27" s="106"/>
-      <c r="G27" s="106"/>
-      <c r="H27" s="106"/>
-      <c r="I27" s="106"/>
-      <c r="J27" s="106"/>
-      <c r="K27" s="106"/>
-      <c r="L27" s="106"/>
-      <c r="M27" s="106"/>
-      <c r="N27" s="106"/>
-      <c r="O27" s="106"/>
+      <c r="C27" s="101"/>
+      <c r="D27" s="101"/>
+      <c r="E27" s="101"/>
+      <c r="F27" s="101"/>
+      <c r="G27" s="101"/>
+      <c r="H27" s="101"/>
+      <c r="I27" s="101"/>
+      <c r="J27" s="101"/>
+      <c r="K27" s="101"/>
+      <c r="L27" s="101"/>
+      <c r="M27" s="101"/>
+      <c r="N27" s="101"/>
+      <c r="O27" s="101"/>
       <c r="R27" s="26"/>
       <c r="S27" s="24"/>
       <c r="T27" s="24"/>
@@ -3108,51 +3170,51 @@
       <c r="AQ27" s="18"/>
     </row>
     <row r="28" spans="2:43" ht="15" customHeight="1">
-      <c r="B28" s="106"/>
-      <c r="C28" s="106"/>
-      <c r="D28" s="106"/>
-      <c r="E28" s="106"/>
-      <c r="F28" s="106"/>
-      <c r="G28" s="106"/>
-      <c r="H28" s="106"/>
-      <c r="I28" s="106"/>
-      <c r="J28" s="106"/>
-      <c r="K28" s="106"/>
-      <c r="L28" s="106"/>
-      <c r="M28" s="106"/>
-      <c r="N28" s="106"/>
-      <c r="O28" s="106"/>
+      <c r="B28" s="101"/>
+      <c r="C28" s="101"/>
+      <c r="D28" s="101"/>
+      <c r="E28" s="101"/>
+      <c r="F28" s="101"/>
+      <c r="G28" s="101"/>
+      <c r="H28" s="101"/>
+      <c r="I28" s="101"/>
+      <c r="J28" s="101"/>
+      <c r="K28" s="101"/>
+      <c r="L28" s="101"/>
+      <c r="M28" s="101"/>
+      <c r="N28" s="101"/>
+      <c r="O28" s="101"/>
       <c r="R28" s="26"/>
       <c r="AC28" s="27"/>
     </row>
     <row r="29" spans="2:43" ht="17.25">
-      <c r="B29" s="106"/>
-      <c r="C29" s="106"/>
-      <c r="D29" s="106"/>
-      <c r="E29" s="106"/>
-      <c r="F29" s="106"/>
-      <c r="G29" s="106"/>
-      <c r="H29" s="106"/>
-      <c r="I29" s="106"/>
-      <c r="J29" s="106"/>
-      <c r="K29" s="106"/>
-      <c r="L29" s="106"/>
-      <c r="M29" s="106"/>
-      <c r="N29" s="106"/>
-      <c r="O29" s="106"/>
+      <c r="B29" s="101"/>
+      <c r="C29" s="101"/>
+      <c r="D29" s="101"/>
+      <c r="E29" s="101"/>
+      <c r="F29" s="101"/>
+      <c r="G29" s="101"/>
+      <c r="H29" s="101"/>
+      <c r="I29" s="101"/>
+      <c r="J29" s="101"/>
+      <c r="K29" s="101"/>
+      <c r="L29" s="101"/>
+      <c r="M29" s="101"/>
+      <c r="N29" s="101"/>
+      <c r="O29" s="101"/>
       <c r="R29" s="26"/>
-      <c r="S29" s="109" t="s">
+      <c r="S29" s="113" t="s">
         <v>107</v>
       </c>
-      <c r="T29" s="109"/>
-      <c r="U29" s="109"/>
-      <c r="V29" s="109"/>
-      <c r="W29" s="109"/>
-      <c r="X29" s="109"/>
-      <c r="Y29" s="109"/>
-      <c r="Z29" s="109"/>
-      <c r="AA29" s="109"/>
-      <c r="AB29" s="109"/>
+      <c r="T29" s="113"/>
+      <c r="U29" s="113"/>
+      <c r="V29" s="113"/>
+      <c r="W29" s="113"/>
+      <c r="X29" s="113"/>
+      <c r="Y29" s="113"/>
+      <c r="Z29" s="113"/>
+      <c r="AA29" s="113"/>
+      <c r="AB29" s="113"/>
       <c r="AC29" s="27"/>
     </row>
     <row r="30" spans="2:43">
@@ -3170,52 +3232,52 @@
       <c r="AC30" s="27"/>
     </row>
     <row r="31" spans="2:43" ht="17.25">
-      <c r="B31" s="106" t="s">
+      <c r="B31" s="101" t="s">
         <v>140</v>
       </c>
-      <c r="C31" s="106"/>
-      <c r="D31" s="106"/>
-      <c r="E31" s="106"/>
-      <c r="F31" s="106"/>
-      <c r="G31" s="106"/>
-      <c r="H31" s="106"/>
-      <c r="I31" s="106"/>
-      <c r="J31" s="106"/>
-      <c r="K31" s="106"/>
-      <c r="L31" s="106"/>
-      <c r="M31" s="106"/>
-      <c r="N31" s="106"/>
-      <c r="O31" s="106"/>
+      <c r="C31" s="101"/>
+      <c r="D31" s="101"/>
+      <c r="E31" s="101"/>
+      <c r="F31" s="101"/>
+      <c r="G31" s="101"/>
+      <c r="H31" s="101"/>
+      <c r="I31" s="101"/>
+      <c r="J31" s="101"/>
+      <c r="K31" s="101"/>
+      <c r="L31" s="101"/>
+      <c r="M31" s="101"/>
+      <c r="N31" s="101"/>
+      <c r="O31" s="101"/>
       <c r="R31" s="26"/>
       <c r="S31" s="18"/>
       <c r="T31" s="18"/>
       <c r="U31" s="18"/>
-      <c r="V31" s="116" t="s">
+      <c r="V31" s="111" t="s">
         <v>109</v>
       </c>
-      <c r="W31" s="116"/>
-      <c r="X31" s="116"/>
-      <c r="Y31" s="116"/>
-      <c r="Z31" s="116"/>
+      <c r="W31" s="111"/>
+      <c r="X31" s="111"/>
+      <c r="Y31" s="111"/>
+      <c r="Z31" s="111"/>
       <c r="AA31" s="18"/>
       <c r="AB31" s="18"/>
       <c r="AC31" s="27"/>
     </row>
     <row r="32" spans="2:43" ht="15" customHeight="1">
-      <c r="B32" s="106"/>
-      <c r="C32" s="106"/>
-      <c r="D32" s="106"/>
-      <c r="E32" s="106"/>
-      <c r="F32" s="106"/>
-      <c r="G32" s="106"/>
-      <c r="H32" s="106"/>
-      <c r="I32" s="106"/>
-      <c r="J32" s="106"/>
-      <c r="K32" s="106"/>
-      <c r="L32" s="106"/>
-      <c r="M32" s="106"/>
-      <c r="N32" s="106"/>
-      <c r="O32" s="106"/>
+      <c r="B32" s="101"/>
+      <c r="C32" s="101"/>
+      <c r="D32" s="101"/>
+      <c r="E32" s="101"/>
+      <c r="F32" s="101"/>
+      <c r="G32" s="101"/>
+      <c r="H32" s="101"/>
+      <c r="I32" s="101"/>
+      <c r="J32" s="101"/>
+      <c r="K32" s="101"/>
+      <c r="L32" s="101"/>
+      <c r="M32" s="101"/>
+      <c r="N32" s="101"/>
+      <c r="O32" s="101"/>
       <c r="R32" s="26"/>
       <c r="S32" s="18"/>
       <c r="T32" s="18"/>
@@ -3230,61 +3292,61 @@
       <c r="AC32" s="27"/>
     </row>
     <row r="33" spans="2:32" ht="17.25" customHeight="1">
-      <c r="B33" s="106" t="s">
+      <c r="B33" s="101" t="s">
         <v>172</v>
       </c>
-      <c r="C33" s="106"/>
-      <c r="D33" s="106"/>
-      <c r="E33" s="106"/>
-      <c r="F33" s="106"/>
-      <c r="G33" s="106"/>
-      <c r="H33" s="106"/>
-      <c r="I33" s="106"/>
-      <c r="J33" s="106"/>
-      <c r="K33" s="106"/>
-      <c r="L33" s="106"/>
-      <c r="M33" s="106"/>
-      <c r="N33" s="106"/>
+      <c r="C33" s="101"/>
+      <c r="D33" s="101"/>
+      <c r="E33" s="101"/>
+      <c r="F33" s="101"/>
+      <c r="G33" s="101"/>
+      <c r="H33" s="101"/>
+      <c r="I33" s="101"/>
+      <c r="J33" s="101"/>
+      <c r="K33" s="101"/>
+      <c r="L33" s="101"/>
+      <c r="M33" s="101"/>
+      <c r="N33" s="101"/>
       <c r="R33" s="26"/>
-      <c r="S33" s="107" t="s">
+      <c r="S33" s="115" t="s">
         <v>108</v>
       </c>
-      <c r="T33" s="107"/>
-      <c r="U33" s="107"/>
-      <c r="V33" s="107"/>
-      <c r="W33" s="107"/>
-      <c r="X33" s="107"/>
-      <c r="Y33" s="107"/>
-      <c r="Z33" s="107"/>
-      <c r="AA33" s="107"/>
-      <c r="AB33" s="107"/>
+      <c r="T33" s="115"/>
+      <c r="U33" s="115"/>
+      <c r="V33" s="115"/>
+      <c r="W33" s="115"/>
+      <c r="X33" s="115"/>
+      <c r="Y33" s="115"/>
+      <c r="Z33" s="115"/>
+      <c r="AA33" s="115"/>
+      <c r="AB33" s="115"/>
       <c r="AC33" s="27"/>
     </row>
     <row r="34" spans="2:32" ht="17.25" customHeight="1">
-      <c r="B34" s="106"/>
-      <c r="C34" s="106"/>
-      <c r="D34" s="106"/>
-      <c r="E34" s="106"/>
-      <c r="F34" s="106"/>
-      <c r="G34" s="106"/>
-      <c r="H34" s="106"/>
-      <c r="I34" s="106"/>
-      <c r="J34" s="106"/>
-      <c r="K34" s="106"/>
-      <c r="L34" s="106"/>
-      <c r="M34" s="106"/>
-      <c r="N34" s="106"/>
+      <c r="B34" s="101"/>
+      <c r="C34" s="101"/>
+      <c r="D34" s="101"/>
+      <c r="E34" s="101"/>
+      <c r="F34" s="101"/>
+      <c r="G34" s="101"/>
+      <c r="H34" s="101"/>
+      <c r="I34" s="101"/>
+      <c r="J34" s="101"/>
+      <c r="K34" s="101"/>
+      <c r="L34" s="101"/>
+      <c r="M34" s="101"/>
+      <c r="N34" s="101"/>
       <c r="R34" s="26"/>
-      <c r="S34" s="107"/>
-      <c r="T34" s="107"/>
-      <c r="U34" s="107"/>
-      <c r="V34" s="107"/>
-      <c r="W34" s="107"/>
-      <c r="X34" s="107"/>
-      <c r="Y34" s="107"/>
-      <c r="Z34" s="107"/>
-      <c r="AA34" s="107"/>
-      <c r="AB34" s="107"/>
+      <c r="S34" s="115"/>
+      <c r="T34" s="115"/>
+      <c r="U34" s="115"/>
+      <c r="V34" s="115"/>
+      <c r="W34" s="115"/>
+      <c r="X34" s="115"/>
+      <c r="Y34" s="115"/>
+      <c r="Z34" s="115"/>
+      <c r="AA34" s="115"/>
+      <c r="AB34" s="115"/>
       <c r="AC34" s="27"/>
     </row>
     <row r="35" spans="2:32">
@@ -3322,67 +3384,67 @@
     </row>
     <row r="37" spans="2:32">
       <c r="R37" s="26"/>
-      <c r="S37" s="108" t="s">
+      <c r="S37" s="116" t="s">
         <v>111</v>
       </c>
-      <c r="T37" s="108"/>
-      <c r="U37" s="108"/>
-      <c r="V37" s="108"/>
-      <c r="W37" s="108"/>
-      <c r="X37" s="108"/>
-      <c r="Y37" s="108"/>
-      <c r="Z37" s="108"/>
-      <c r="AA37" s="108"/>
-      <c r="AB37" s="108"/>
+      <c r="T37" s="116"/>
+      <c r="U37" s="116"/>
+      <c r="V37" s="116"/>
+      <c r="W37" s="116"/>
+      <c r="X37" s="116"/>
+      <c r="Y37" s="116"/>
+      <c r="Z37" s="116"/>
+      <c r="AA37" s="116"/>
+      <c r="AB37" s="116"/>
       <c r="AC37" s="27"/>
       <c r="AF37" s="9"/>
     </row>
     <row r="38" spans="2:32">
-      <c r="B38" s="106" t="s">
+      <c r="B38" s="101" t="s">
         <v>142</v>
       </c>
-      <c r="C38" s="106"/>
-      <c r="D38" s="106"/>
-      <c r="E38" s="106"/>
-      <c r="F38" s="106"/>
-      <c r="G38" s="106"/>
-      <c r="H38" s="106"/>
-      <c r="I38" s="106"/>
-      <c r="J38" s="106"/>
-      <c r="K38" s="106"/>
-      <c r="L38" s="106"/>
-      <c r="M38" s="106"/>
-      <c r="N38" s="106"/>
-      <c r="O38" s="106"/>
+      <c r="C38" s="101"/>
+      <c r="D38" s="101"/>
+      <c r="E38" s="101"/>
+      <c r="F38" s="101"/>
+      <c r="G38" s="101"/>
+      <c r="H38" s="101"/>
+      <c r="I38" s="101"/>
+      <c r="J38" s="101"/>
+      <c r="K38" s="101"/>
+      <c r="L38" s="101"/>
+      <c r="M38" s="101"/>
+      <c r="N38" s="101"/>
+      <c r="O38" s="101"/>
       <c r="R38" s="26"/>
-      <c r="S38" s="108"/>
-      <c r="T38" s="108"/>
-      <c r="U38" s="108"/>
-      <c r="V38" s="108"/>
-      <c r="W38" s="108"/>
-      <c r="X38" s="108"/>
-      <c r="Y38" s="108"/>
-      <c r="Z38" s="108"/>
-      <c r="AA38" s="108"/>
-      <c r="AB38" s="108"/>
+      <c r="S38" s="116"/>
+      <c r="T38" s="116"/>
+      <c r="U38" s="116"/>
+      <c r="V38" s="116"/>
+      <c r="W38" s="116"/>
+      <c r="X38" s="116"/>
+      <c r="Y38" s="116"/>
+      <c r="Z38" s="116"/>
+      <c r="AA38" s="116"/>
+      <c r="AB38" s="116"/>
       <c r="AC38" s="27"/>
       <c r="AF38" s="9"/>
     </row>
     <row r="39" spans="2:32">
-      <c r="B39" s="106"/>
-      <c r="C39" s="106"/>
-      <c r="D39" s="106"/>
-      <c r="E39" s="106"/>
-      <c r="F39" s="106"/>
-      <c r="G39" s="106"/>
-      <c r="H39" s="106"/>
-      <c r="I39" s="106"/>
-      <c r="J39" s="106"/>
-      <c r="K39" s="106"/>
-      <c r="L39" s="106"/>
-      <c r="M39" s="106"/>
-      <c r="N39" s="106"/>
-      <c r="O39" s="106"/>
+      <c r="B39" s="101"/>
+      <c r="C39" s="101"/>
+      <c r="D39" s="101"/>
+      <c r="E39" s="101"/>
+      <c r="F39" s="101"/>
+      <c r="G39" s="101"/>
+      <c r="H39" s="101"/>
+      <c r="I39" s="101"/>
+      <c r="J39" s="101"/>
+      <c r="K39" s="101"/>
+      <c r="L39" s="101"/>
+      <c r="M39" s="101"/>
+      <c r="N39" s="101"/>
+      <c r="O39" s="101"/>
       <c r="R39" s="26"/>
       <c r="S39" s="18"/>
       <c r="T39" s="19"/>
@@ -3402,34 +3464,34 @@
       <c r="S40" s="18"/>
       <c r="T40" s="19"/>
       <c r="U40" s="19"/>
-      <c r="V40" s="117" t="s">
+      <c r="V40" s="112" t="s">
         <v>110</v>
       </c>
-      <c r="W40" s="117"/>
-      <c r="X40" s="117"/>
-      <c r="Y40" s="117"/>
-      <c r="Z40" s="117"/>
+      <c r="W40" s="112"/>
+      <c r="X40" s="112"/>
+      <c r="Y40" s="112"/>
+      <c r="Z40" s="112"/>
       <c r="AA40" s="19"/>
       <c r="AB40" s="19"/>
       <c r="AC40" s="27"/>
     </row>
     <row r="41" spans="2:32" ht="17.25">
-      <c r="B41" s="101" t="s">
+      <c r="B41" s="109" t="s">
         <v>104</v>
       </c>
-      <c r="C41" s="101"/>
-      <c r="D41" s="101"/>
-      <c r="E41" s="101"/>
-      <c r="F41" s="101"/>
-      <c r="G41" s="101"/>
-      <c r="H41" s="101"/>
-      <c r="I41" s="101"/>
-      <c r="J41" s="101"/>
-      <c r="K41" s="101"/>
-      <c r="L41" s="101"/>
-      <c r="M41" s="101"/>
-      <c r="N41" s="101"/>
-      <c r="O41" s="101"/>
+      <c r="C41" s="109"/>
+      <c r="D41" s="109"/>
+      <c r="E41" s="109"/>
+      <c r="F41" s="109"/>
+      <c r="G41" s="109"/>
+      <c r="H41" s="109"/>
+      <c r="I41" s="109"/>
+      <c r="J41" s="109"/>
+      <c r="K41" s="109"/>
+      <c r="L41" s="109"/>
+      <c r="M41" s="109"/>
+      <c r="N41" s="109"/>
+      <c r="O41" s="109"/>
       <c r="R41" s="26"/>
       <c r="S41" s="18"/>
       <c r="T41" s="18"/>
@@ -3445,18 +3507,18 @@
     </row>
     <row r="42" spans="2:32" ht="17.25">
       <c r="R42" s="26"/>
-      <c r="S42" s="109" t="s">
+      <c r="S42" s="113" t="s">
         <v>112</v>
       </c>
-      <c r="T42" s="109"/>
-      <c r="U42" s="109"/>
-      <c r="V42" s="109"/>
-      <c r="W42" s="109"/>
-      <c r="X42" s="109"/>
-      <c r="Y42" s="109"/>
-      <c r="Z42" s="109"/>
-      <c r="AA42" s="109"/>
-      <c r="AB42" s="109"/>
+      <c r="T42" s="113"/>
+      <c r="U42" s="113"/>
+      <c r="V42" s="113"/>
+      <c r="W42" s="113"/>
+      <c r="X42" s="113"/>
+      <c r="Y42" s="113"/>
+      <c r="Z42" s="113"/>
+      <c r="AA42" s="113"/>
+      <c r="AB42" s="113"/>
       <c r="AC42" s="27"/>
     </row>
     <row r="43" spans="2:32" ht="17.25">
@@ -3491,63 +3553,63 @@
       <c r="AC44" s="27"/>
     </row>
     <row r="45" spans="2:32">
-      <c r="B45" s="106" t="s">
+      <c r="B45" s="101" t="s">
         <v>143</v>
       </c>
-      <c r="C45" s="106"/>
-      <c r="D45" s="106"/>
-      <c r="E45" s="106"/>
-      <c r="F45" s="106"/>
-      <c r="G45" s="106"/>
-      <c r="H45" s="106"/>
-      <c r="I45" s="106"/>
-      <c r="J45" s="106"/>
-      <c r="K45" s="106"/>
-      <c r="L45" s="106"/>
-      <c r="M45" s="106"/>
-      <c r="N45" s="106"/>
-      <c r="O45" s="106"/>
+      <c r="C45" s="101"/>
+      <c r="D45" s="101"/>
+      <c r="E45" s="101"/>
+      <c r="F45" s="101"/>
+      <c r="G45" s="101"/>
+      <c r="H45" s="101"/>
+      <c r="I45" s="101"/>
+      <c r="J45" s="101"/>
+      <c r="K45" s="101"/>
+      <c r="L45" s="101"/>
+      <c r="M45" s="101"/>
+      <c r="N45" s="101"/>
+      <c r="O45" s="101"/>
       <c r="R45" s="26"/>
-      <c r="S45" s="107" t="s">
+      <c r="S45" s="115" t="s">
         <v>113</v>
       </c>
-      <c r="T45" s="107"/>
-      <c r="U45" s="107"/>
-      <c r="V45" s="107"/>
-      <c r="W45" s="107"/>
-      <c r="X45" s="107"/>
-      <c r="Y45" s="107"/>
-      <c r="Z45" s="107"/>
-      <c r="AA45" s="107"/>
-      <c r="AB45" s="107"/>
+      <c r="T45" s="115"/>
+      <c r="U45" s="115"/>
+      <c r="V45" s="115"/>
+      <c r="W45" s="115"/>
+      <c r="X45" s="115"/>
+      <c r="Y45" s="115"/>
+      <c r="Z45" s="115"/>
+      <c r="AA45" s="115"/>
+      <c r="AB45" s="115"/>
       <c r="AC45" s="27"/>
     </row>
     <row r="46" spans="2:32" ht="15" customHeight="1">
-      <c r="B46" s="106"/>
-      <c r="C46" s="106"/>
-      <c r="D46" s="106"/>
-      <c r="E46" s="106"/>
-      <c r="F46" s="106"/>
-      <c r="G46" s="106"/>
-      <c r="H46" s="106"/>
-      <c r="I46" s="106"/>
-      <c r="J46" s="106"/>
-      <c r="K46" s="106"/>
-      <c r="L46" s="106"/>
-      <c r="M46" s="106"/>
-      <c r="N46" s="106"/>
-      <c r="O46" s="106"/>
+      <c r="B46" s="101"/>
+      <c r="C46" s="101"/>
+      <c r="D46" s="101"/>
+      <c r="E46" s="101"/>
+      <c r="F46" s="101"/>
+      <c r="G46" s="101"/>
+      <c r="H46" s="101"/>
+      <c r="I46" s="101"/>
+      <c r="J46" s="101"/>
+      <c r="K46" s="101"/>
+      <c r="L46" s="101"/>
+      <c r="M46" s="101"/>
+      <c r="N46" s="101"/>
+      <c r="O46" s="101"/>
       <c r="R46" s="26"/>
-      <c r="S46" s="107"/>
-      <c r="T46" s="107"/>
-      <c r="U46" s="107"/>
-      <c r="V46" s="107"/>
-      <c r="W46" s="107"/>
-      <c r="X46" s="107"/>
-      <c r="Y46" s="107"/>
-      <c r="Z46" s="107"/>
-      <c r="AA46" s="107"/>
-      <c r="AB46" s="107"/>
+      <c r="S46" s="115"/>
+      <c r="T46" s="115"/>
+      <c r="U46" s="115"/>
+      <c r="V46" s="115"/>
+      <c r="W46" s="115"/>
+      <c r="X46" s="115"/>
+      <c r="Y46" s="115"/>
+      <c r="Z46" s="115"/>
+      <c r="AA46" s="115"/>
+      <c r="AB46" s="115"/>
       <c r="AC46" s="27"/>
     </row>
     <row r="47" spans="2:32" ht="15" customHeight="1">
@@ -3572,13 +3634,13 @@
       <c r="S48" s="18"/>
       <c r="T48" s="18"/>
       <c r="U48" s="18"/>
-      <c r="V48" s="104" t="s">
+      <c r="V48" s="118" t="s">
         <v>114</v>
       </c>
-      <c r="W48" s="104"/>
-      <c r="X48" s="104"/>
-      <c r="Y48" s="104"/>
-      <c r="Z48" s="104"/>
+      <c r="W48" s="118"/>
+      <c r="X48" s="118"/>
+      <c r="Y48" s="118"/>
+      <c r="Z48" s="118"/>
       <c r="AA48" s="18"/>
       <c r="AB48" s="18"/>
       <c r="AC48" s="27"/>
@@ -3598,52 +3660,52 @@
       <c r="AC49" s="27"/>
     </row>
     <row r="50" spans="2:43">
-      <c r="B50" s="106" t="s">
+      <c r="B50" s="101" t="s">
         <v>145</v>
       </c>
-      <c r="C50" s="106"/>
-      <c r="D50" s="106"/>
-      <c r="E50" s="106"/>
-      <c r="F50" s="106"/>
-      <c r="G50" s="106"/>
-      <c r="H50" s="106"/>
-      <c r="I50" s="106"/>
-      <c r="J50" s="106"/>
-      <c r="K50" s="106"/>
-      <c r="L50" s="106"/>
-      <c r="M50" s="106"/>
-      <c r="N50" s="106"/>
-      <c r="O50" s="106"/>
+      <c r="C50" s="101"/>
+      <c r="D50" s="101"/>
+      <c r="E50" s="101"/>
+      <c r="F50" s="101"/>
+      <c r="G50" s="101"/>
+      <c r="H50" s="101"/>
+      <c r="I50" s="101"/>
+      <c r="J50" s="101"/>
+      <c r="K50" s="101"/>
+      <c r="L50" s="101"/>
+      <c r="M50" s="101"/>
+      <c r="N50" s="101"/>
+      <c r="O50" s="101"/>
       <c r="R50" s="26"/>
-      <c r="S50" s="105" t="s">
+      <c r="S50" s="106" t="s">
         <v>115</v>
       </c>
-      <c r="T50" s="105"/>
-      <c r="U50" s="105"/>
-      <c r="V50" s="105"/>
-      <c r="W50" s="105"/>
-      <c r="X50" s="105"/>
-      <c r="Y50" s="105"/>
-      <c r="Z50" s="105"/>
-      <c r="AA50" s="105"/>
-      <c r="AB50" s="105"/>
+      <c r="T50" s="106"/>
+      <c r="U50" s="106"/>
+      <c r="V50" s="106"/>
+      <c r="W50" s="106"/>
+      <c r="X50" s="106"/>
+      <c r="Y50" s="106"/>
+      <c r="Z50" s="106"/>
+      <c r="AA50" s="106"/>
+      <c r="AB50" s="106"/>
       <c r="AC50" s="27"/>
     </row>
     <row r="51" spans="2:43" ht="15" customHeight="1">
-      <c r="B51" s="106"/>
-      <c r="C51" s="106"/>
-      <c r="D51" s="106"/>
-      <c r="E51" s="106"/>
-      <c r="F51" s="106"/>
-      <c r="G51" s="106"/>
-      <c r="H51" s="106"/>
-      <c r="I51" s="106"/>
-      <c r="J51" s="106"/>
-      <c r="K51" s="106"/>
-      <c r="L51" s="106"/>
-      <c r="M51" s="106"/>
-      <c r="N51" s="106"/>
-      <c r="O51" s="106"/>
+      <c r="B51" s="101"/>
+      <c r="C51" s="101"/>
+      <c r="D51" s="101"/>
+      <c r="E51" s="101"/>
+      <c r="F51" s="101"/>
+      <c r="G51" s="101"/>
+      <c r="H51" s="101"/>
+      <c r="I51" s="101"/>
+      <c r="J51" s="101"/>
+      <c r="K51" s="101"/>
+      <c r="L51" s="101"/>
+      <c r="M51" s="101"/>
+      <c r="N51" s="101"/>
+      <c r="O51" s="101"/>
       <c r="R51" s="26"/>
       <c r="S51" s="18"/>
       <c r="T51" s="18"/>
@@ -3659,18 +3721,18 @@
     </row>
     <row r="52" spans="2:43">
       <c r="R52" s="26"/>
-      <c r="S52" s="105" t="s">
+      <c r="S52" s="106" t="s">
         <v>116</v>
       </c>
-      <c r="T52" s="105"/>
-      <c r="U52" s="105"/>
-      <c r="V52" s="105"/>
-      <c r="W52" s="105"/>
-      <c r="X52" s="105"/>
-      <c r="Y52" s="105"/>
-      <c r="Z52" s="105"/>
-      <c r="AA52" s="105"/>
-      <c r="AB52" s="105"/>
+      <c r="T52" s="106"/>
+      <c r="U52" s="106"/>
+      <c r="V52" s="106"/>
+      <c r="W52" s="106"/>
+      <c r="X52" s="106"/>
+      <c r="Y52" s="106"/>
+      <c r="Z52" s="106"/>
+      <c r="AA52" s="106"/>
+      <c r="AB52" s="106"/>
       <c r="AC52" s="27"/>
     </row>
     <row r="53" spans="2:43" ht="15.75" customHeight="1">
@@ -3678,16 +3740,16 @@
         <v>147</v>
       </c>
       <c r="R53" s="26"/>
-      <c r="S53" s="105"/>
-      <c r="T53" s="105"/>
-      <c r="U53" s="105"/>
-      <c r="V53" s="105"/>
-      <c r="W53" s="105"/>
-      <c r="X53" s="105"/>
-      <c r="Y53" s="105"/>
-      <c r="Z53" s="105"/>
-      <c r="AA53" s="105"/>
-      <c r="AB53" s="105"/>
+      <c r="S53" s="106"/>
+      <c r="T53" s="106"/>
+      <c r="U53" s="106"/>
+      <c r="V53" s="106"/>
+      <c r="W53" s="106"/>
+      <c r="X53" s="106"/>
+      <c r="Y53" s="106"/>
+      <c r="Z53" s="106"/>
+      <c r="AA53" s="106"/>
+      <c r="AB53" s="106"/>
       <c r="AC53" s="27"/>
       <c r="AH53" s="22"/>
       <c r="AI53" s="22"/>
@@ -3715,22 +3777,22 @@
       <c r="AC54" s="27"/>
     </row>
     <row r="55" spans="2:43">
-      <c r="B55" s="106" t="s">
+      <c r="B55" s="101" t="s">
         <v>154</v>
       </c>
-      <c r="C55" s="106"/>
-      <c r="D55" s="106"/>
-      <c r="E55" s="106"/>
-      <c r="F55" s="106"/>
-      <c r="G55" s="106"/>
-      <c r="H55" s="106"/>
-      <c r="I55" s="106"/>
-      <c r="J55" s="106"/>
-      <c r="K55" s="106"/>
-      <c r="L55" s="106"/>
-      <c r="M55" s="106"/>
-      <c r="N55" s="106"/>
-      <c r="O55" s="106"/>
+      <c r="C55" s="101"/>
+      <c r="D55" s="101"/>
+      <c r="E55" s="101"/>
+      <c r="F55" s="101"/>
+      <c r="G55" s="101"/>
+      <c r="H55" s="101"/>
+      <c r="I55" s="101"/>
+      <c r="J55" s="101"/>
+      <c r="K55" s="101"/>
+      <c r="L55" s="101"/>
+      <c r="M55" s="101"/>
+      <c r="N55" s="101"/>
+      <c r="O55" s="101"/>
       <c r="R55" s="28"/>
       <c r="S55" s="29"/>
       <c r="T55" s="29"/>
@@ -3745,272 +3807,272 @@
       <c r="AC55" s="30"/>
     </row>
     <row r="56" spans="2:43">
-      <c r="B56" s="106"/>
-      <c r="C56" s="106"/>
-      <c r="D56" s="106"/>
-      <c r="E56" s="106"/>
-      <c r="F56" s="106"/>
-      <c r="G56" s="106"/>
-      <c r="H56" s="106"/>
-      <c r="I56" s="106"/>
-      <c r="J56" s="106"/>
-      <c r="K56" s="106"/>
-      <c r="L56" s="106"/>
-      <c r="M56" s="106"/>
-      <c r="N56" s="106"/>
-      <c r="O56" s="106"/>
+      <c r="B56" s="101"/>
+      <c r="C56" s="101"/>
+      <c r="D56" s="101"/>
+      <c r="E56" s="101"/>
+      <c r="F56" s="101"/>
+      <c r="G56" s="101"/>
+      <c r="H56" s="101"/>
+      <c r="I56" s="101"/>
+      <c r="J56" s="101"/>
+      <c r="K56" s="101"/>
+      <c r="L56" s="101"/>
+      <c r="M56" s="101"/>
+      <c r="N56" s="101"/>
+      <c r="O56" s="101"/>
     </row>
     <row r="58" spans="2:43" ht="17.25">
-      <c r="B58" s="101" t="s">
+      <c r="B58" s="109" t="s">
         <v>97</v>
       </c>
-      <c r="C58" s="101"/>
-      <c r="D58" s="101"/>
-      <c r="E58" s="101"/>
-      <c r="F58" s="101"/>
-      <c r="G58" s="101"/>
-      <c r="H58" s="101"/>
-      <c r="I58" s="101"/>
-      <c r="J58" s="101"/>
-      <c r="K58" s="101"/>
-      <c r="L58" s="101"/>
-      <c r="M58" s="101"/>
-      <c r="N58" s="101"/>
-      <c r="O58" s="101"/>
-      <c r="Q58" s="102" t="s">
+      <c r="C58" s="109"/>
+      <c r="D58" s="109"/>
+      <c r="E58" s="109"/>
+      <c r="F58" s="109"/>
+      <c r="G58" s="109"/>
+      <c r="H58" s="109"/>
+      <c r="I58" s="109"/>
+      <c r="J58" s="109"/>
+      <c r="K58" s="109"/>
+      <c r="L58" s="109"/>
+      <c r="M58" s="109"/>
+      <c r="N58" s="109"/>
+      <c r="O58" s="109"/>
+      <c r="Q58" s="117" t="s">
         <v>169</v>
       </c>
-      <c r="R58" s="102"/>
-      <c r="S58" s="102"/>
-      <c r="T58" s="102"/>
-      <c r="U58" s="102"/>
-      <c r="V58" s="102"/>
-      <c r="W58" s="102"/>
-      <c r="X58" s="102"/>
-      <c r="Y58" s="102"/>
-      <c r="Z58" s="102"/>
-      <c r="AA58" s="102"/>
-      <c r="AB58" s="102"/>
-      <c r="AC58" s="102"/>
-      <c r="AD58" s="102"/>
+      <c r="R58" s="117"/>
+      <c r="S58" s="117"/>
+      <c r="T58" s="117"/>
+      <c r="U58" s="117"/>
+      <c r="V58" s="117"/>
+      <c r="W58" s="117"/>
+      <c r="X58" s="117"/>
+      <c r="Y58" s="117"/>
+      <c r="Z58" s="117"/>
+      <c r="AA58" s="117"/>
+      <c r="AB58" s="117"/>
+      <c r="AC58" s="117"/>
+      <c r="AD58" s="117"/>
     </row>
     <row r="60" spans="2:43" ht="17.25">
-      <c r="B60" s="103" t="s">
+      <c r="B60" s="102" t="s">
         <v>198</v>
       </c>
-      <c r="C60" s="103"/>
-      <c r="D60" s="103"/>
-      <c r="E60" s="103"/>
-      <c r="F60" s="103"/>
-      <c r="G60" s="103"/>
-      <c r="H60" s="103"/>
-      <c r="I60" s="103"/>
-      <c r="J60" s="103"/>
-      <c r="K60" s="103"/>
-      <c r="L60" s="103"/>
-      <c r="M60" s="103"/>
-      <c r="N60" s="103"/>
-      <c r="O60" s="103"/>
+      <c r="C60" s="102"/>
+      <c r="D60" s="102"/>
+      <c r="E60" s="102"/>
+      <c r="F60" s="102"/>
+      <c r="G60" s="102"/>
+      <c r="H60" s="102"/>
+      <c r="I60" s="102"/>
+      <c r="J60" s="102"/>
+      <c r="K60" s="102"/>
+      <c r="L60" s="102"/>
+      <c r="M60" s="102"/>
+      <c r="N60" s="102"/>
+      <c r="O60" s="102"/>
       <c r="Q60" s="20" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="61" spans="2:43">
-      <c r="B61" s="103"/>
-      <c r="C61" s="103"/>
-      <c r="D61" s="103"/>
-      <c r="E61" s="103"/>
-      <c r="F61" s="103"/>
-      <c r="G61" s="103"/>
-      <c r="H61" s="103"/>
-      <c r="I61" s="103"/>
-      <c r="J61" s="103"/>
-      <c r="K61" s="103"/>
-      <c r="L61" s="103"/>
-      <c r="M61" s="103"/>
-      <c r="N61" s="103"/>
-      <c r="O61" s="103"/>
+      <c r="B61" s="102"/>
+      <c r="C61" s="102"/>
+      <c r="D61" s="102"/>
+      <c r="E61" s="102"/>
+      <c r="F61" s="102"/>
+      <c r="G61" s="102"/>
+      <c r="H61" s="102"/>
+      <c r="I61" s="102"/>
+      <c r="J61" s="102"/>
+      <c r="K61" s="102"/>
+      <c r="L61" s="102"/>
+      <c r="M61" s="102"/>
+      <c r="N61" s="102"/>
+      <c r="O61" s="102"/>
     </row>
     <row r="62" spans="2:43">
-      <c r="Q62" s="106" t="s">
+      <c r="Q62" s="101" t="s">
         <v>195</v>
       </c>
-      <c r="R62" s="106"/>
-      <c r="S62" s="106"/>
-      <c r="T62" s="106"/>
-      <c r="U62" s="106"/>
-      <c r="V62" s="106"/>
-      <c r="W62" s="106"/>
-      <c r="X62" s="106"/>
-      <c r="Y62" s="106"/>
-      <c r="Z62" s="106"/>
-      <c r="AA62" s="106"/>
-      <c r="AB62" s="106"/>
-      <c r="AC62" s="106"/>
-      <c r="AD62" s="106"/>
+      <c r="R62" s="101"/>
+      <c r="S62" s="101"/>
+      <c r="T62" s="101"/>
+      <c r="U62" s="101"/>
+      <c r="V62" s="101"/>
+      <c r="W62" s="101"/>
+      <c r="X62" s="101"/>
+      <c r="Y62" s="101"/>
+      <c r="Z62" s="101"/>
+      <c r="AA62" s="101"/>
+      <c r="AB62" s="101"/>
+      <c r="AC62" s="101"/>
+      <c r="AD62" s="101"/>
     </row>
     <row r="63" spans="2:43" ht="15" customHeight="1">
-      <c r="B63" s="103" t="s">
+      <c r="B63" s="102" t="s">
         <v>213</v>
       </c>
-      <c r="C63" s="103"/>
-      <c r="D63" s="103"/>
-      <c r="E63" s="103"/>
-      <c r="F63" s="103"/>
-      <c r="G63" s="103"/>
-      <c r="H63" s="103"/>
-      <c r="I63" s="103"/>
-      <c r="J63" s="103"/>
-      <c r="K63" s="103"/>
-      <c r="L63" s="103"/>
-      <c r="M63" s="103"/>
-      <c r="N63" s="103"/>
-      <c r="O63" s="103"/>
-      <c r="Q63" s="106"/>
-      <c r="R63" s="106"/>
-      <c r="S63" s="106"/>
-      <c r="T63" s="106"/>
-      <c r="U63" s="106"/>
-      <c r="V63" s="106"/>
-      <c r="W63" s="106"/>
-      <c r="X63" s="106"/>
-      <c r="Y63" s="106"/>
-      <c r="Z63" s="106"/>
-      <c r="AA63" s="106"/>
-      <c r="AB63" s="106"/>
-      <c r="AC63" s="106"/>
-      <c r="AD63" s="106"/>
+      <c r="C63" s="102"/>
+      <c r="D63" s="102"/>
+      <c r="E63" s="102"/>
+      <c r="F63" s="102"/>
+      <c r="G63" s="102"/>
+      <c r="H63" s="102"/>
+      <c r="I63" s="102"/>
+      <c r="J63" s="102"/>
+      <c r="K63" s="102"/>
+      <c r="L63" s="102"/>
+      <c r="M63" s="102"/>
+      <c r="N63" s="102"/>
+      <c r="O63" s="102"/>
+      <c r="Q63" s="101"/>
+      <c r="R63" s="101"/>
+      <c r="S63" s="101"/>
+      <c r="T63" s="101"/>
+      <c r="U63" s="101"/>
+      <c r="V63" s="101"/>
+      <c r="W63" s="101"/>
+      <c r="X63" s="101"/>
+      <c r="Y63" s="101"/>
+      <c r="Z63" s="101"/>
+      <c r="AA63" s="101"/>
+      <c r="AB63" s="101"/>
+      <c r="AC63" s="101"/>
+      <c r="AD63" s="101"/>
     </row>
     <row r="64" spans="2:43">
-      <c r="B64" s="103"/>
-      <c r="C64" s="103"/>
-      <c r="D64" s="103"/>
-      <c r="E64" s="103"/>
-      <c r="F64" s="103"/>
-      <c r="G64" s="103"/>
-      <c r="H64" s="103"/>
-      <c r="I64" s="103"/>
-      <c r="J64" s="103"/>
-      <c r="K64" s="103"/>
-      <c r="L64" s="103"/>
-      <c r="M64" s="103"/>
-      <c r="N64" s="103"/>
-      <c r="O64" s="103"/>
+      <c r="B64" s="102"/>
+      <c r="C64" s="102"/>
+      <c r="D64" s="102"/>
+      <c r="E64" s="102"/>
+      <c r="F64" s="102"/>
+      <c r="G64" s="102"/>
+      <c r="H64" s="102"/>
+      <c r="I64" s="102"/>
+      <c r="J64" s="102"/>
+      <c r="K64" s="102"/>
+      <c r="L64" s="102"/>
+      <c r="M64" s="102"/>
+      <c r="N64" s="102"/>
+      <c r="O64" s="102"/>
     </row>
     <row r="65" spans="2:30" ht="17.25">
-      <c r="B65" s="103"/>
-      <c r="C65" s="103"/>
-      <c r="D65" s="103"/>
-      <c r="E65" s="103"/>
-      <c r="F65" s="103"/>
-      <c r="G65" s="103"/>
-      <c r="H65" s="103"/>
-      <c r="I65" s="103"/>
-      <c r="J65" s="103"/>
-      <c r="K65" s="103"/>
-      <c r="L65" s="103"/>
-      <c r="M65" s="103"/>
-      <c r="N65" s="103"/>
-      <c r="O65" s="103"/>
+      <c r="B65" s="102"/>
+      <c r="C65" s="102"/>
+      <c r="D65" s="102"/>
+      <c r="E65" s="102"/>
+      <c r="F65" s="102"/>
+      <c r="G65" s="102"/>
+      <c r="H65" s="102"/>
+      <c r="I65" s="102"/>
+      <c r="J65" s="102"/>
+      <c r="K65" s="102"/>
+      <c r="L65" s="102"/>
+      <c r="M65" s="102"/>
+      <c r="N65" s="102"/>
+      <c r="O65" s="102"/>
       <c r="Q65" s="20" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="66" spans="2:30">
-      <c r="B66" s="103"/>
-      <c r="C66" s="103"/>
-      <c r="D66" s="103"/>
-      <c r="E66" s="103"/>
-      <c r="F66" s="103"/>
-      <c r="G66" s="103"/>
-      <c r="H66" s="103"/>
-      <c r="I66" s="103"/>
-      <c r="J66" s="103"/>
-      <c r="K66" s="103"/>
-      <c r="L66" s="103"/>
-      <c r="M66" s="103"/>
-      <c r="N66" s="103"/>
-      <c r="O66" s="103"/>
+      <c r="B66" s="102"/>
+      <c r="C66" s="102"/>
+      <c r="D66" s="102"/>
+      <c r="E66" s="102"/>
+      <c r="F66" s="102"/>
+      <c r="G66" s="102"/>
+      <c r="H66" s="102"/>
+      <c r="I66" s="102"/>
+      <c r="J66" s="102"/>
+      <c r="K66" s="102"/>
+      <c r="L66" s="102"/>
+      <c r="M66" s="102"/>
+      <c r="N66" s="102"/>
+      <c r="O66" s="102"/>
     </row>
     <row r="67" spans="2:30" ht="15" customHeight="1">
-      <c r="B67" s="106" t="s">
+      <c r="B67" s="101" t="s">
         <v>200</v>
       </c>
-      <c r="C67" s="106"/>
-      <c r="D67" s="106"/>
-      <c r="E67" s="106"/>
-      <c r="F67" s="106"/>
-      <c r="G67" s="106"/>
-      <c r="H67" s="106"/>
-      <c r="I67" s="106"/>
-      <c r="J67" s="106"/>
-      <c r="K67" s="106"/>
-      <c r="L67" s="106"/>
-      <c r="M67" s="106"/>
-      <c r="N67" s="106"/>
-      <c r="O67" s="106"/>
-      <c r="Q67" s="106" t="s">
+      <c r="C67" s="101"/>
+      <c r="D67" s="101"/>
+      <c r="E67" s="101"/>
+      <c r="F67" s="101"/>
+      <c r="G67" s="101"/>
+      <c r="H67" s="101"/>
+      <c r="I67" s="101"/>
+      <c r="J67" s="101"/>
+      <c r="K67" s="101"/>
+      <c r="L67" s="101"/>
+      <c r="M67" s="101"/>
+      <c r="N67" s="101"/>
+      <c r="O67" s="101"/>
+      <c r="Q67" s="101" t="s">
         <v>209</v>
       </c>
-      <c r="R67" s="106"/>
-      <c r="S67" s="106"/>
-      <c r="T67" s="106"/>
-      <c r="U67" s="106"/>
-      <c r="V67" s="106"/>
-      <c r="W67" s="106"/>
-      <c r="X67" s="106"/>
-      <c r="Y67" s="106"/>
-      <c r="Z67" s="106"/>
-      <c r="AA67" s="106"/>
-      <c r="AB67" s="106"/>
-      <c r="AC67" s="106"/>
-      <c r="AD67" s="106"/>
+      <c r="R67" s="101"/>
+      <c r="S67" s="101"/>
+      <c r="T67" s="101"/>
+      <c r="U67" s="101"/>
+      <c r="V67" s="101"/>
+      <c r="W67" s="101"/>
+      <c r="X67" s="101"/>
+      <c r="Y67" s="101"/>
+      <c r="Z67" s="101"/>
+      <c r="AA67" s="101"/>
+      <c r="AB67" s="101"/>
+      <c r="AC67" s="101"/>
+      <c r="AD67" s="101"/>
     </row>
     <row r="68" spans="2:30">
-      <c r="B68" s="106"/>
-      <c r="C68" s="106"/>
-      <c r="D68" s="106"/>
-      <c r="E68" s="106"/>
-      <c r="F68" s="106"/>
-      <c r="G68" s="106"/>
-      <c r="H68" s="106"/>
-      <c r="I68" s="106"/>
-      <c r="J68" s="106"/>
-      <c r="K68" s="106"/>
-      <c r="L68" s="106"/>
-      <c r="M68" s="106"/>
-      <c r="N68" s="106"/>
-      <c r="O68" s="106"/>
-      <c r="Q68" s="106"/>
-      <c r="R68" s="106"/>
-      <c r="S68" s="106"/>
-      <c r="T68" s="106"/>
-      <c r="U68" s="106"/>
-      <c r="V68" s="106"/>
-      <c r="W68" s="106"/>
-      <c r="X68" s="106"/>
-      <c r="Y68" s="106"/>
-      <c r="Z68" s="106"/>
-      <c r="AA68" s="106"/>
-      <c r="AB68" s="106"/>
-      <c r="AC68" s="106"/>
-      <c r="AD68" s="106"/>
+      <c r="B68" s="101"/>
+      <c r="C68" s="101"/>
+      <c r="D68" s="101"/>
+      <c r="E68" s="101"/>
+      <c r="F68" s="101"/>
+      <c r="G68" s="101"/>
+      <c r="H68" s="101"/>
+      <c r="I68" s="101"/>
+      <c r="J68" s="101"/>
+      <c r="K68" s="101"/>
+      <c r="L68" s="101"/>
+      <c r="M68" s="101"/>
+      <c r="N68" s="101"/>
+      <c r="O68" s="101"/>
+      <c r="Q68" s="101"/>
+      <c r="R68" s="101"/>
+      <c r="S68" s="101"/>
+      <c r="T68" s="101"/>
+      <c r="U68" s="101"/>
+      <c r="V68" s="101"/>
+      <c r="W68" s="101"/>
+      <c r="X68" s="101"/>
+      <c r="Y68" s="101"/>
+      <c r="Z68" s="101"/>
+      <c r="AA68" s="101"/>
+      <c r="AB68" s="101"/>
+      <c r="AC68" s="101"/>
+      <c r="AD68" s="101"/>
     </row>
     <row r="69" spans="2:30">
-      <c r="Q69" s="106"/>
-      <c r="R69" s="106"/>
-      <c r="S69" s="106"/>
-      <c r="T69" s="106"/>
-      <c r="U69" s="106"/>
-      <c r="V69" s="106"/>
-      <c r="W69" s="106"/>
-      <c r="X69" s="106"/>
-      <c r="Y69" s="106"/>
-      <c r="Z69" s="106"/>
-      <c r="AA69" s="106"/>
-      <c r="AB69" s="106"/>
-      <c r="AC69" s="106"/>
-      <c r="AD69" s="106"/>
+      <c r="Q69" s="101"/>
+      <c r="R69" s="101"/>
+      <c r="S69" s="101"/>
+      <c r="T69" s="101"/>
+      <c r="U69" s="101"/>
+      <c r="V69" s="101"/>
+      <c r="W69" s="101"/>
+      <c r="X69" s="101"/>
+      <c r="Y69" s="101"/>
+      <c r="Z69" s="101"/>
+      <c r="AA69" s="101"/>
+      <c r="AB69" s="101"/>
+      <c r="AC69" s="101"/>
+      <c r="AD69" s="101"/>
     </row>
     <row r="70" spans="2:30" ht="17.25">
       <c r="B70" s="10" t="s">
@@ -4023,196 +4085,207 @@
       </c>
     </row>
     <row r="73" spans="2:30">
-      <c r="Q73" s="103" t="s">
+      <c r="Q73" s="102" t="s">
         <v>203</v>
       </c>
-      <c r="R73" s="103"/>
-      <c r="S73" s="103"/>
-      <c r="T73" s="103"/>
-      <c r="U73" s="103"/>
-      <c r="V73" s="103"/>
-      <c r="W73" s="103"/>
-      <c r="X73" s="103"/>
-      <c r="Y73" s="103"/>
-      <c r="Z73" s="103"/>
-      <c r="AA73" s="103"/>
-      <c r="AB73" s="103"/>
-      <c r="AC73" s="103"/>
-      <c r="AD73" s="103"/>
+      <c r="R73" s="102"/>
+      <c r="S73" s="102"/>
+      <c r="T73" s="102"/>
+      <c r="U73" s="102"/>
+      <c r="V73" s="102"/>
+      <c r="W73" s="102"/>
+      <c r="X73" s="102"/>
+      <c r="Y73" s="102"/>
+      <c r="Z73" s="102"/>
+      <c r="AA73" s="102"/>
+      <c r="AB73" s="102"/>
+      <c r="AC73" s="102"/>
+      <c r="AD73" s="102"/>
     </row>
     <row r="74" spans="2:30">
-      <c r="Q74" s="103"/>
-      <c r="R74" s="103"/>
-      <c r="S74" s="103"/>
-      <c r="T74" s="103"/>
-      <c r="U74" s="103"/>
-      <c r="V74" s="103"/>
-      <c r="W74" s="103"/>
-      <c r="X74" s="103"/>
-      <c r="Y74" s="103"/>
-      <c r="Z74" s="103"/>
-      <c r="AA74" s="103"/>
-      <c r="AB74" s="103"/>
-      <c r="AC74" s="103"/>
-      <c r="AD74" s="103"/>
+      <c r="Q74" s="102"/>
+      <c r="R74" s="102"/>
+      <c r="S74" s="102"/>
+      <c r="T74" s="102"/>
+      <c r="U74" s="102"/>
+      <c r="V74" s="102"/>
+      <c r="W74" s="102"/>
+      <c r="X74" s="102"/>
+      <c r="Y74" s="102"/>
+      <c r="Z74" s="102"/>
+      <c r="AA74" s="102"/>
+      <c r="AB74" s="102"/>
+      <c r="AC74" s="102"/>
+      <c r="AD74" s="102"/>
     </row>
     <row r="75" spans="2:30" ht="15" customHeight="1">
-      <c r="Q75" s="103"/>
-      <c r="R75" s="103"/>
-      <c r="S75" s="103"/>
-      <c r="T75" s="103"/>
-      <c r="U75" s="103"/>
-      <c r="V75" s="103"/>
-      <c r="W75" s="103"/>
-      <c r="X75" s="103"/>
-      <c r="Y75" s="103"/>
-      <c r="Z75" s="103"/>
-      <c r="AA75" s="103"/>
-      <c r="AB75" s="103"/>
-      <c r="AC75" s="103"/>
-      <c r="AD75" s="103"/>
+      <c r="Q75" s="102"/>
+      <c r="R75" s="102"/>
+      <c r="S75" s="102"/>
+      <c r="T75" s="102"/>
+      <c r="U75" s="102"/>
+      <c r="V75" s="102"/>
+      <c r="W75" s="102"/>
+      <c r="X75" s="102"/>
+      <c r="Y75" s="102"/>
+      <c r="Z75" s="102"/>
+      <c r="AA75" s="102"/>
+      <c r="AB75" s="102"/>
+      <c r="AC75" s="102"/>
+      <c r="AD75" s="102"/>
     </row>
     <row r="76" spans="2:30">
-      <c r="Q76" s="103"/>
-      <c r="R76" s="103"/>
-      <c r="S76" s="103"/>
-      <c r="T76" s="103"/>
-      <c r="U76" s="103"/>
-      <c r="V76" s="103"/>
-      <c r="W76" s="103"/>
-      <c r="X76" s="103"/>
-      <c r="Y76" s="103"/>
-      <c r="Z76" s="103"/>
-      <c r="AA76" s="103"/>
-      <c r="AB76" s="103"/>
-      <c r="AC76" s="103"/>
-      <c r="AD76" s="103"/>
+      <c r="Q76" s="102"/>
+      <c r="R76" s="102"/>
+      <c r="S76" s="102"/>
+      <c r="T76" s="102"/>
+      <c r="U76" s="102"/>
+      <c r="V76" s="102"/>
+      <c r="W76" s="102"/>
+      <c r="X76" s="102"/>
+      <c r="Y76" s="102"/>
+      <c r="Z76" s="102"/>
+      <c r="AA76" s="102"/>
+      <c r="AB76" s="102"/>
+      <c r="AC76" s="102"/>
+      <c r="AD76" s="102"/>
     </row>
     <row r="77" spans="2:30">
-      <c r="Q77" s="103"/>
-      <c r="R77" s="103"/>
-      <c r="S77" s="103"/>
-      <c r="T77" s="103"/>
-      <c r="U77" s="103"/>
-      <c r="V77" s="103"/>
-      <c r="W77" s="103"/>
-      <c r="X77" s="103"/>
-      <c r="Y77" s="103"/>
-      <c r="Z77" s="103"/>
-      <c r="AA77" s="103"/>
-      <c r="AB77" s="103"/>
-      <c r="AC77" s="103"/>
-      <c r="AD77" s="103"/>
+      <c r="Q77" s="102"/>
+      <c r="R77" s="102"/>
+      <c r="S77" s="102"/>
+      <c r="T77" s="102"/>
+      <c r="U77" s="102"/>
+      <c r="V77" s="102"/>
+      <c r="W77" s="102"/>
+      <c r="X77" s="102"/>
+      <c r="Y77" s="102"/>
+      <c r="Z77" s="102"/>
+      <c r="AA77" s="102"/>
+      <c r="AB77" s="102"/>
+      <c r="AC77" s="102"/>
+      <c r="AD77" s="102"/>
     </row>
     <row r="79" spans="2:30" ht="17.25">
-      <c r="B79" s="101" t="s">
+      <c r="B79" s="109" t="s">
         <v>101</v>
       </c>
-      <c r="C79" s="101"/>
-      <c r="D79" s="101"/>
-      <c r="E79" s="101"/>
-      <c r="F79" s="101"/>
-      <c r="G79" s="101"/>
-      <c r="H79" s="101"/>
-      <c r="I79" s="101"/>
-      <c r="J79" s="101"/>
-      <c r="K79" s="101"/>
-      <c r="L79" s="101"/>
-      <c r="M79" s="101"/>
-      <c r="N79" s="101"/>
-      <c r="O79" s="101"/>
+      <c r="C79" s="109"/>
+      <c r="D79" s="109"/>
+      <c r="E79" s="109"/>
+      <c r="F79" s="109"/>
+      <c r="G79" s="109"/>
+      <c r="H79" s="109"/>
+      <c r="I79" s="109"/>
+      <c r="J79" s="109"/>
+      <c r="K79" s="109"/>
+      <c r="L79" s="109"/>
+      <c r="M79" s="109"/>
+      <c r="N79" s="109"/>
+      <c r="O79" s="109"/>
       <c r="Q79" s="20" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="81" spans="2:30" ht="15" customHeight="1">
-      <c r="B81" s="106" t="s">
+      <c r="B81" s="101" t="s">
         <v>193</v>
       </c>
-      <c r="C81" s="106"/>
-      <c r="D81" s="106"/>
-      <c r="E81" s="106"/>
-      <c r="F81" s="106"/>
-      <c r="G81" s="106"/>
-      <c r="H81" s="106"/>
-      <c r="I81" s="106"/>
-      <c r="J81" s="106"/>
-      <c r="K81" s="106"/>
-      <c r="L81" s="106"/>
-      <c r="M81" s="106"/>
-      <c r="N81" s="106"/>
-      <c r="O81" s="106"/>
-      <c r="Q81" s="103" t="s">
+      <c r="C81" s="101"/>
+      <c r="D81" s="101"/>
+      <c r="E81" s="101"/>
+      <c r="F81" s="101"/>
+      <c r="G81" s="101"/>
+      <c r="H81" s="101"/>
+      <c r="I81" s="101"/>
+      <c r="J81" s="101"/>
+      <c r="K81" s="101"/>
+      <c r="L81" s="101"/>
+      <c r="M81" s="101"/>
+      <c r="N81" s="101"/>
+      <c r="O81" s="101"/>
+      <c r="Q81" s="102" t="s">
         <v>202</v>
       </c>
-      <c r="R81" s="103"/>
-      <c r="S81" s="103"/>
-      <c r="T81" s="103"/>
-      <c r="U81" s="103"/>
-      <c r="V81" s="103"/>
-      <c r="W81" s="103"/>
-      <c r="X81" s="103"/>
-      <c r="Y81" s="103"/>
-      <c r="Z81" s="103"/>
-      <c r="AA81" s="103"/>
-      <c r="AB81" s="103"/>
-      <c r="AC81" s="103"/>
-      <c r="AD81" s="103"/>
+      <c r="R81" s="102"/>
+      <c r="S81" s="102"/>
+      <c r="T81" s="102"/>
+      <c r="U81" s="102"/>
+      <c r="V81" s="102"/>
+      <c r="W81" s="102"/>
+      <c r="X81" s="102"/>
+      <c r="Y81" s="102"/>
+      <c r="Z81" s="102"/>
+      <c r="AA81" s="102"/>
+      <c r="AB81" s="102"/>
+      <c r="AC81" s="102"/>
+      <c r="AD81" s="102"/>
     </row>
     <row r="82" spans="2:30">
-      <c r="B82" s="106"/>
-      <c r="C82" s="106"/>
-      <c r="D82" s="106"/>
-      <c r="E82" s="106"/>
-      <c r="F82" s="106"/>
-      <c r="G82" s="106"/>
-      <c r="H82" s="106"/>
-      <c r="I82" s="106"/>
-      <c r="J82" s="106"/>
-      <c r="K82" s="106"/>
-      <c r="L82" s="106"/>
-      <c r="M82" s="106"/>
-      <c r="N82" s="106"/>
-      <c r="O82" s="106"/>
-      <c r="Q82" s="103"/>
-      <c r="R82" s="103"/>
-      <c r="S82" s="103"/>
-      <c r="T82" s="103"/>
-      <c r="U82" s="103"/>
-      <c r="V82" s="103"/>
-      <c r="W82" s="103"/>
-      <c r="X82" s="103"/>
-      <c r="Y82" s="103"/>
-      <c r="Z82" s="103"/>
-      <c r="AA82" s="103"/>
-      <c r="AB82" s="103"/>
-      <c r="AC82" s="103"/>
-      <c r="AD82" s="103"/>
+      <c r="B82" s="101"/>
+      <c r="C82" s="101"/>
+      <c r="D82" s="101"/>
+      <c r="E82" s="101"/>
+      <c r="F82" s="101"/>
+      <c r="G82" s="101"/>
+      <c r="H82" s="101"/>
+      <c r="I82" s="101"/>
+      <c r="J82" s="101"/>
+      <c r="K82" s="101"/>
+      <c r="L82" s="101"/>
+      <c r="M82" s="101"/>
+      <c r="N82" s="101"/>
+      <c r="O82" s="101"/>
+      <c r="Q82" s="102"/>
+      <c r="R82" s="102"/>
+      <c r="S82" s="102"/>
+      <c r="T82" s="102"/>
+      <c r="U82" s="102"/>
+      <c r="V82" s="102"/>
+      <c r="W82" s="102"/>
+      <c r="X82" s="102"/>
+      <c r="Y82" s="102"/>
+      <c r="Z82" s="102"/>
+      <c r="AA82" s="102"/>
+      <c r="AB82" s="102"/>
+      <c r="AC82" s="102"/>
+      <c r="AD82" s="102"/>
     </row>
     <row r="83" spans="2:30">
-      <c r="Q83" s="103"/>
-      <c r="R83" s="103"/>
-      <c r="S83" s="103"/>
-      <c r="T83" s="103"/>
-      <c r="U83" s="103"/>
-      <c r="V83" s="103"/>
-      <c r="W83" s="103"/>
-      <c r="X83" s="103"/>
-      <c r="Y83" s="103"/>
-      <c r="Z83" s="103"/>
-      <c r="AA83" s="103"/>
-      <c r="AB83" s="103"/>
-      <c r="AC83" s="103"/>
-      <c r="AD83" s="103"/>
+      <c r="Q83" s="102"/>
+      <c r="R83" s="102"/>
+      <c r="S83" s="102"/>
+      <c r="T83" s="102"/>
+      <c r="U83" s="102"/>
+      <c r="V83" s="102"/>
+      <c r="W83" s="102"/>
+      <c r="X83" s="102"/>
+      <c r="Y83" s="102"/>
+      <c r="Z83" s="102"/>
+      <c r="AA83" s="102"/>
+      <c r="AB83" s="102"/>
+      <c r="AC83" s="102"/>
+      <c r="AD83" s="102"/>
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="B81:O82"/>
-    <mergeCell ref="Q62:AD63"/>
-    <mergeCell ref="B63:O66"/>
-    <mergeCell ref="B67:O68"/>
-    <mergeCell ref="Q73:AD77"/>
-    <mergeCell ref="Q81:AD83"/>
+    <mergeCell ref="B58:O58"/>
+    <mergeCell ref="B79:O79"/>
+    <mergeCell ref="Q58:AD58"/>
+    <mergeCell ref="B60:O61"/>
+    <mergeCell ref="V48:Z48"/>
+    <mergeCell ref="S50:AB50"/>
+    <mergeCell ref="Q67:AD69"/>
+    <mergeCell ref="B50:O51"/>
+    <mergeCell ref="S33:AB34"/>
+    <mergeCell ref="S37:AB38"/>
+    <mergeCell ref="S42:AB42"/>
+    <mergeCell ref="S45:AB46"/>
+    <mergeCell ref="B55:O56"/>
+    <mergeCell ref="B33:N34"/>
+    <mergeCell ref="B38:O39"/>
+    <mergeCell ref="B41:O41"/>
+    <mergeCell ref="B45:O46"/>
     <mergeCell ref="B2:O2"/>
     <mergeCell ref="B4:O5"/>
     <mergeCell ref="B8:O9"/>
@@ -4229,23 +4302,12 @@
     <mergeCell ref="V40:Z40"/>
     <mergeCell ref="S29:AB29"/>
     <mergeCell ref="S26:AB26"/>
-    <mergeCell ref="S33:AB34"/>
-    <mergeCell ref="S37:AB38"/>
-    <mergeCell ref="S42:AB42"/>
-    <mergeCell ref="S45:AB46"/>
-    <mergeCell ref="B55:O56"/>
-    <mergeCell ref="B33:N34"/>
-    <mergeCell ref="B38:O39"/>
-    <mergeCell ref="B41:O41"/>
-    <mergeCell ref="B45:O46"/>
-    <mergeCell ref="B58:O58"/>
-    <mergeCell ref="B79:O79"/>
-    <mergeCell ref="Q58:AD58"/>
-    <mergeCell ref="B60:O61"/>
-    <mergeCell ref="V48:Z48"/>
-    <mergeCell ref="S50:AB50"/>
-    <mergeCell ref="Q67:AD69"/>
-    <mergeCell ref="B50:O51"/>
+    <mergeCell ref="B81:O82"/>
+    <mergeCell ref="Q62:AD63"/>
+    <mergeCell ref="B63:O66"/>
+    <mergeCell ref="B67:O68"/>
+    <mergeCell ref="Q73:AD77"/>
+    <mergeCell ref="Q81:AD83"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4254,6 +4316,101 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F1513E-F3B7-4E2D-855D-C70B365C968F}">
+  <sheetPr>
+    <tabColor theme="7" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A4:B12"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20:B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A4" s="119" t="s">
+        <v>228</v>
+      </c>
+      <c r="B4" s="119" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" thickTop="1">
+      <c r="A5" t="s">
+        <v>220</v>
+      </c>
+      <c r="B5">
+        <v>0.4521856341365087</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>221</v>
+      </c>
+      <c r="B6">
+        <v>0.38308555478780298</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>222</v>
+      </c>
+      <c r="B7">
+        <v>0.39666773771891822</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>223</v>
+      </c>
+      <c r="B8">
+        <v>0.43517066185236231</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>224</v>
+      </c>
+      <c r="B9">
+        <v>0.37190757391651003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>225</v>
+      </c>
+      <c r="B10">
+        <v>0.47216441970460488</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>226</v>
+      </c>
+      <c r="B11">
+        <v>0.33605820330095793</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>227</v>
+      </c>
+      <c r="B12">
+        <v>0.62986877068882074</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B46DDACF-D0ED-4CB1-BA1F-87BB8EEFE26F}">
   <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
@@ -4755,7 +4912,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07E26828-25FC-4634-987C-5618292A93B9}">
   <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
@@ -4836,7 +4993,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC4C435-8BC3-449D-901D-3701FB9529AC}">
   <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
@@ -4946,7 +5103,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7A50504-DB74-4372-80E7-81330A036E34}">
   <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
@@ -5089,7 +5246,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3E2194D-F24C-4F86-853D-6FD3370F64B7}">
   <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
@@ -5232,7 +5389,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48D3AC3D-A586-4510-8963-9751795FC8CB}">
   <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
@@ -5366,7 +5523,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27DAF99A-77C4-4B04-A50C-7585BCDCC48B}">
   <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
@@ -5469,7 +5626,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50F8DE8A-8846-4F1C-A15F-BB0A1B1DF3CC}">
   <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
@@ -71726,8 +71883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1B821FE-871F-4FF6-AD12-EEE4379083E0}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -72292,10 +72449,10 @@
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -72305,9 +72462,10 @@
     <col min="3" max="3" width="32" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1">
       <c r="A1" s="56" t="s">
         <v>148</v>
       </c>
@@ -72323,8 +72481,11 @@
       <c r="E1" s="56" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" thickTop="1">
+      <c r="G1" s="120" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickTop="1">
       <c r="A2" s="55">
         <f>Regiones!A2</f>
         <v>1</v>
@@ -72342,8 +72503,9 @@
       <c r="E2" s="35">
         <v>1000</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="G2" s="121"/>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="55">
         <f>Regiones!A3</f>
         <v>2</v>
@@ -72362,7 +72524,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:7">
       <c r="A4" s="55">
         <f>Regiones!A4</f>
         <v>3</v>
@@ -72381,7 +72543,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:7">
       <c r="A5" s="55">
         <f>Regiones!A5</f>
         <v>4</v>
@@ -72400,7 +72562,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:7">
       <c r="A6" s="55">
         <f>Regiones!A6</f>
         <v>5</v>
@@ -72419,7 +72581,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:7">
       <c r="A7" s="55">
         <f>Regiones!A7</f>
         <v>6</v>
@@ -72438,7 +72600,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:7">
       <c r="A8" s="55">
         <f>Regiones!A8</f>
         <v>7</v>
@@ -72457,7 +72619,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:7">
       <c r="A9" s="55">
         <f>Regiones!A9</f>
         <v>8</v>
@@ -72476,7 +72638,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:7">
       <c r="A10" s="55">
         <f>Regiones!A10</f>
         <v>9</v>
@@ -72495,7 +72657,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:7">
       <c r="A11" s="55">
         <f>Regiones!A11</f>
         <v>10</v>
@@ -72514,7 +72676,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:7">
       <c r="A12" s="55">
         <f>Regiones!A12</f>
         <v>11</v>
@@ -72533,7 +72695,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:7">
       <c r="A13" s="55">
         <f>Regiones!A13</f>
         <v>12</v>
@@ -72552,7 +72714,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:7">
       <c r="A14" s="55">
         <f>Regiones!A14</f>
         <v>13</v>
@@ -72571,7 +72733,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:7">
       <c r="A15" s="55">
         <f>Regiones!A15</f>
         <v>14</v>
@@ -72590,7 +72752,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:7">
       <c r="A16" s="55">
         <f>Regiones!A16</f>
         <v>15</v>
@@ -72810,10 +72972,10 @@
   <sheetPr>
     <tabColor theme="4" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -72821,9 +72983,10 @@
     <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1" s="34" t="s">
         <v>157</v>
       </c>
@@ -72833,8 +72996,11 @@
       <c r="C1" s="34" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1">
+      <c r="E1" s="122" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickTop="1">
       <c r="A2" s="43">
         <f>Regiones!A2</f>
         <v>1</v>
@@ -72846,8 +73012,11 @@
       <c r="C2" s="35">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="E2" s="123" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="43">
         <f>Regiones!A3</f>
         <v>2</v>
@@ -72860,7 +73029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:5">
       <c r="A4" s="43">
         <f>Regiones!A4</f>
         <v>3</v>
@@ -72873,7 +73042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:5">
       <c r="A5" s="43">
         <f>Regiones!A5</f>
         <v>4</v>
@@ -72886,7 +73055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:5">
       <c r="A6" s="43">
         <f>Regiones!A6</f>
         <v>5</v>
@@ -72899,7 +73068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:5">
       <c r="A7" s="43">
         <f>Regiones!A7</f>
         <v>6</v>
@@ -72912,7 +73081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:5">
       <c r="A8" s="43">
         <f>Regiones!A8</f>
         <v>7</v>
@@ -72925,7 +73094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:5">
       <c r="A9" s="43">
         <f>Regiones!A9</f>
         <v>8</v>
@@ -72938,7 +73107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:5">
       <c r="A10" s="43">
         <f>Regiones!A10</f>
         <v>9</v>
@@ -72951,7 +73120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:5">
       <c r="A11" s="43">
         <f>Regiones!A11</f>
         <v>10</v>
@@ -72964,7 +73133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:5">
       <c r="A12" s="43">
         <f>Regiones!A12</f>
         <v>11</v>
@@ -72977,7 +73146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:5">
       <c r="A13" s="43">
         <f>Regiones!A13</f>
         <v>12</v>
@@ -72990,7 +73159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:5">
       <c r="A14" s="43">
         <f>Regiones!A14</f>
         <v>13</v>
@@ -73003,7 +73172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:5">
       <c r="A15" s="43">
         <f>Regiones!A15</f>
         <v>14</v>
@@ -73016,7 +73185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:5">
       <c r="A16" s="43">
         <f>Regiones!A16</f>
         <v>15</v>

</xml_diff>

<commit_message>
adds maximun daily testing capacity fixes bugs in simulation start date
</commit_message>
<xml_diff>
--- a/COVID Simulator v 1.1/Input/Input_Simulador.xlsx
+++ b/COVID Simulator v 1.1/Input/Input_Simulador.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignacio.brottier\Documents\COVID 19\COVID-19-Simulation-Argentina\COVID Simulator v 1.1\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF8274AA-8A1E-43AD-B5B6-2300EE290271}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96884975-E76F-4A0F-B944-B6D9EE845F6D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="29040" windowHeight="15750" firstSheet="6" activeTab="8" xr2:uid="{55AC4C4C-7526-4060-9BB2-10E89010456B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="5" activeTab="8" xr2:uid="{55AC4C4C-7526-4060-9BB2-10E89010456B}"/>
   </bookViews>
   <sheets>
     <sheet name="Información" sheetId="28" r:id="rId1"/>
@@ -1632,22 +1632,23 @@
     <t>5. Fecha Inicial [dd/mm/aaaa]</t>
   </si>
   <si>
-    <t>03/03/2020</t>
+    <t>10/1/2020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="m\-d"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="167" formatCode="0.0000"/>
     <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="171" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="32">
+  <fonts count="33">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1864,6 +1865,12 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -1916,7 +1923,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2071,7 +2078,7 @@
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2303,11 +2310,41 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2318,16 +2355,10 @@
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2339,34 +2370,13 @@
     <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="8">
@@ -2820,22 +2830,22 @@
   <sheetData>
     <row r="1" spans="2:45" s="9" customFormat="1"/>
     <row r="2" spans="2:45" s="9" customFormat="1" ht="33.75" customHeight="1" thickBot="1">
-      <c r="B2" s="103" t="s">
+      <c r="B2" s="113" t="s">
         <v>105</v>
       </c>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103"/>
-      <c r="N2" s="103"/>
-      <c r="O2" s="103"/>
+      <c r="C2" s="113"/>
+      <c r="D2" s="113"/>
+      <c r="E2" s="113"/>
+      <c r="F2" s="113"/>
+      <c r="G2" s="113"/>
+      <c r="H2" s="113"/>
+      <c r="I2" s="113"/>
+      <c r="J2" s="113"/>
+      <c r="K2" s="113"/>
+      <c r="L2" s="113"/>
+      <c r="M2" s="113"/>
+      <c r="N2" s="113"/>
+      <c r="O2" s="113"/>
       <c r="Q2" s="57"/>
       <c r="R2" s="57"/>
       <c r="S2" s="57"/>
@@ -2853,248 +2863,248 @@
     </row>
     <row r="3" spans="2:45" ht="15.75" thickTop="1"/>
     <row r="4" spans="2:45" ht="15" customHeight="1">
-      <c r="B4" s="101" t="s">
+      <c r="B4" s="109" t="s">
         <v>99</v>
       </c>
-      <c r="C4" s="101"/>
-      <c r="D4" s="101"/>
-      <c r="E4" s="101"/>
-      <c r="F4" s="101"/>
-      <c r="G4" s="101"/>
-      <c r="H4" s="101"/>
-      <c r="I4" s="101"/>
-      <c r="J4" s="101"/>
-      <c r="K4" s="101"/>
-      <c r="L4" s="101"/>
-      <c r="M4" s="101"/>
-      <c r="N4" s="101"/>
-      <c r="O4" s="101"/>
+      <c r="C4" s="109"/>
+      <c r="D4" s="109"/>
+      <c r="E4" s="109"/>
+      <c r="F4" s="109"/>
+      <c r="G4" s="109"/>
+      <c r="H4" s="109"/>
+      <c r="I4" s="109"/>
+      <c r="J4" s="109"/>
+      <c r="K4" s="109"/>
+      <c r="L4" s="109"/>
+      <c r="M4" s="109"/>
+      <c r="N4" s="109"/>
+      <c r="O4" s="109"/>
     </row>
     <row r="5" spans="2:45" ht="22.5" customHeight="1">
-      <c r="B5" s="101"/>
-      <c r="C5" s="101"/>
-      <c r="D5" s="101"/>
-      <c r="E5" s="101"/>
-      <c r="F5" s="101"/>
-      <c r="G5" s="101"/>
-      <c r="H5" s="101"/>
-      <c r="I5" s="101"/>
-      <c r="J5" s="101"/>
-      <c r="K5" s="101"/>
-      <c r="L5" s="101"/>
-      <c r="M5" s="101"/>
-      <c r="N5" s="101"/>
-      <c r="O5" s="101"/>
-      <c r="Q5" s="108" t="s">
+      <c r="B5" s="109"/>
+      <c r="C5" s="109"/>
+      <c r="D5" s="109"/>
+      <c r="E5" s="109"/>
+      <c r="F5" s="109"/>
+      <c r="G5" s="109"/>
+      <c r="H5" s="109"/>
+      <c r="I5" s="109"/>
+      <c r="J5" s="109"/>
+      <c r="K5" s="109"/>
+      <c r="L5" s="109"/>
+      <c r="M5" s="109"/>
+      <c r="N5" s="109"/>
+      <c r="O5" s="109"/>
+      <c r="Q5" s="117" t="s">
         <v>173</v>
       </c>
-      <c r="R5" s="108"/>
-      <c r="S5" s="108"/>
-      <c r="T5" s="108"/>
-      <c r="U5" s="108"/>
-      <c r="V5" s="108"/>
-      <c r="W5" s="108"/>
-      <c r="X5" s="108"/>
-      <c r="Y5" s="108"/>
-      <c r="Z5" s="108"/>
-      <c r="AA5" s="108"/>
-      <c r="AB5" s="108"/>
-      <c r="AC5" s="108"/>
-      <c r="AD5" s="108"/>
+      <c r="R5" s="117"/>
+      <c r="S5" s="117"/>
+      <c r="T5" s="117"/>
+      <c r="U5" s="117"/>
+      <c r="V5" s="117"/>
+      <c r="W5" s="117"/>
+      <c r="X5" s="117"/>
+      <c r="Y5" s="117"/>
+      <c r="Z5" s="117"/>
+      <c r="AA5" s="117"/>
+      <c r="AB5" s="117"/>
+      <c r="AC5" s="117"/>
+      <c r="AD5" s="117"/>
       <c r="AQ5" s="9"/>
       <c r="AR5" s="9"/>
       <c r="AS5" s="9"/>
     </row>
     <row r="6" spans="2:45">
-      <c r="Q6" s="107" t="s">
+      <c r="Q6" s="116" t="s">
         <v>174</v>
       </c>
-      <c r="R6" s="107"/>
-      <c r="S6" s="107"/>
-      <c r="T6" s="107"/>
-      <c r="U6" s="107"/>
-      <c r="V6" s="107"/>
-      <c r="W6" s="107"/>
-      <c r="X6" s="107"/>
-      <c r="Y6" s="107"/>
-      <c r="Z6" s="107"/>
-      <c r="AA6" s="107"/>
-      <c r="AB6" s="107"/>
-      <c r="AC6" s="107"/>
-      <c r="AD6" s="107"/>
+      <c r="R6" s="116"/>
+      <c r="S6" s="116"/>
+      <c r="T6" s="116"/>
+      <c r="U6" s="116"/>
+      <c r="V6" s="116"/>
+      <c r="W6" s="116"/>
+      <c r="X6" s="116"/>
+      <c r="Y6" s="116"/>
+      <c r="Z6" s="116"/>
+      <c r="AA6" s="116"/>
+      <c r="AB6" s="116"/>
+      <c r="AC6" s="116"/>
+      <c r="AD6" s="116"/>
     </row>
     <row r="7" spans="2:45">
-      <c r="Q7" s="107"/>
-      <c r="R7" s="107"/>
-      <c r="S7" s="107"/>
-      <c r="T7" s="107"/>
-      <c r="U7" s="107"/>
-      <c r="V7" s="107"/>
-      <c r="W7" s="107"/>
-      <c r="X7" s="107"/>
-      <c r="Y7" s="107"/>
-      <c r="Z7" s="107"/>
-      <c r="AA7" s="107"/>
-      <c r="AB7" s="107"/>
-      <c r="AC7" s="107"/>
-      <c r="AD7" s="107"/>
+      <c r="Q7" s="116"/>
+      <c r="R7" s="116"/>
+      <c r="S7" s="116"/>
+      <c r="T7" s="116"/>
+      <c r="U7" s="116"/>
+      <c r="V7" s="116"/>
+      <c r="W7" s="116"/>
+      <c r="X7" s="116"/>
+      <c r="Y7" s="116"/>
+      <c r="Z7" s="116"/>
+      <c r="AA7" s="116"/>
+      <c r="AB7" s="116"/>
+      <c r="AC7" s="116"/>
+      <c r="AD7" s="116"/>
     </row>
     <row r="8" spans="2:45" ht="15" customHeight="1">
-      <c r="B8" s="101" t="s">
+      <c r="B8" s="109" t="s">
         <v>103</v>
       </c>
-      <c r="C8" s="101"/>
-      <c r="D8" s="101"/>
-      <c r="E8" s="101"/>
-      <c r="F8" s="101"/>
-      <c r="G8" s="101"/>
-      <c r="H8" s="101"/>
-      <c r="I8" s="101"/>
-      <c r="J8" s="101"/>
-      <c r="K8" s="101"/>
-      <c r="L8" s="101"/>
-      <c r="M8" s="101"/>
-      <c r="N8" s="101"/>
-      <c r="O8" s="101"/>
-      <c r="Q8" s="107"/>
-      <c r="R8" s="107"/>
-      <c r="S8" s="107"/>
-      <c r="T8" s="107"/>
-      <c r="U8" s="107"/>
-      <c r="V8" s="107"/>
-      <c r="W8" s="107"/>
-      <c r="X8" s="107"/>
-      <c r="Y8" s="107"/>
-      <c r="Z8" s="107"/>
-      <c r="AA8" s="107"/>
-      <c r="AB8" s="107"/>
-      <c r="AC8" s="107"/>
-      <c r="AD8" s="107"/>
+      <c r="C8" s="109"/>
+      <c r="D8" s="109"/>
+      <c r="E8" s="109"/>
+      <c r="F8" s="109"/>
+      <c r="G8" s="109"/>
+      <c r="H8" s="109"/>
+      <c r="I8" s="109"/>
+      <c r="J8" s="109"/>
+      <c r="K8" s="109"/>
+      <c r="L8" s="109"/>
+      <c r="M8" s="109"/>
+      <c r="N8" s="109"/>
+      <c r="O8" s="109"/>
+      <c r="Q8" s="116"/>
+      <c r="R8" s="116"/>
+      <c r="S8" s="116"/>
+      <c r="T8" s="116"/>
+      <c r="U8" s="116"/>
+      <c r="V8" s="116"/>
+      <c r="W8" s="116"/>
+      <c r="X8" s="116"/>
+      <c r="Y8" s="116"/>
+      <c r="Z8" s="116"/>
+      <c r="AA8" s="116"/>
+      <c r="AB8" s="116"/>
+      <c r="AC8" s="116"/>
+      <c r="AD8" s="116"/>
     </row>
     <row r="9" spans="2:45" ht="17.25" customHeight="1">
-      <c r="B9" s="101"/>
-      <c r="C9" s="101"/>
-      <c r="D9" s="101"/>
-      <c r="E9" s="101"/>
-      <c r="F9" s="101"/>
-      <c r="G9" s="101"/>
-      <c r="H9" s="101"/>
-      <c r="I9" s="101"/>
-      <c r="J9" s="101"/>
-      <c r="K9" s="101"/>
-      <c r="L9" s="101"/>
-      <c r="M9" s="101"/>
-      <c r="N9" s="101"/>
-      <c r="O9" s="101"/>
+      <c r="B9" s="109"/>
+      <c r="C9" s="109"/>
+      <c r="D9" s="109"/>
+      <c r="E9" s="109"/>
+      <c r="F9" s="109"/>
+      <c r="G9" s="109"/>
+      <c r="H9" s="109"/>
+      <c r="I9" s="109"/>
+      <c r="J9" s="109"/>
+      <c r="K9" s="109"/>
+      <c r="L9" s="109"/>
+      <c r="M9" s="109"/>
+      <c r="N9" s="109"/>
+      <c r="O9" s="109"/>
     </row>
     <row r="12" spans="2:45" ht="17.25" customHeight="1">
       <c r="D12" s="15" t="s">
         <v>96</v>
       </c>
       <c r="H12" s="17"/>
-      <c r="I12" s="104" t="s">
+      <c r="I12" s="114" t="s">
         <v>100</v>
       </c>
-      <c r="J12" s="105"/>
-      <c r="K12" s="105"/>
-      <c r="L12" s="105"/>
-      <c r="M12" s="105"/>
+      <c r="J12" s="115"/>
+      <c r="K12" s="115"/>
+      <c r="L12" s="115"/>
+      <c r="M12" s="115"/>
     </row>
     <row r="13" spans="2:45" ht="17.25">
       <c r="D13" s="11" t="s">
         <v>104</v>
       </c>
       <c r="H13" s="17"/>
-      <c r="I13" s="104"/>
-      <c r="J13" s="105"/>
-      <c r="K13" s="105"/>
-      <c r="L13" s="105"/>
-      <c r="M13" s="105"/>
+      <c r="I13" s="114"/>
+      <c r="J13" s="115"/>
+      <c r="K13" s="115"/>
+      <c r="L13" s="115"/>
+      <c r="M13" s="115"/>
     </row>
     <row r="14" spans="2:45" ht="17.25">
       <c r="D14" s="13" t="s">
         <v>97</v>
       </c>
       <c r="H14" s="17"/>
-      <c r="I14" s="104"/>
-      <c r="J14" s="105"/>
-      <c r="K14" s="105"/>
-      <c r="L14" s="105"/>
-      <c r="M14" s="105"/>
+      <c r="I14" s="114"/>
+      <c r="J14" s="115"/>
+      <c r="K14" s="115"/>
+      <c r="L14" s="115"/>
+      <c r="M14" s="115"/>
     </row>
     <row r="15" spans="2:45" ht="17.25" customHeight="1">
       <c r="D15" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="I15" s="104"/>
-      <c r="J15" s="105"/>
-      <c r="K15" s="105"/>
-      <c r="L15" s="105"/>
-      <c r="M15" s="105"/>
+      <c r="I15" s="114"/>
+      <c r="J15" s="115"/>
+      <c r="K15" s="115"/>
+      <c r="L15" s="115"/>
+      <c r="M15" s="115"/>
     </row>
     <row r="17" spans="2:43" ht="17.25" customHeight="1">
       <c r="G17" s="18"/>
-      <c r="I17" s="104" t="s">
+      <c r="I17" s="114" t="s">
         <v>102</v>
       </c>
-      <c r="J17" s="105"/>
-      <c r="K17" s="105"/>
-      <c r="L17" s="105"/>
-      <c r="M17" s="105"/>
+      <c r="J17" s="115"/>
+      <c r="K17" s="115"/>
+      <c r="L17" s="115"/>
+      <c r="M17" s="115"/>
     </row>
     <row r="18" spans="2:43" ht="17.25">
       <c r="D18" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="I18" s="104"/>
-      <c r="J18" s="105"/>
-      <c r="K18" s="105"/>
-      <c r="L18" s="105"/>
-      <c r="M18" s="105"/>
+      <c r="I18" s="114"/>
+      <c r="J18" s="115"/>
+      <c r="K18" s="115"/>
+      <c r="L18" s="115"/>
+      <c r="M18" s="115"/>
     </row>
     <row r="19" spans="2:43" ht="15" customHeight="1">
-      <c r="I19" s="104"/>
-      <c r="J19" s="105"/>
-      <c r="K19" s="105"/>
-      <c r="L19" s="105"/>
-      <c r="M19" s="105"/>
+      <c r="I19" s="114"/>
+      <c r="J19" s="115"/>
+      <c r="K19" s="115"/>
+      <c r="L19" s="115"/>
+      <c r="M19" s="115"/>
     </row>
     <row r="22" spans="2:43">
-      <c r="B22" s="110" t="s">
+      <c r="B22" s="118" t="s">
         <v>139</v>
       </c>
-      <c r="C22" s="110"/>
-      <c r="D22" s="110"/>
-      <c r="E22" s="110"/>
-      <c r="F22" s="110"/>
-      <c r="G22" s="110"/>
-      <c r="H22" s="110"/>
-      <c r="I22" s="110"/>
-      <c r="J22" s="110"/>
-      <c r="K22" s="110"/>
-      <c r="L22" s="110"/>
-      <c r="M22" s="110"/>
-      <c r="N22" s="110"/>
-      <c r="O22" s="110"/>
+      <c r="C22" s="118"/>
+      <c r="D22" s="118"/>
+      <c r="E22" s="118"/>
+      <c r="F22" s="118"/>
+      <c r="G22" s="118"/>
+      <c r="H22" s="118"/>
+      <c r="I22" s="118"/>
+      <c r="J22" s="118"/>
+      <c r="K22" s="118"/>
+      <c r="L22" s="118"/>
+      <c r="M22" s="118"/>
+      <c r="N22" s="118"/>
+      <c r="O22" s="118"/>
     </row>
     <row r="23" spans="2:43" ht="15" customHeight="1"/>
     <row r="24" spans="2:43" ht="17.25">
-      <c r="B24" s="109" t="s">
+      <c r="B24" s="104" t="s">
         <v>96</v>
       </c>
-      <c r="C24" s="109"/>
-      <c r="D24" s="109"/>
-      <c r="E24" s="109"/>
-      <c r="F24" s="109"/>
-      <c r="G24" s="109"/>
-      <c r="H24" s="109"/>
-      <c r="I24" s="109"/>
-      <c r="J24" s="109"/>
-      <c r="K24" s="109"/>
-      <c r="L24" s="109"/>
-      <c r="M24" s="109"/>
-      <c r="N24" s="109"/>
-      <c r="O24" s="109"/>
+      <c r="C24" s="104"/>
+      <c r="D24" s="104"/>
+      <c r="E24" s="104"/>
+      <c r="F24" s="104"/>
+      <c r="G24" s="104"/>
+      <c r="H24" s="104"/>
+      <c r="I24" s="104"/>
+      <c r="J24" s="104"/>
+      <c r="K24" s="104"/>
+      <c r="L24" s="104"/>
+      <c r="M24" s="104"/>
+      <c r="N24" s="104"/>
+      <c r="O24" s="104"/>
     </row>
     <row r="25" spans="2:43">
       <c r="R25" s="23"/>
@@ -3115,37 +3125,37 @@
         <v>96</v>
       </c>
       <c r="R26" s="26"/>
-      <c r="S26" s="114" t="s">
+      <c r="S26" s="121" t="s">
         <v>106</v>
       </c>
-      <c r="T26" s="114"/>
-      <c r="U26" s="114"/>
-      <c r="V26" s="114"/>
-      <c r="W26" s="114"/>
-      <c r="X26" s="114"/>
-      <c r="Y26" s="114"/>
-      <c r="Z26" s="114"/>
-      <c r="AA26" s="114"/>
-      <c r="AB26" s="114"/>
+      <c r="T26" s="121"/>
+      <c r="U26" s="121"/>
+      <c r="V26" s="121"/>
+      <c r="W26" s="121"/>
+      <c r="X26" s="121"/>
+      <c r="Y26" s="121"/>
+      <c r="Z26" s="121"/>
+      <c r="AA26" s="121"/>
+      <c r="AB26" s="121"/>
       <c r="AC26" s="27"/>
     </row>
     <row r="27" spans="2:43" ht="15" customHeight="1">
-      <c r="B27" s="101" t="s">
+      <c r="B27" s="109" t="s">
         <v>117</v>
       </c>
-      <c r="C27" s="101"/>
-      <c r="D27" s="101"/>
-      <c r="E27" s="101"/>
-      <c r="F27" s="101"/>
-      <c r="G27" s="101"/>
-      <c r="H27" s="101"/>
-      <c r="I27" s="101"/>
-      <c r="J27" s="101"/>
-      <c r="K27" s="101"/>
-      <c r="L27" s="101"/>
-      <c r="M27" s="101"/>
-      <c r="N27" s="101"/>
-      <c r="O27" s="101"/>
+      <c r="C27" s="109"/>
+      <c r="D27" s="109"/>
+      <c r="E27" s="109"/>
+      <c r="F27" s="109"/>
+      <c r="G27" s="109"/>
+      <c r="H27" s="109"/>
+      <c r="I27" s="109"/>
+      <c r="J27" s="109"/>
+      <c r="K27" s="109"/>
+      <c r="L27" s="109"/>
+      <c r="M27" s="109"/>
+      <c r="N27" s="109"/>
+      <c r="O27" s="109"/>
       <c r="R27" s="26"/>
       <c r="S27" s="24"/>
       <c r="T27" s="24"/>
@@ -3170,51 +3180,51 @@
       <c r="AQ27" s="18"/>
     </row>
     <row r="28" spans="2:43" ht="15" customHeight="1">
-      <c r="B28" s="101"/>
-      <c r="C28" s="101"/>
-      <c r="D28" s="101"/>
-      <c r="E28" s="101"/>
-      <c r="F28" s="101"/>
-      <c r="G28" s="101"/>
-      <c r="H28" s="101"/>
-      <c r="I28" s="101"/>
-      <c r="J28" s="101"/>
-      <c r="K28" s="101"/>
-      <c r="L28" s="101"/>
-      <c r="M28" s="101"/>
-      <c r="N28" s="101"/>
-      <c r="O28" s="101"/>
+      <c r="B28" s="109"/>
+      <c r="C28" s="109"/>
+      <c r="D28" s="109"/>
+      <c r="E28" s="109"/>
+      <c r="F28" s="109"/>
+      <c r="G28" s="109"/>
+      <c r="H28" s="109"/>
+      <c r="I28" s="109"/>
+      <c r="J28" s="109"/>
+      <c r="K28" s="109"/>
+      <c r="L28" s="109"/>
+      <c r="M28" s="109"/>
+      <c r="N28" s="109"/>
+      <c r="O28" s="109"/>
       <c r="R28" s="26"/>
       <c r="AC28" s="27"/>
     </row>
     <row r="29" spans="2:43" ht="17.25">
-      <c r="B29" s="101"/>
-      <c r="C29" s="101"/>
-      <c r="D29" s="101"/>
-      <c r="E29" s="101"/>
-      <c r="F29" s="101"/>
-      <c r="G29" s="101"/>
-      <c r="H29" s="101"/>
-      <c r="I29" s="101"/>
-      <c r="J29" s="101"/>
-      <c r="K29" s="101"/>
-      <c r="L29" s="101"/>
-      <c r="M29" s="101"/>
-      <c r="N29" s="101"/>
-      <c r="O29" s="101"/>
+      <c r="B29" s="109"/>
+      <c r="C29" s="109"/>
+      <c r="D29" s="109"/>
+      <c r="E29" s="109"/>
+      <c r="F29" s="109"/>
+      <c r="G29" s="109"/>
+      <c r="H29" s="109"/>
+      <c r="I29" s="109"/>
+      <c r="J29" s="109"/>
+      <c r="K29" s="109"/>
+      <c r="L29" s="109"/>
+      <c r="M29" s="109"/>
+      <c r="N29" s="109"/>
+      <c r="O29" s="109"/>
       <c r="R29" s="26"/>
-      <c r="S29" s="113" t="s">
+      <c r="S29" s="112" t="s">
         <v>107</v>
       </c>
-      <c r="T29" s="113"/>
-      <c r="U29" s="113"/>
-      <c r="V29" s="113"/>
-      <c r="W29" s="113"/>
-      <c r="X29" s="113"/>
-      <c r="Y29" s="113"/>
-      <c r="Z29" s="113"/>
-      <c r="AA29" s="113"/>
-      <c r="AB29" s="113"/>
+      <c r="T29" s="112"/>
+      <c r="U29" s="112"/>
+      <c r="V29" s="112"/>
+      <c r="W29" s="112"/>
+      <c r="X29" s="112"/>
+      <c r="Y29" s="112"/>
+      <c r="Z29" s="112"/>
+      <c r="AA29" s="112"/>
+      <c r="AB29" s="112"/>
       <c r="AC29" s="27"/>
     </row>
     <row r="30" spans="2:43">
@@ -3232,52 +3242,52 @@
       <c r="AC30" s="27"/>
     </row>
     <row r="31" spans="2:43" ht="17.25">
-      <c r="B31" s="101" t="s">
+      <c r="B31" s="109" t="s">
         <v>140</v>
       </c>
-      <c r="C31" s="101"/>
-      <c r="D31" s="101"/>
-      <c r="E31" s="101"/>
-      <c r="F31" s="101"/>
-      <c r="G31" s="101"/>
-      <c r="H31" s="101"/>
-      <c r="I31" s="101"/>
-      <c r="J31" s="101"/>
-      <c r="K31" s="101"/>
-      <c r="L31" s="101"/>
-      <c r="M31" s="101"/>
-      <c r="N31" s="101"/>
-      <c r="O31" s="101"/>
+      <c r="C31" s="109"/>
+      <c r="D31" s="109"/>
+      <c r="E31" s="109"/>
+      <c r="F31" s="109"/>
+      <c r="G31" s="109"/>
+      <c r="H31" s="109"/>
+      <c r="I31" s="109"/>
+      <c r="J31" s="109"/>
+      <c r="K31" s="109"/>
+      <c r="L31" s="109"/>
+      <c r="M31" s="109"/>
+      <c r="N31" s="109"/>
+      <c r="O31" s="109"/>
       <c r="R31" s="26"/>
       <c r="S31" s="18"/>
       <c r="T31" s="18"/>
       <c r="U31" s="18"/>
-      <c r="V31" s="111" t="s">
+      <c r="V31" s="119" t="s">
         <v>109</v>
       </c>
-      <c r="W31" s="111"/>
-      <c r="X31" s="111"/>
-      <c r="Y31" s="111"/>
-      <c r="Z31" s="111"/>
+      <c r="W31" s="119"/>
+      <c r="X31" s="119"/>
+      <c r="Y31" s="119"/>
+      <c r="Z31" s="119"/>
       <c r="AA31" s="18"/>
       <c r="AB31" s="18"/>
       <c r="AC31" s="27"/>
     </row>
     <row r="32" spans="2:43" ht="15" customHeight="1">
-      <c r="B32" s="101"/>
-      <c r="C32" s="101"/>
-      <c r="D32" s="101"/>
-      <c r="E32" s="101"/>
-      <c r="F32" s="101"/>
-      <c r="G32" s="101"/>
-      <c r="H32" s="101"/>
-      <c r="I32" s="101"/>
-      <c r="J32" s="101"/>
-      <c r="K32" s="101"/>
-      <c r="L32" s="101"/>
-      <c r="M32" s="101"/>
-      <c r="N32" s="101"/>
-      <c r="O32" s="101"/>
+      <c r="B32" s="109"/>
+      <c r="C32" s="109"/>
+      <c r="D32" s="109"/>
+      <c r="E32" s="109"/>
+      <c r="F32" s="109"/>
+      <c r="G32" s="109"/>
+      <c r="H32" s="109"/>
+      <c r="I32" s="109"/>
+      <c r="J32" s="109"/>
+      <c r="K32" s="109"/>
+      <c r="L32" s="109"/>
+      <c r="M32" s="109"/>
+      <c r="N32" s="109"/>
+      <c r="O32" s="109"/>
       <c r="R32" s="26"/>
       <c r="S32" s="18"/>
       <c r="T32" s="18"/>
@@ -3292,61 +3302,61 @@
       <c r="AC32" s="27"/>
     </row>
     <row r="33" spans="2:32" ht="17.25" customHeight="1">
-      <c r="B33" s="101" t="s">
+      <c r="B33" s="109" t="s">
         <v>172</v>
       </c>
-      <c r="C33" s="101"/>
-      <c r="D33" s="101"/>
-      <c r="E33" s="101"/>
-      <c r="F33" s="101"/>
-      <c r="G33" s="101"/>
-      <c r="H33" s="101"/>
-      <c r="I33" s="101"/>
-      <c r="J33" s="101"/>
-      <c r="K33" s="101"/>
-      <c r="L33" s="101"/>
-      <c r="M33" s="101"/>
-      <c r="N33" s="101"/>
+      <c r="C33" s="109"/>
+      <c r="D33" s="109"/>
+      <c r="E33" s="109"/>
+      <c r="F33" s="109"/>
+      <c r="G33" s="109"/>
+      <c r="H33" s="109"/>
+      <c r="I33" s="109"/>
+      <c r="J33" s="109"/>
+      <c r="K33" s="109"/>
+      <c r="L33" s="109"/>
+      <c r="M33" s="109"/>
+      <c r="N33" s="109"/>
       <c r="R33" s="26"/>
-      <c r="S33" s="115" t="s">
+      <c r="S33" s="110" t="s">
         <v>108</v>
       </c>
-      <c r="T33" s="115"/>
-      <c r="U33" s="115"/>
-      <c r="V33" s="115"/>
-      <c r="W33" s="115"/>
-      <c r="X33" s="115"/>
-      <c r="Y33" s="115"/>
-      <c r="Z33" s="115"/>
-      <c r="AA33" s="115"/>
-      <c r="AB33" s="115"/>
+      <c r="T33" s="110"/>
+      <c r="U33" s="110"/>
+      <c r="V33" s="110"/>
+      <c r="W33" s="110"/>
+      <c r="X33" s="110"/>
+      <c r="Y33" s="110"/>
+      <c r="Z33" s="110"/>
+      <c r="AA33" s="110"/>
+      <c r="AB33" s="110"/>
       <c r="AC33" s="27"/>
     </row>
     <row r="34" spans="2:32" ht="17.25" customHeight="1">
-      <c r="B34" s="101"/>
-      <c r="C34" s="101"/>
-      <c r="D34" s="101"/>
-      <c r="E34" s="101"/>
-      <c r="F34" s="101"/>
-      <c r="G34" s="101"/>
-      <c r="H34" s="101"/>
-      <c r="I34" s="101"/>
-      <c r="J34" s="101"/>
-      <c r="K34" s="101"/>
-      <c r="L34" s="101"/>
-      <c r="M34" s="101"/>
-      <c r="N34" s="101"/>
+      <c r="B34" s="109"/>
+      <c r="C34" s="109"/>
+      <c r="D34" s="109"/>
+      <c r="E34" s="109"/>
+      <c r="F34" s="109"/>
+      <c r="G34" s="109"/>
+      <c r="H34" s="109"/>
+      <c r="I34" s="109"/>
+      <c r="J34" s="109"/>
+      <c r="K34" s="109"/>
+      <c r="L34" s="109"/>
+      <c r="M34" s="109"/>
+      <c r="N34" s="109"/>
       <c r="R34" s="26"/>
-      <c r="S34" s="115"/>
-      <c r="T34" s="115"/>
-      <c r="U34" s="115"/>
-      <c r="V34" s="115"/>
-      <c r="W34" s="115"/>
-      <c r="X34" s="115"/>
-      <c r="Y34" s="115"/>
-      <c r="Z34" s="115"/>
-      <c r="AA34" s="115"/>
-      <c r="AB34" s="115"/>
+      <c r="S34" s="110"/>
+      <c r="T34" s="110"/>
+      <c r="U34" s="110"/>
+      <c r="V34" s="110"/>
+      <c r="W34" s="110"/>
+      <c r="X34" s="110"/>
+      <c r="Y34" s="110"/>
+      <c r="Z34" s="110"/>
+      <c r="AA34" s="110"/>
+      <c r="AB34" s="110"/>
       <c r="AC34" s="27"/>
     </row>
     <row r="35" spans="2:32">
@@ -3384,67 +3394,67 @@
     </row>
     <row r="37" spans="2:32">
       <c r="R37" s="26"/>
-      <c r="S37" s="116" t="s">
+      <c r="S37" s="111" t="s">
         <v>111</v>
       </c>
-      <c r="T37" s="116"/>
-      <c r="U37" s="116"/>
-      <c r="V37" s="116"/>
-      <c r="W37" s="116"/>
-      <c r="X37" s="116"/>
-      <c r="Y37" s="116"/>
-      <c r="Z37" s="116"/>
-      <c r="AA37" s="116"/>
-      <c r="AB37" s="116"/>
+      <c r="T37" s="111"/>
+      <c r="U37" s="111"/>
+      <c r="V37" s="111"/>
+      <c r="W37" s="111"/>
+      <c r="X37" s="111"/>
+      <c r="Y37" s="111"/>
+      <c r="Z37" s="111"/>
+      <c r="AA37" s="111"/>
+      <c r="AB37" s="111"/>
       <c r="AC37" s="27"/>
       <c r="AF37" s="9"/>
     </row>
     <row r="38" spans="2:32">
-      <c r="B38" s="101" t="s">
+      <c r="B38" s="109" t="s">
         <v>142</v>
       </c>
-      <c r="C38" s="101"/>
-      <c r="D38" s="101"/>
-      <c r="E38" s="101"/>
-      <c r="F38" s="101"/>
-      <c r="G38" s="101"/>
-      <c r="H38" s="101"/>
-      <c r="I38" s="101"/>
-      <c r="J38" s="101"/>
-      <c r="K38" s="101"/>
-      <c r="L38" s="101"/>
-      <c r="M38" s="101"/>
-      <c r="N38" s="101"/>
-      <c r="O38" s="101"/>
+      <c r="C38" s="109"/>
+      <c r="D38" s="109"/>
+      <c r="E38" s="109"/>
+      <c r="F38" s="109"/>
+      <c r="G38" s="109"/>
+      <c r="H38" s="109"/>
+      <c r="I38" s="109"/>
+      <c r="J38" s="109"/>
+      <c r="K38" s="109"/>
+      <c r="L38" s="109"/>
+      <c r="M38" s="109"/>
+      <c r="N38" s="109"/>
+      <c r="O38" s="109"/>
       <c r="R38" s="26"/>
-      <c r="S38" s="116"/>
-      <c r="T38" s="116"/>
-      <c r="U38" s="116"/>
-      <c r="V38" s="116"/>
-      <c r="W38" s="116"/>
-      <c r="X38" s="116"/>
-      <c r="Y38" s="116"/>
-      <c r="Z38" s="116"/>
-      <c r="AA38" s="116"/>
-      <c r="AB38" s="116"/>
+      <c r="S38" s="111"/>
+      <c r="T38" s="111"/>
+      <c r="U38" s="111"/>
+      <c r="V38" s="111"/>
+      <c r="W38" s="111"/>
+      <c r="X38" s="111"/>
+      <c r="Y38" s="111"/>
+      <c r="Z38" s="111"/>
+      <c r="AA38" s="111"/>
+      <c r="AB38" s="111"/>
       <c r="AC38" s="27"/>
       <c r="AF38" s="9"/>
     </row>
     <row r="39" spans="2:32">
-      <c r="B39" s="101"/>
-      <c r="C39" s="101"/>
-      <c r="D39" s="101"/>
-      <c r="E39" s="101"/>
-      <c r="F39" s="101"/>
-      <c r="G39" s="101"/>
-      <c r="H39" s="101"/>
-      <c r="I39" s="101"/>
-      <c r="J39" s="101"/>
-      <c r="K39" s="101"/>
-      <c r="L39" s="101"/>
-      <c r="M39" s="101"/>
-      <c r="N39" s="101"/>
-      <c r="O39" s="101"/>
+      <c r="B39" s="109"/>
+      <c r="C39" s="109"/>
+      <c r="D39" s="109"/>
+      <c r="E39" s="109"/>
+      <c r="F39" s="109"/>
+      <c r="G39" s="109"/>
+      <c r="H39" s="109"/>
+      <c r="I39" s="109"/>
+      <c r="J39" s="109"/>
+      <c r="K39" s="109"/>
+      <c r="L39" s="109"/>
+      <c r="M39" s="109"/>
+      <c r="N39" s="109"/>
+      <c r="O39" s="109"/>
       <c r="R39" s="26"/>
       <c r="S39" s="18"/>
       <c r="T39" s="19"/>
@@ -3464,34 +3474,34 @@
       <c r="S40" s="18"/>
       <c r="T40" s="19"/>
       <c r="U40" s="19"/>
-      <c r="V40" s="112" t="s">
+      <c r="V40" s="120" t="s">
         <v>110</v>
       </c>
-      <c r="W40" s="112"/>
-      <c r="X40" s="112"/>
-      <c r="Y40" s="112"/>
-      <c r="Z40" s="112"/>
+      <c r="W40" s="120"/>
+      <c r="X40" s="120"/>
+      <c r="Y40" s="120"/>
+      <c r="Z40" s="120"/>
       <c r="AA40" s="19"/>
       <c r="AB40" s="19"/>
       <c r="AC40" s="27"/>
     </row>
     <row r="41" spans="2:32" ht="17.25">
-      <c r="B41" s="109" t="s">
+      <c r="B41" s="104" t="s">
         <v>104</v>
       </c>
-      <c r="C41" s="109"/>
-      <c r="D41" s="109"/>
-      <c r="E41" s="109"/>
-      <c r="F41" s="109"/>
-      <c r="G41" s="109"/>
-      <c r="H41" s="109"/>
-      <c r="I41" s="109"/>
-      <c r="J41" s="109"/>
-      <c r="K41" s="109"/>
-      <c r="L41" s="109"/>
-      <c r="M41" s="109"/>
-      <c r="N41" s="109"/>
-      <c r="O41" s="109"/>
+      <c r="C41" s="104"/>
+      <c r="D41" s="104"/>
+      <c r="E41" s="104"/>
+      <c r="F41" s="104"/>
+      <c r="G41" s="104"/>
+      <c r="H41" s="104"/>
+      <c r="I41" s="104"/>
+      <c r="J41" s="104"/>
+      <c r="K41" s="104"/>
+      <c r="L41" s="104"/>
+      <c r="M41" s="104"/>
+      <c r="N41" s="104"/>
+      <c r="O41" s="104"/>
       <c r="R41" s="26"/>
       <c r="S41" s="18"/>
       <c r="T41" s="18"/>
@@ -3507,18 +3517,18 @@
     </row>
     <row r="42" spans="2:32" ht="17.25">
       <c r="R42" s="26"/>
-      <c r="S42" s="113" t="s">
+      <c r="S42" s="112" t="s">
         <v>112</v>
       </c>
-      <c r="T42" s="113"/>
-      <c r="U42" s="113"/>
-      <c r="V42" s="113"/>
-      <c r="W42" s="113"/>
-      <c r="X42" s="113"/>
-      <c r="Y42" s="113"/>
-      <c r="Z42" s="113"/>
-      <c r="AA42" s="113"/>
-      <c r="AB42" s="113"/>
+      <c r="T42" s="112"/>
+      <c r="U42" s="112"/>
+      <c r="V42" s="112"/>
+      <c r="W42" s="112"/>
+      <c r="X42" s="112"/>
+      <c r="Y42" s="112"/>
+      <c r="Z42" s="112"/>
+      <c r="AA42" s="112"/>
+      <c r="AB42" s="112"/>
       <c r="AC42" s="27"/>
     </row>
     <row r="43" spans="2:32" ht="17.25">
@@ -3553,63 +3563,63 @@
       <c r="AC44" s="27"/>
     </row>
     <row r="45" spans="2:32">
-      <c r="B45" s="101" t="s">
+      <c r="B45" s="109" t="s">
         <v>143</v>
       </c>
-      <c r="C45" s="101"/>
-      <c r="D45" s="101"/>
-      <c r="E45" s="101"/>
-      <c r="F45" s="101"/>
-      <c r="G45" s="101"/>
-      <c r="H45" s="101"/>
-      <c r="I45" s="101"/>
-      <c r="J45" s="101"/>
-      <c r="K45" s="101"/>
-      <c r="L45" s="101"/>
-      <c r="M45" s="101"/>
-      <c r="N45" s="101"/>
-      <c r="O45" s="101"/>
+      <c r="C45" s="109"/>
+      <c r="D45" s="109"/>
+      <c r="E45" s="109"/>
+      <c r="F45" s="109"/>
+      <c r="G45" s="109"/>
+      <c r="H45" s="109"/>
+      <c r="I45" s="109"/>
+      <c r="J45" s="109"/>
+      <c r="K45" s="109"/>
+      <c r="L45" s="109"/>
+      <c r="M45" s="109"/>
+      <c r="N45" s="109"/>
+      <c r="O45" s="109"/>
       <c r="R45" s="26"/>
-      <c r="S45" s="115" t="s">
+      <c r="S45" s="110" t="s">
         <v>113</v>
       </c>
-      <c r="T45" s="115"/>
-      <c r="U45" s="115"/>
-      <c r="V45" s="115"/>
-      <c r="W45" s="115"/>
-      <c r="X45" s="115"/>
-      <c r="Y45" s="115"/>
-      <c r="Z45" s="115"/>
-      <c r="AA45" s="115"/>
-      <c r="AB45" s="115"/>
+      <c r="T45" s="110"/>
+      <c r="U45" s="110"/>
+      <c r="V45" s="110"/>
+      <c r="W45" s="110"/>
+      <c r="X45" s="110"/>
+      <c r="Y45" s="110"/>
+      <c r="Z45" s="110"/>
+      <c r="AA45" s="110"/>
+      <c r="AB45" s="110"/>
       <c r="AC45" s="27"/>
     </row>
     <row r="46" spans="2:32" ht="15" customHeight="1">
-      <c r="B46" s="101"/>
-      <c r="C46" s="101"/>
-      <c r="D46" s="101"/>
-      <c r="E46" s="101"/>
-      <c r="F46" s="101"/>
-      <c r="G46" s="101"/>
-      <c r="H46" s="101"/>
-      <c r="I46" s="101"/>
-      <c r="J46" s="101"/>
-      <c r="K46" s="101"/>
-      <c r="L46" s="101"/>
-      <c r="M46" s="101"/>
-      <c r="N46" s="101"/>
-      <c r="O46" s="101"/>
+      <c r="B46" s="109"/>
+      <c r="C46" s="109"/>
+      <c r="D46" s="109"/>
+      <c r="E46" s="109"/>
+      <c r="F46" s="109"/>
+      <c r="G46" s="109"/>
+      <c r="H46" s="109"/>
+      <c r="I46" s="109"/>
+      <c r="J46" s="109"/>
+      <c r="K46" s="109"/>
+      <c r="L46" s="109"/>
+      <c r="M46" s="109"/>
+      <c r="N46" s="109"/>
+      <c r="O46" s="109"/>
       <c r="R46" s="26"/>
-      <c r="S46" s="115"/>
-      <c r="T46" s="115"/>
-      <c r="U46" s="115"/>
-      <c r="V46" s="115"/>
-      <c r="W46" s="115"/>
-      <c r="X46" s="115"/>
-      <c r="Y46" s="115"/>
-      <c r="Z46" s="115"/>
-      <c r="AA46" s="115"/>
-      <c r="AB46" s="115"/>
+      <c r="S46" s="110"/>
+      <c r="T46" s="110"/>
+      <c r="U46" s="110"/>
+      <c r="V46" s="110"/>
+      <c r="W46" s="110"/>
+      <c r="X46" s="110"/>
+      <c r="Y46" s="110"/>
+      <c r="Z46" s="110"/>
+      <c r="AA46" s="110"/>
+      <c r="AB46" s="110"/>
       <c r="AC46" s="27"/>
     </row>
     <row r="47" spans="2:32" ht="15" customHeight="1">
@@ -3634,13 +3644,13 @@
       <c r="S48" s="18"/>
       <c r="T48" s="18"/>
       <c r="U48" s="18"/>
-      <c r="V48" s="118" t="s">
+      <c r="V48" s="107" t="s">
         <v>114</v>
       </c>
-      <c r="W48" s="118"/>
-      <c r="X48" s="118"/>
-      <c r="Y48" s="118"/>
-      <c r="Z48" s="118"/>
+      <c r="W48" s="107"/>
+      <c r="X48" s="107"/>
+      <c r="Y48" s="107"/>
+      <c r="Z48" s="107"/>
       <c r="AA48" s="18"/>
       <c r="AB48" s="18"/>
       <c r="AC48" s="27"/>
@@ -3660,52 +3670,52 @@
       <c r="AC49" s="27"/>
     </row>
     <row r="50" spans="2:43">
-      <c r="B50" s="101" t="s">
+      <c r="B50" s="109" t="s">
         <v>145</v>
       </c>
-      <c r="C50" s="101"/>
-      <c r="D50" s="101"/>
-      <c r="E50" s="101"/>
-      <c r="F50" s="101"/>
-      <c r="G50" s="101"/>
-      <c r="H50" s="101"/>
-      <c r="I50" s="101"/>
-      <c r="J50" s="101"/>
-      <c r="K50" s="101"/>
-      <c r="L50" s="101"/>
-      <c r="M50" s="101"/>
-      <c r="N50" s="101"/>
-      <c r="O50" s="101"/>
+      <c r="C50" s="109"/>
+      <c r="D50" s="109"/>
+      <c r="E50" s="109"/>
+      <c r="F50" s="109"/>
+      <c r="G50" s="109"/>
+      <c r="H50" s="109"/>
+      <c r="I50" s="109"/>
+      <c r="J50" s="109"/>
+      <c r="K50" s="109"/>
+      <c r="L50" s="109"/>
+      <c r="M50" s="109"/>
+      <c r="N50" s="109"/>
+      <c r="O50" s="109"/>
       <c r="R50" s="26"/>
-      <c r="S50" s="106" t="s">
+      <c r="S50" s="108" t="s">
         <v>115</v>
       </c>
-      <c r="T50" s="106"/>
-      <c r="U50" s="106"/>
-      <c r="V50" s="106"/>
-      <c r="W50" s="106"/>
-      <c r="X50" s="106"/>
-      <c r="Y50" s="106"/>
-      <c r="Z50" s="106"/>
-      <c r="AA50" s="106"/>
-      <c r="AB50" s="106"/>
+      <c r="T50" s="108"/>
+      <c r="U50" s="108"/>
+      <c r="V50" s="108"/>
+      <c r="W50" s="108"/>
+      <c r="X50" s="108"/>
+      <c r="Y50" s="108"/>
+      <c r="Z50" s="108"/>
+      <c r="AA50" s="108"/>
+      <c r="AB50" s="108"/>
       <c r="AC50" s="27"/>
     </row>
     <row r="51" spans="2:43" ht="15" customHeight="1">
-      <c r="B51" s="101"/>
-      <c r="C51" s="101"/>
-      <c r="D51" s="101"/>
-      <c r="E51" s="101"/>
-      <c r="F51" s="101"/>
-      <c r="G51" s="101"/>
-      <c r="H51" s="101"/>
-      <c r="I51" s="101"/>
-      <c r="J51" s="101"/>
-      <c r="K51" s="101"/>
-      <c r="L51" s="101"/>
-      <c r="M51" s="101"/>
-      <c r="N51" s="101"/>
-      <c r="O51" s="101"/>
+      <c r="B51" s="109"/>
+      <c r="C51" s="109"/>
+      <c r="D51" s="109"/>
+      <c r="E51" s="109"/>
+      <c r="F51" s="109"/>
+      <c r="G51" s="109"/>
+      <c r="H51" s="109"/>
+      <c r="I51" s="109"/>
+      <c r="J51" s="109"/>
+      <c r="K51" s="109"/>
+      <c r="L51" s="109"/>
+      <c r="M51" s="109"/>
+      <c r="N51" s="109"/>
+      <c r="O51" s="109"/>
       <c r="R51" s="26"/>
       <c r="S51" s="18"/>
       <c r="T51" s="18"/>
@@ -3721,18 +3731,18 @@
     </row>
     <row r="52" spans="2:43">
       <c r="R52" s="26"/>
-      <c r="S52" s="106" t="s">
+      <c r="S52" s="108" t="s">
         <v>116</v>
       </c>
-      <c r="T52" s="106"/>
-      <c r="U52" s="106"/>
-      <c r="V52" s="106"/>
-      <c r="W52" s="106"/>
-      <c r="X52" s="106"/>
-      <c r="Y52" s="106"/>
-      <c r="Z52" s="106"/>
-      <c r="AA52" s="106"/>
-      <c r="AB52" s="106"/>
+      <c r="T52" s="108"/>
+      <c r="U52" s="108"/>
+      <c r="V52" s="108"/>
+      <c r="W52" s="108"/>
+      <c r="X52" s="108"/>
+      <c r="Y52" s="108"/>
+      <c r="Z52" s="108"/>
+      <c r="AA52" s="108"/>
+      <c r="AB52" s="108"/>
       <c r="AC52" s="27"/>
     </row>
     <row r="53" spans="2:43" ht="15.75" customHeight="1">
@@ -3740,16 +3750,16 @@
         <v>147</v>
       </c>
       <c r="R53" s="26"/>
-      <c r="S53" s="106"/>
-      <c r="T53" s="106"/>
-      <c r="U53" s="106"/>
-      <c r="V53" s="106"/>
-      <c r="W53" s="106"/>
-      <c r="X53" s="106"/>
-      <c r="Y53" s="106"/>
-      <c r="Z53" s="106"/>
-      <c r="AA53" s="106"/>
-      <c r="AB53" s="106"/>
+      <c r="S53" s="108"/>
+      <c r="T53" s="108"/>
+      <c r="U53" s="108"/>
+      <c r="V53" s="108"/>
+      <c r="W53" s="108"/>
+      <c r="X53" s="108"/>
+      <c r="Y53" s="108"/>
+      <c r="Z53" s="108"/>
+      <c r="AA53" s="108"/>
+      <c r="AB53" s="108"/>
       <c r="AC53" s="27"/>
       <c r="AH53" s="22"/>
       <c r="AI53" s="22"/>
@@ -3777,22 +3787,22 @@
       <c r="AC54" s="27"/>
     </row>
     <row r="55" spans="2:43">
-      <c r="B55" s="101" t="s">
+      <c r="B55" s="109" t="s">
         <v>154</v>
       </c>
-      <c r="C55" s="101"/>
-      <c r="D55" s="101"/>
-      <c r="E55" s="101"/>
-      <c r="F55" s="101"/>
-      <c r="G55" s="101"/>
-      <c r="H55" s="101"/>
-      <c r="I55" s="101"/>
-      <c r="J55" s="101"/>
-      <c r="K55" s="101"/>
-      <c r="L55" s="101"/>
-      <c r="M55" s="101"/>
-      <c r="N55" s="101"/>
-      <c r="O55" s="101"/>
+      <c r="C55" s="109"/>
+      <c r="D55" s="109"/>
+      <c r="E55" s="109"/>
+      <c r="F55" s="109"/>
+      <c r="G55" s="109"/>
+      <c r="H55" s="109"/>
+      <c r="I55" s="109"/>
+      <c r="J55" s="109"/>
+      <c r="K55" s="109"/>
+      <c r="L55" s="109"/>
+      <c r="M55" s="109"/>
+      <c r="N55" s="109"/>
+      <c r="O55" s="109"/>
       <c r="R55" s="28"/>
       <c r="S55" s="29"/>
       <c r="T55" s="29"/>
@@ -3807,272 +3817,272 @@
       <c r="AC55" s="30"/>
     </row>
     <row r="56" spans="2:43">
-      <c r="B56" s="101"/>
-      <c r="C56" s="101"/>
-      <c r="D56" s="101"/>
-      <c r="E56" s="101"/>
-      <c r="F56" s="101"/>
-      <c r="G56" s="101"/>
-      <c r="H56" s="101"/>
-      <c r="I56" s="101"/>
-      <c r="J56" s="101"/>
-      <c r="K56" s="101"/>
-      <c r="L56" s="101"/>
-      <c r="M56" s="101"/>
-      <c r="N56" s="101"/>
-      <c r="O56" s="101"/>
+      <c r="B56" s="109"/>
+      <c r="C56" s="109"/>
+      <c r="D56" s="109"/>
+      <c r="E56" s="109"/>
+      <c r="F56" s="109"/>
+      <c r="G56" s="109"/>
+      <c r="H56" s="109"/>
+      <c r="I56" s="109"/>
+      <c r="J56" s="109"/>
+      <c r="K56" s="109"/>
+      <c r="L56" s="109"/>
+      <c r="M56" s="109"/>
+      <c r="N56" s="109"/>
+      <c r="O56" s="109"/>
     </row>
     <row r="58" spans="2:43" ht="17.25">
-      <c r="B58" s="109" t="s">
+      <c r="B58" s="104" t="s">
         <v>97</v>
       </c>
-      <c r="C58" s="109"/>
-      <c r="D58" s="109"/>
-      <c r="E58" s="109"/>
-      <c r="F58" s="109"/>
-      <c r="G58" s="109"/>
-      <c r="H58" s="109"/>
-      <c r="I58" s="109"/>
-      <c r="J58" s="109"/>
-      <c r="K58" s="109"/>
-      <c r="L58" s="109"/>
-      <c r="M58" s="109"/>
-      <c r="N58" s="109"/>
-      <c r="O58" s="109"/>
-      <c r="Q58" s="117" t="s">
+      <c r="C58" s="104"/>
+      <c r="D58" s="104"/>
+      <c r="E58" s="104"/>
+      <c r="F58" s="104"/>
+      <c r="G58" s="104"/>
+      <c r="H58" s="104"/>
+      <c r="I58" s="104"/>
+      <c r="J58" s="104"/>
+      <c r="K58" s="104"/>
+      <c r="L58" s="104"/>
+      <c r="M58" s="104"/>
+      <c r="N58" s="104"/>
+      <c r="O58" s="104"/>
+      <c r="Q58" s="105" t="s">
         <v>169</v>
       </c>
-      <c r="R58" s="117"/>
-      <c r="S58" s="117"/>
-      <c r="T58" s="117"/>
-      <c r="U58" s="117"/>
-      <c r="V58" s="117"/>
-      <c r="W58" s="117"/>
-      <c r="X58" s="117"/>
-      <c r="Y58" s="117"/>
-      <c r="Z58" s="117"/>
-      <c r="AA58" s="117"/>
-      <c r="AB58" s="117"/>
-      <c r="AC58" s="117"/>
-      <c r="AD58" s="117"/>
+      <c r="R58" s="105"/>
+      <c r="S58" s="105"/>
+      <c r="T58" s="105"/>
+      <c r="U58" s="105"/>
+      <c r="V58" s="105"/>
+      <c r="W58" s="105"/>
+      <c r="X58" s="105"/>
+      <c r="Y58" s="105"/>
+      <c r="Z58" s="105"/>
+      <c r="AA58" s="105"/>
+      <c r="AB58" s="105"/>
+      <c r="AC58" s="105"/>
+      <c r="AD58" s="105"/>
     </row>
     <row r="60" spans="2:43" ht="17.25">
-      <c r="B60" s="102" t="s">
+      <c r="B60" s="106" t="s">
         <v>198</v>
       </c>
-      <c r="C60" s="102"/>
-      <c r="D60" s="102"/>
-      <c r="E60" s="102"/>
-      <c r="F60" s="102"/>
-      <c r="G60" s="102"/>
-      <c r="H60" s="102"/>
-      <c r="I60" s="102"/>
-      <c r="J60" s="102"/>
-      <c r="K60" s="102"/>
-      <c r="L60" s="102"/>
-      <c r="M60" s="102"/>
-      <c r="N60" s="102"/>
-      <c r="O60" s="102"/>
+      <c r="C60" s="106"/>
+      <c r="D60" s="106"/>
+      <c r="E60" s="106"/>
+      <c r="F60" s="106"/>
+      <c r="G60" s="106"/>
+      <c r="H60" s="106"/>
+      <c r="I60" s="106"/>
+      <c r="J60" s="106"/>
+      <c r="K60" s="106"/>
+      <c r="L60" s="106"/>
+      <c r="M60" s="106"/>
+      <c r="N60" s="106"/>
+      <c r="O60" s="106"/>
       <c r="Q60" s="20" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="61" spans="2:43">
-      <c r="B61" s="102"/>
-      <c r="C61" s="102"/>
-      <c r="D61" s="102"/>
-      <c r="E61" s="102"/>
-      <c r="F61" s="102"/>
-      <c r="G61" s="102"/>
-      <c r="H61" s="102"/>
-      <c r="I61" s="102"/>
-      <c r="J61" s="102"/>
-      <c r="K61" s="102"/>
-      <c r="L61" s="102"/>
-      <c r="M61" s="102"/>
-      <c r="N61" s="102"/>
-      <c r="O61" s="102"/>
+      <c r="B61" s="106"/>
+      <c r="C61" s="106"/>
+      <c r="D61" s="106"/>
+      <c r="E61" s="106"/>
+      <c r="F61" s="106"/>
+      <c r="G61" s="106"/>
+      <c r="H61" s="106"/>
+      <c r="I61" s="106"/>
+      <c r="J61" s="106"/>
+      <c r="K61" s="106"/>
+      <c r="L61" s="106"/>
+      <c r="M61" s="106"/>
+      <c r="N61" s="106"/>
+      <c r="O61" s="106"/>
     </row>
     <row r="62" spans="2:43">
-      <c r="Q62" s="101" t="s">
+      <c r="Q62" s="109" t="s">
         <v>195</v>
       </c>
-      <c r="R62" s="101"/>
-      <c r="S62" s="101"/>
-      <c r="T62" s="101"/>
-      <c r="U62" s="101"/>
-      <c r="V62" s="101"/>
-      <c r="W62" s="101"/>
-      <c r="X62" s="101"/>
-      <c r="Y62" s="101"/>
-      <c r="Z62" s="101"/>
-      <c r="AA62" s="101"/>
-      <c r="AB62" s="101"/>
-      <c r="AC62" s="101"/>
-      <c r="AD62" s="101"/>
+      <c r="R62" s="109"/>
+      <c r="S62" s="109"/>
+      <c r="T62" s="109"/>
+      <c r="U62" s="109"/>
+      <c r="V62" s="109"/>
+      <c r="W62" s="109"/>
+      <c r="X62" s="109"/>
+      <c r="Y62" s="109"/>
+      <c r="Z62" s="109"/>
+      <c r="AA62" s="109"/>
+      <c r="AB62" s="109"/>
+      <c r="AC62" s="109"/>
+      <c r="AD62" s="109"/>
     </row>
     <row r="63" spans="2:43" ht="15" customHeight="1">
-      <c r="B63" s="102" t="s">
+      <c r="B63" s="106" t="s">
         <v>213</v>
       </c>
-      <c r="C63" s="102"/>
-      <c r="D63" s="102"/>
-      <c r="E63" s="102"/>
-      <c r="F63" s="102"/>
-      <c r="G63" s="102"/>
-      <c r="H63" s="102"/>
-      <c r="I63" s="102"/>
-      <c r="J63" s="102"/>
-      <c r="K63" s="102"/>
-      <c r="L63" s="102"/>
-      <c r="M63" s="102"/>
-      <c r="N63" s="102"/>
-      <c r="O63" s="102"/>
-      <c r="Q63" s="101"/>
-      <c r="R63" s="101"/>
-      <c r="S63" s="101"/>
-      <c r="T63" s="101"/>
-      <c r="U63" s="101"/>
-      <c r="V63" s="101"/>
-      <c r="W63" s="101"/>
-      <c r="X63" s="101"/>
-      <c r="Y63" s="101"/>
-      <c r="Z63" s="101"/>
-      <c r="AA63" s="101"/>
-      <c r="AB63" s="101"/>
-      <c r="AC63" s="101"/>
-      <c r="AD63" s="101"/>
+      <c r="C63" s="106"/>
+      <c r="D63" s="106"/>
+      <c r="E63" s="106"/>
+      <c r="F63" s="106"/>
+      <c r="G63" s="106"/>
+      <c r="H63" s="106"/>
+      <c r="I63" s="106"/>
+      <c r="J63" s="106"/>
+      <c r="K63" s="106"/>
+      <c r="L63" s="106"/>
+      <c r="M63" s="106"/>
+      <c r="N63" s="106"/>
+      <c r="O63" s="106"/>
+      <c r="Q63" s="109"/>
+      <c r="R63" s="109"/>
+      <c r="S63" s="109"/>
+      <c r="T63" s="109"/>
+      <c r="U63" s="109"/>
+      <c r="V63" s="109"/>
+      <c r="W63" s="109"/>
+      <c r="X63" s="109"/>
+      <c r="Y63" s="109"/>
+      <c r="Z63" s="109"/>
+      <c r="AA63" s="109"/>
+      <c r="AB63" s="109"/>
+      <c r="AC63" s="109"/>
+      <c r="AD63" s="109"/>
     </row>
     <row r="64" spans="2:43">
-      <c r="B64" s="102"/>
-      <c r="C64" s="102"/>
-      <c r="D64" s="102"/>
-      <c r="E64" s="102"/>
-      <c r="F64" s="102"/>
-      <c r="G64" s="102"/>
-      <c r="H64" s="102"/>
-      <c r="I64" s="102"/>
-      <c r="J64" s="102"/>
-      <c r="K64" s="102"/>
-      <c r="L64" s="102"/>
-      <c r="M64" s="102"/>
-      <c r="N64" s="102"/>
-      <c r="O64" s="102"/>
+      <c r="B64" s="106"/>
+      <c r="C64" s="106"/>
+      <c r="D64" s="106"/>
+      <c r="E64" s="106"/>
+      <c r="F64" s="106"/>
+      <c r="G64" s="106"/>
+      <c r="H64" s="106"/>
+      <c r="I64" s="106"/>
+      <c r="J64" s="106"/>
+      <c r="K64" s="106"/>
+      <c r="L64" s="106"/>
+      <c r="M64" s="106"/>
+      <c r="N64" s="106"/>
+      <c r="O64" s="106"/>
     </row>
     <row r="65" spans="2:30" ht="17.25">
-      <c r="B65" s="102"/>
-      <c r="C65" s="102"/>
-      <c r="D65" s="102"/>
-      <c r="E65" s="102"/>
-      <c r="F65" s="102"/>
-      <c r="G65" s="102"/>
-      <c r="H65" s="102"/>
-      <c r="I65" s="102"/>
-      <c r="J65" s="102"/>
-      <c r="K65" s="102"/>
-      <c r="L65" s="102"/>
-      <c r="M65" s="102"/>
-      <c r="N65" s="102"/>
-      <c r="O65" s="102"/>
+      <c r="B65" s="106"/>
+      <c r="C65" s="106"/>
+      <c r="D65" s="106"/>
+      <c r="E65" s="106"/>
+      <c r="F65" s="106"/>
+      <c r="G65" s="106"/>
+      <c r="H65" s="106"/>
+      <c r="I65" s="106"/>
+      <c r="J65" s="106"/>
+      <c r="K65" s="106"/>
+      <c r="L65" s="106"/>
+      <c r="M65" s="106"/>
+      <c r="N65" s="106"/>
+      <c r="O65" s="106"/>
       <c r="Q65" s="20" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="66" spans="2:30">
-      <c r="B66" s="102"/>
-      <c r="C66" s="102"/>
-      <c r="D66" s="102"/>
-      <c r="E66" s="102"/>
-      <c r="F66" s="102"/>
-      <c r="G66" s="102"/>
-      <c r="H66" s="102"/>
-      <c r="I66" s="102"/>
-      <c r="J66" s="102"/>
-      <c r="K66" s="102"/>
-      <c r="L66" s="102"/>
-      <c r="M66" s="102"/>
-      <c r="N66" s="102"/>
-      <c r="O66" s="102"/>
+      <c r="B66" s="106"/>
+      <c r="C66" s="106"/>
+      <c r="D66" s="106"/>
+      <c r="E66" s="106"/>
+      <c r="F66" s="106"/>
+      <c r="G66" s="106"/>
+      <c r="H66" s="106"/>
+      <c r="I66" s="106"/>
+      <c r="J66" s="106"/>
+      <c r="K66" s="106"/>
+      <c r="L66" s="106"/>
+      <c r="M66" s="106"/>
+      <c r="N66" s="106"/>
+      <c r="O66" s="106"/>
     </row>
     <row r="67" spans="2:30" ht="15" customHeight="1">
-      <c r="B67" s="101" t="s">
+      <c r="B67" s="109" t="s">
         <v>200</v>
       </c>
-      <c r="C67" s="101"/>
-      <c r="D67" s="101"/>
-      <c r="E67" s="101"/>
-      <c r="F67" s="101"/>
-      <c r="G67" s="101"/>
-      <c r="H67" s="101"/>
-      <c r="I67" s="101"/>
-      <c r="J67" s="101"/>
-      <c r="K67" s="101"/>
-      <c r="L67" s="101"/>
-      <c r="M67" s="101"/>
-      <c r="N67" s="101"/>
-      <c r="O67" s="101"/>
-      <c r="Q67" s="101" t="s">
+      <c r="C67" s="109"/>
+      <c r="D67" s="109"/>
+      <c r="E67" s="109"/>
+      <c r="F67" s="109"/>
+      <c r="G67" s="109"/>
+      <c r="H67" s="109"/>
+      <c r="I67" s="109"/>
+      <c r="J67" s="109"/>
+      <c r="K67" s="109"/>
+      <c r="L67" s="109"/>
+      <c r="M67" s="109"/>
+      <c r="N67" s="109"/>
+      <c r="O67" s="109"/>
+      <c r="Q67" s="109" t="s">
         <v>209</v>
       </c>
-      <c r="R67" s="101"/>
-      <c r="S67" s="101"/>
-      <c r="T67" s="101"/>
-      <c r="U67" s="101"/>
-      <c r="V67" s="101"/>
-      <c r="W67" s="101"/>
-      <c r="X67" s="101"/>
-      <c r="Y67" s="101"/>
-      <c r="Z67" s="101"/>
-      <c r="AA67" s="101"/>
-      <c r="AB67" s="101"/>
-      <c r="AC67" s="101"/>
-      <c r="AD67" s="101"/>
+      <c r="R67" s="109"/>
+      <c r="S67" s="109"/>
+      <c r="T67" s="109"/>
+      <c r="U67" s="109"/>
+      <c r="V67" s="109"/>
+      <c r="W67" s="109"/>
+      <c r="X67" s="109"/>
+      <c r="Y67" s="109"/>
+      <c r="Z67" s="109"/>
+      <c r="AA67" s="109"/>
+      <c r="AB67" s="109"/>
+      <c r="AC67" s="109"/>
+      <c r="AD67" s="109"/>
     </row>
     <row r="68" spans="2:30">
-      <c r="B68" s="101"/>
-      <c r="C68" s="101"/>
-      <c r="D68" s="101"/>
-      <c r="E68" s="101"/>
-      <c r="F68" s="101"/>
-      <c r="G68" s="101"/>
-      <c r="H68" s="101"/>
-      <c r="I68" s="101"/>
-      <c r="J68" s="101"/>
-      <c r="K68" s="101"/>
-      <c r="L68" s="101"/>
-      <c r="M68" s="101"/>
-      <c r="N68" s="101"/>
-      <c r="O68" s="101"/>
-      <c r="Q68" s="101"/>
-      <c r="R68" s="101"/>
-      <c r="S68" s="101"/>
-      <c r="T68" s="101"/>
-      <c r="U68" s="101"/>
-      <c r="V68" s="101"/>
-      <c r="W68" s="101"/>
-      <c r="X68" s="101"/>
-      <c r="Y68" s="101"/>
-      <c r="Z68" s="101"/>
-      <c r="AA68" s="101"/>
-      <c r="AB68" s="101"/>
-      <c r="AC68" s="101"/>
-      <c r="AD68" s="101"/>
+      <c r="B68" s="109"/>
+      <c r="C68" s="109"/>
+      <c r="D68" s="109"/>
+      <c r="E68" s="109"/>
+      <c r="F68" s="109"/>
+      <c r="G68" s="109"/>
+      <c r="H68" s="109"/>
+      <c r="I68" s="109"/>
+      <c r="J68" s="109"/>
+      <c r="K68" s="109"/>
+      <c r="L68" s="109"/>
+      <c r="M68" s="109"/>
+      <c r="N68" s="109"/>
+      <c r="O68" s="109"/>
+      <c r="Q68" s="109"/>
+      <c r="R68" s="109"/>
+      <c r="S68" s="109"/>
+      <c r="T68" s="109"/>
+      <c r="U68" s="109"/>
+      <c r="V68" s="109"/>
+      <c r="W68" s="109"/>
+      <c r="X68" s="109"/>
+      <c r="Y68" s="109"/>
+      <c r="Z68" s="109"/>
+      <c r="AA68" s="109"/>
+      <c r="AB68" s="109"/>
+      <c r="AC68" s="109"/>
+      <c r="AD68" s="109"/>
     </row>
     <row r="69" spans="2:30">
-      <c r="Q69" s="101"/>
-      <c r="R69" s="101"/>
-      <c r="S69" s="101"/>
-      <c r="T69" s="101"/>
-      <c r="U69" s="101"/>
-      <c r="V69" s="101"/>
-      <c r="W69" s="101"/>
-      <c r="X69" s="101"/>
-      <c r="Y69" s="101"/>
-      <c r="Z69" s="101"/>
-      <c r="AA69" s="101"/>
-      <c r="AB69" s="101"/>
-      <c r="AC69" s="101"/>
-      <c r="AD69" s="101"/>
+      <c r="Q69" s="109"/>
+      <c r="R69" s="109"/>
+      <c r="S69" s="109"/>
+      <c r="T69" s="109"/>
+      <c r="U69" s="109"/>
+      <c r="V69" s="109"/>
+      <c r="W69" s="109"/>
+      <c r="X69" s="109"/>
+      <c r="Y69" s="109"/>
+      <c r="Z69" s="109"/>
+      <c r="AA69" s="109"/>
+      <c r="AB69" s="109"/>
+      <c r="AC69" s="109"/>
+      <c r="AD69" s="109"/>
     </row>
     <row r="70" spans="2:30" ht="17.25">
       <c r="B70" s="10" t="s">
@@ -4085,207 +4095,196 @@
       </c>
     </row>
     <row r="73" spans="2:30">
-      <c r="Q73" s="102" t="s">
+      <c r="Q73" s="106" t="s">
         <v>203</v>
       </c>
-      <c r="R73" s="102"/>
-      <c r="S73" s="102"/>
-      <c r="T73" s="102"/>
-      <c r="U73" s="102"/>
-      <c r="V73" s="102"/>
-      <c r="W73" s="102"/>
-      <c r="X73" s="102"/>
-      <c r="Y73" s="102"/>
-      <c r="Z73" s="102"/>
-      <c r="AA73" s="102"/>
-      <c r="AB73" s="102"/>
-      <c r="AC73" s="102"/>
-      <c r="AD73" s="102"/>
+      <c r="R73" s="106"/>
+      <c r="S73" s="106"/>
+      <c r="T73" s="106"/>
+      <c r="U73" s="106"/>
+      <c r="V73" s="106"/>
+      <c r="W73" s="106"/>
+      <c r="X73" s="106"/>
+      <c r="Y73" s="106"/>
+      <c r="Z73" s="106"/>
+      <c r="AA73" s="106"/>
+      <c r="AB73" s="106"/>
+      <c r="AC73" s="106"/>
+      <c r="AD73" s="106"/>
     </row>
     <row r="74" spans="2:30">
-      <c r="Q74" s="102"/>
-      <c r="R74" s="102"/>
-      <c r="S74" s="102"/>
-      <c r="T74" s="102"/>
-      <c r="U74" s="102"/>
-      <c r="V74" s="102"/>
-      <c r="W74" s="102"/>
-      <c r="X74" s="102"/>
-      <c r="Y74" s="102"/>
-      <c r="Z74" s="102"/>
-      <c r="AA74" s="102"/>
-      <c r="AB74" s="102"/>
-      <c r="AC74" s="102"/>
-      <c r="AD74" s="102"/>
+      <c r="Q74" s="106"/>
+      <c r="R74" s="106"/>
+      <c r="S74" s="106"/>
+      <c r="T74" s="106"/>
+      <c r="U74" s="106"/>
+      <c r="V74" s="106"/>
+      <c r="W74" s="106"/>
+      <c r="X74" s="106"/>
+      <c r="Y74" s="106"/>
+      <c r="Z74" s="106"/>
+      <c r="AA74" s="106"/>
+      <c r="AB74" s="106"/>
+      <c r="AC74" s="106"/>
+      <c r="AD74" s="106"/>
     </row>
     <row r="75" spans="2:30" ht="15" customHeight="1">
-      <c r="Q75" s="102"/>
-      <c r="R75" s="102"/>
-      <c r="S75" s="102"/>
-      <c r="T75" s="102"/>
-      <c r="U75" s="102"/>
-      <c r="V75" s="102"/>
-      <c r="W75" s="102"/>
-      <c r="X75" s="102"/>
-      <c r="Y75" s="102"/>
-      <c r="Z75" s="102"/>
-      <c r="AA75" s="102"/>
-      <c r="AB75" s="102"/>
-      <c r="AC75" s="102"/>
-      <c r="AD75" s="102"/>
+      <c r="Q75" s="106"/>
+      <c r="R75" s="106"/>
+      <c r="S75" s="106"/>
+      <c r="T75" s="106"/>
+      <c r="U75" s="106"/>
+      <c r="V75" s="106"/>
+      <c r="W75" s="106"/>
+      <c r="X75" s="106"/>
+      <c r="Y75" s="106"/>
+      <c r="Z75" s="106"/>
+      <c r="AA75" s="106"/>
+      <c r="AB75" s="106"/>
+      <c r="AC75" s="106"/>
+      <c r="AD75" s="106"/>
     </row>
     <row r="76" spans="2:30">
-      <c r="Q76" s="102"/>
-      <c r="R76" s="102"/>
-      <c r="S76" s="102"/>
-      <c r="T76" s="102"/>
-      <c r="U76" s="102"/>
-      <c r="V76" s="102"/>
-      <c r="W76" s="102"/>
-      <c r="X76" s="102"/>
-      <c r="Y76" s="102"/>
-      <c r="Z76" s="102"/>
-      <c r="AA76" s="102"/>
-      <c r="AB76" s="102"/>
-      <c r="AC76" s="102"/>
-      <c r="AD76" s="102"/>
+      <c r="Q76" s="106"/>
+      <c r="R76" s="106"/>
+      <c r="S76" s="106"/>
+      <c r="T76" s="106"/>
+      <c r="U76" s="106"/>
+      <c r="V76" s="106"/>
+      <c r="W76" s="106"/>
+      <c r="X76" s="106"/>
+      <c r="Y76" s="106"/>
+      <c r="Z76" s="106"/>
+      <c r="AA76" s="106"/>
+      <c r="AB76" s="106"/>
+      <c r="AC76" s="106"/>
+      <c r="AD76" s="106"/>
     </row>
     <row r="77" spans="2:30">
-      <c r="Q77" s="102"/>
-      <c r="R77" s="102"/>
-      <c r="S77" s="102"/>
-      <c r="T77" s="102"/>
-      <c r="U77" s="102"/>
-      <c r="V77" s="102"/>
-      <c r="W77" s="102"/>
-      <c r="X77" s="102"/>
-      <c r="Y77" s="102"/>
-      <c r="Z77" s="102"/>
-      <c r="AA77" s="102"/>
-      <c r="AB77" s="102"/>
-      <c r="AC77" s="102"/>
-      <c r="AD77" s="102"/>
+      <c r="Q77" s="106"/>
+      <c r="R77" s="106"/>
+      <c r="S77" s="106"/>
+      <c r="T77" s="106"/>
+      <c r="U77" s="106"/>
+      <c r="V77" s="106"/>
+      <c r="W77" s="106"/>
+      <c r="X77" s="106"/>
+      <c r="Y77" s="106"/>
+      <c r="Z77" s="106"/>
+      <c r="AA77" s="106"/>
+      <c r="AB77" s="106"/>
+      <c r="AC77" s="106"/>
+      <c r="AD77" s="106"/>
     </row>
     <row r="79" spans="2:30" ht="17.25">
-      <c r="B79" s="109" t="s">
+      <c r="B79" s="104" t="s">
         <v>101</v>
       </c>
-      <c r="C79" s="109"/>
-      <c r="D79" s="109"/>
-      <c r="E79" s="109"/>
-      <c r="F79" s="109"/>
-      <c r="G79" s="109"/>
-      <c r="H79" s="109"/>
-      <c r="I79" s="109"/>
-      <c r="J79" s="109"/>
-      <c r="K79" s="109"/>
-      <c r="L79" s="109"/>
-      <c r="M79" s="109"/>
-      <c r="N79" s="109"/>
-      <c r="O79" s="109"/>
+      <c r="C79" s="104"/>
+      <c r="D79" s="104"/>
+      <c r="E79" s="104"/>
+      <c r="F79" s="104"/>
+      <c r="G79" s="104"/>
+      <c r="H79" s="104"/>
+      <c r="I79" s="104"/>
+      <c r="J79" s="104"/>
+      <c r="K79" s="104"/>
+      <c r="L79" s="104"/>
+      <c r="M79" s="104"/>
+      <c r="N79" s="104"/>
+      <c r="O79" s="104"/>
       <c r="Q79" s="20" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="81" spans="2:30" ht="15" customHeight="1">
-      <c r="B81" s="101" t="s">
+      <c r="B81" s="109" t="s">
         <v>193</v>
       </c>
-      <c r="C81" s="101"/>
-      <c r="D81" s="101"/>
-      <c r="E81" s="101"/>
-      <c r="F81" s="101"/>
-      <c r="G81" s="101"/>
-      <c r="H81" s="101"/>
-      <c r="I81" s="101"/>
-      <c r="J81" s="101"/>
-      <c r="K81" s="101"/>
-      <c r="L81" s="101"/>
-      <c r="M81" s="101"/>
-      <c r="N81" s="101"/>
-      <c r="O81" s="101"/>
-      <c r="Q81" s="102" t="s">
+      <c r="C81" s="109"/>
+      <c r="D81" s="109"/>
+      <c r="E81" s="109"/>
+      <c r="F81" s="109"/>
+      <c r="G81" s="109"/>
+      <c r="H81" s="109"/>
+      <c r="I81" s="109"/>
+      <c r="J81" s="109"/>
+      <c r="K81" s="109"/>
+      <c r="L81" s="109"/>
+      <c r="M81" s="109"/>
+      <c r="N81" s="109"/>
+      <c r="O81" s="109"/>
+      <c r="Q81" s="106" t="s">
         <v>202</v>
       </c>
-      <c r="R81" s="102"/>
-      <c r="S81" s="102"/>
-      <c r="T81" s="102"/>
-      <c r="U81" s="102"/>
-      <c r="V81" s="102"/>
-      <c r="W81" s="102"/>
-      <c r="X81" s="102"/>
-      <c r="Y81" s="102"/>
-      <c r="Z81" s="102"/>
-      <c r="AA81" s="102"/>
-      <c r="AB81" s="102"/>
-      <c r="AC81" s="102"/>
-      <c r="AD81" s="102"/>
+      <c r="R81" s="106"/>
+      <c r="S81" s="106"/>
+      <c r="T81" s="106"/>
+      <c r="U81" s="106"/>
+      <c r="V81" s="106"/>
+      <c r="W81" s="106"/>
+      <c r="X81" s="106"/>
+      <c r="Y81" s="106"/>
+      <c r="Z81" s="106"/>
+      <c r="AA81" s="106"/>
+      <c r="AB81" s="106"/>
+      <c r="AC81" s="106"/>
+      <c r="AD81" s="106"/>
     </row>
     <row r="82" spans="2:30">
-      <c r="B82" s="101"/>
-      <c r="C82" s="101"/>
-      <c r="D82" s="101"/>
-      <c r="E82" s="101"/>
-      <c r="F82" s="101"/>
-      <c r="G82" s="101"/>
-      <c r="H82" s="101"/>
-      <c r="I82" s="101"/>
-      <c r="J82" s="101"/>
-      <c r="K82" s="101"/>
-      <c r="L82" s="101"/>
-      <c r="M82" s="101"/>
-      <c r="N82" s="101"/>
-      <c r="O82" s="101"/>
-      <c r="Q82" s="102"/>
-      <c r="R82" s="102"/>
-      <c r="S82" s="102"/>
-      <c r="T82" s="102"/>
-      <c r="U82" s="102"/>
-      <c r="V82" s="102"/>
-      <c r="W82" s="102"/>
-      <c r="X82" s="102"/>
-      <c r="Y82" s="102"/>
-      <c r="Z82" s="102"/>
-      <c r="AA82" s="102"/>
-      <c r="AB82" s="102"/>
-      <c r="AC82" s="102"/>
-      <c r="AD82" s="102"/>
+      <c r="B82" s="109"/>
+      <c r="C82" s="109"/>
+      <c r="D82" s="109"/>
+      <c r="E82" s="109"/>
+      <c r="F82" s="109"/>
+      <c r="G82" s="109"/>
+      <c r="H82" s="109"/>
+      <c r="I82" s="109"/>
+      <c r="J82" s="109"/>
+      <c r="K82" s="109"/>
+      <c r="L82" s="109"/>
+      <c r="M82" s="109"/>
+      <c r="N82" s="109"/>
+      <c r="O82" s="109"/>
+      <c r="Q82" s="106"/>
+      <c r="R82" s="106"/>
+      <c r="S82" s="106"/>
+      <c r="T82" s="106"/>
+      <c r="U82" s="106"/>
+      <c r="V82" s="106"/>
+      <c r="W82" s="106"/>
+      <c r="X82" s="106"/>
+      <c r="Y82" s="106"/>
+      <c r="Z82" s="106"/>
+      <c r="AA82" s="106"/>
+      <c r="AB82" s="106"/>
+      <c r="AC82" s="106"/>
+      <c r="AD82" s="106"/>
     </row>
     <row r="83" spans="2:30">
-      <c r="Q83" s="102"/>
-      <c r="R83" s="102"/>
-      <c r="S83" s="102"/>
-      <c r="T83" s="102"/>
-      <c r="U83" s="102"/>
-      <c r="V83" s="102"/>
-      <c r="W83" s="102"/>
-      <c r="X83" s="102"/>
-      <c r="Y83" s="102"/>
-      <c r="Z83" s="102"/>
-      <c r="AA83" s="102"/>
-      <c r="AB83" s="102"/>
-      <c r="AC83" s="102"/>
-      <c r="AD83" s="102"/>
+      <c r="Q83" s="106"/>
+      <c r="R83" s="106"/>
+      <c r="S83" s="106"/>
+      <c r="T83" s="106"/>
+      <c r="U83" s="106"/>
+      <c r="V83" s="106"/>
+      <c r="W83" s="106"/>
+      <c r="X83" s="106"/>
+      <c r="Y83" s="106"/>
+      <c r="Z83" s="106"/>
+      <c r="AA83" s="106"/>
+      <c r="AB83" s="106"/>
+      <c r="AC83" s="106"/>
+      <c r="AD83" s="106"/>
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="B58:O58"/>
-    <mergeCell ref="B79:O79"/>
-    <mergeCell ref="Q58:AD58"/>
-    <mergeCell ref="B60:O61"/>
-    <mergeCell ref="V48:Z48"/>
-    <mergeCell ref="S50:AB50"/>
-    <mergeCell ref="Q67:AD69"/>
-    <mergeCell ref="B50:O51"/>
-    <mergeCell ref="S33:AB34"/>
-    <mergeCell ref="S37:AB38"/>
-    <mergeCell ref="S42:AB42"/>
-    <mergeCell ref="S45:AB46"/>
-    <mergeCell ref="B55:O56"/>
-    <mergeCell ref="B33:N34"/>
-    <mergeCell ref="B38:O39"/>
-    <mergeCell ref="B41:O41"/>
-    <mergeCell ref="B45:O46"/>
+    <mergeCell ref="B81:O82"/>
+    <mergeCell ref="Q62:AD63"/>
+    <mergeCell ref="B63:O66"/>
+    <mergeCell ref="B67:O68"/>
+    <mergeCell ref="Q73:AD77"/>
+    <mergeCell ref="Q81:AD83"/>
     <mergeCell ref="B2:O2"/>
     <mergeCell ref="B4:O5"/>
     <mergeCell ref="B8:O9"/>
@@ -4302,12 +4301,23 @@
     <mergeCell ref="V40:Z40"/>
     <mergeCell ref="S29:AB29"/>
     <mergeCell ref="S26:AB26"/>
-    <mergeCell ref="B81:O82"/>
-    <mergeCell ref="Q62:AD63"/>
-    <mergeCell ref="B63:O66"/>
-    <mergeCell ref="B67:O68"/>
-    <mergeCell ref="Q73:AD77"/>
-    <mergeCell ref="Q81:AD83"/>
+    <mergeCell ref="S33:AB34"/>
+    <mergeCell ref="S37:AB38"/>
+    <mergeCell ref="S42:AB42"/>
+    <mergeCell ref="S45:AB46"/>
+    <mergeCell ref="B55:O56"/>
+    <mergeCell ref="B33:N34"/>
+    <mergeCell ref="B38:O39"/>
+    <mergeCell ref="B41:O41"/>
+    <mergeCell ref="B45:O46"/>
+    <mergeCell ref="B58:O58"/>
+    <mergeCell ref="B79:O79"/>
+    <mergeCell ref="Q58:AD58"/>
+    <mergeCell ref="B60:O61"/>
+    <mergeCell ref="V48:Z48"/>
+    <mergeCell ref="S50:AB50"/>
+    <mergeCell ref="Q67:AD69"/>
+    <mergeCell ref="B50:O51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4333,10 +4343,10 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A4" s="119" t="s">
+      <c r="A4" s="101" t="s">
         <v>228</v>
       </c>
-      <c r="B4" s="119" t="s">
+      <c r="B4" s="101" t="s">
         <v>229</v>
       </c>
     </row>
@@ -72452,7 +72462,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -72481,7 +72491,7 @@
       <c r="E1" s="56" t="s">
         <v>156</v>
       </c>
-      <c r="G1" s="120" t="s">
+      <c r="G1" s="102" t="s">
         <v>230</v>
       </c>
     </row>
@@ -72503,7 +72513,9 @@
       <c r="E2" s="35">
         <v>1000</v>
       </c>
-      <c r="G2" s="121"/>
+      <c r="G2" s="41">
+        <v>2000</v>
+      </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="55">
@@ -72523,6 +72535,9 @@
       <c r="E3" s="35">
         <v>1000</v>
       </c>
+      <c r="G3" s="41">
+        <v>2000</v>
+      </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="55">
@@ -72542,6 +72557,9 @@
       <c r="E4" s="35">
         <v>500</v>
       </c>
+      <c r="G4" s="41">
+        <v>2000</v>
+      </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="55">
@@ -72561,6 +72579,9 @@
       <c r="E5" s="35">
         <v>500</v>
       </c>
+      <c r="G5" s="41">
+        <v>2000</v>
+      </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="55">
@@ -72580,6 +72601,9 @@
       <c r="E6" s="35">
         <v>500</v>
       </c>
+      <c r="G6" s="41">
+        <v>2000</v>
+      </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="55">
@@ -72599,6 +72623,9 @@
       <c r="E7" s="35">
         <v>10</v>
       </c>
+      <c r="G7" s="41">
+        <v>2000</v>
+      </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="55">
@@ -72618,6 +72645,9 @@
       <c r="E8" s="35">
         <v>10</v>
       </c>
+      <c r="G8" s="41">
+        <v>2000</v>
+      </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="55">
@@ -72637,6 +72667,9 @@
       <c r="E9" s="35">
         <v>10</v>
       </c>
+      <c r="G9" s="41">
+        <v>2000</v>
+      </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="55">
@@ -72656,6 +72689,9 @@
       <c r="E10" s="35">
         <v>10</v>
       </c>
+      <c r="G10" s="41">
+        <v>2000</v>
+      </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="55">
@@ -72675,6 +72711,9 @@
       <c r="E11" s="35">
         <v>10</v>
       </c>
+      <c r="G11" s="41">
+        <v>2000</v>
+      </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="55">
@@ -72694,6 +72733,9 @@
       <c r="E12" s="35">
         <v>10</v>
       </c>
+      <c r="G12" s="41">
+        <v>2000</v>
+      </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="55">
@@ -72713,6 +72755,9 @@
       <c r="E13" s="35">
         <v>10</v>
       </c>
+      <c r="G13" s="41">
+        <v>2000</v>
+      </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="55">
@@ -72732,6 +72777,9 @@
       <c r="E14" s="35">
         <v>10</v>
       </c>
+      <c r="G14" s="41">
+        <v>2000</v>
+      </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="55">
@@ -72751,6 +72799,9 @@
       <c r="E15" s="35">
         <v>10</v>
       </c>
+      <c r="G15" s="41">
+        <v>2000</v>
+      </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="55">
@@ -72770,8 +72821,11 @@
       <c r="E16" s="35">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="G16" s="41">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="55">
         <f>Regiones!A17</f>
         <v>16</v>
@@ -72789,8 +72843,11 @@
       <c r="E17" s="35">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="G17" s="41">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" s="55">
         <f>Regiones!A18</f>
         <v>17</v>
@@ -72808,8 +72865,11 @@
       <c r="E18" s="35">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="G18" s="41">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="55">
         <f>Regiones!A19</f>
         <v>18</v>
@@ -72827,8 +72887,11 @@
       <c r="E19" s="35">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="G19" s="41">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="55">
         <f>Regiones!A20</f>
         <v>19</v>
@@ -72846,8 +72909,11 @@
       <c r="E20" s="35">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="G20" s="41">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" s="55">
         <f>Regiones!A21</f>
         <v>20</v>
@@ -72865,8 +72931,11 @@
       <c r="E21" s="35">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="G21" s="41">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" s="55">
         <f>Regiones!A22</f>
         <v>21</v>
@@ -72884,8 +72953,11 @@
       <c r="E22" s="35">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="G22" s="41">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" s="55">
         <f>Regiones!A23</f>
         <v>22</v>
@@ -72903,8 +72975,11 @@
       <c r="E23" s="35">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="G23" s="41">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" s="55">
         <f>Regiones!A24</f>
         <v>23</v>
@@ -72922,8 +72997,11 @@
       <c r="E24" s="35">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="G24" s="41">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" s="55">
         <f>Regiones!A25</f>
         <v>24</v>
@@ -72941,8 +73019,11 @@
       <c r="E25" s="35">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="G25" s="41">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" s="55">
         <f>Regiones!A26</f>
         <v>25</v>
@@ -72959,6 +73040,9 @@
       </c>
       <c r="E26" s="35">
         <v>5</v>
+      </c>
+      <c r="G26" s="41">
+        <v>2000</v>
       </c>
     </row>
   </sheetData>
@@ -72972,10 +73056,10 @@
   <sheetPr>
     <tabColor theme="4" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -72984,9 +73068,10 @@
     <col min="2" max="2" width="31.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1">
       <c r="A1" s="34" t="s">
         <v>157</v>
       </c>
@@ -72996,11 +73081,11 @@
       <c r="C1" s="34" t="s">
         <v>168</v>
       </c>
-      <c r="E1" s="122" t="s">
+      <c r="E1" s="103" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" thickTop="1">
+    <row r="2" spans="1:9" ht="15.75" thickTop="1">
       <c r="A2" s="43">
         <f>Regiones!A2</f>
         <v>1</v>
@@ -73012,11 +73097,15 @@
       <c r="C2" s="35">
         <v>1</v>
       </c>
-      <c r="E2" s="123" t="s">
+      <c r="E2" s="124" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="125" t="str">
+        <f>_xlfn.CONCAT(F4+1,RIGHT(F3,7))</f>
+        <v>11/1/2020</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="43">
         <f>Regiones!A3</f>
         <v>2</v>
@@ -73028,8 +73117,12 @@
       <c r="C3" s="35">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" s="126" t="str">
+        <f>E2</f>
+        <v>10/1/2020</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="43">
         <f>Regiones!A4</f>
         <v>3</v>
@@ -73041,8 +73134,14 @@
       <c r="C4" s="35">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="E4" s="123"/>
+      <c r="F4" s="125" t="str">
+        <f>LEFT(F3,2)</f>
+        <v>10</v>
+      </c>
+      <c r="H4" s="122"/>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="43">
         <f>Regiones!A5</f>
         <v>4</v>
@@ -73054,8 +73153,9 @@
       <c r="C5" s="35">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="I5" s="123"/>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="43">
         <f>Regiones!A6</f>
         <v>5</v>
@@ -73067,8 +73167,9 @@
       <c r="C6" s="35">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="I6" s="123"/>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="43">
         <f>Regiones!A7</f>
         <v>6</v>
@@ -73081,7 +73182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:9">
       <c r="A8" s="43">
         <f>Regiones!A8</f>
         <v>7</v>
@@ -73094,7 +73195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:9">
       <c r="A9" s="43">
         <f>Regiones!A9</f>
         <v>8</v>
@@ -73107,7 +73208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:9">
       <c r="A10" s="43">
         <f>Regiones!A10</f>
         <v>9</v>
@@ -73119,8 +73220,9 @@
       <c r="C10" s="35">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="E10" s="122"/>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="43">
         <f>Regiones!A11</f>
         <v>10</v>
@@ -73133,7 +73235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:9">
       <c r="A12" s="43">
         <f>Regiones!A12</f>
         <v>11</v>
@@ -73146,7 +73248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:9">
       <c r="A13" s="43">
         <f>Regiones!A13</f>
         <v>12</v>
@@ -73159,7 +73261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:9">
       <c r="A14" s="43">
         <f>Regiones!A14</f>
         <v>13</v>
@@ -73172,7 +73274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:9">
       <c r="A15" s="43">
         <f>Regiones!A15</f>
         <v>14</v>
@@ -73185,7 +73287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:9">
       <c r="A16" s="43">
         <f>Regiones!A16</f>
         <v>15</v>
@@ -73329,6 +73431,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="32" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
adds better date for regional ventilators availability availability fixes simulation's start date bug
</commit_message>
<xml_diff>
--- a/COVID Simulator v 1.1/Input/Input_Simulador.xlsx
+++ b/COVID Simulator v 1.1/Input/Input_Simulador.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignacio.brottier\Documents\COVID 19\COVID-19-Simulation-Argentina\COVID Simulator v 1.1\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96884975-E76F-4A0F-B944-B6D9EE845F6D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D1A796-2D43-460C-B58F-CF124B395C9B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="5" activeTab="8" xr2:uid="{55AC4C4C-7526-4060-9BB2-10E89010456B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="5" activeTab="7" xr2:uid="{55AC4C4C-7526-4060-9BB2-10E89010456B}"/>
   </bookViews>
   <sheets>
     <sheet name="Información" sheetId="28" r:id="rId1"/>
@@ -1646,7 +1646,7 @@
     <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="167" formatCode="0.0000"/>
     <numFmt numFmtId="168" formatCode="0.000"/>
-    <numFmt numFmtId="171" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="169" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
   <fonts count="33">
     <font>
@@ -1872,7 +1872,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1925,6 +1925,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB4C6E7"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -2078,7 +2084,7 @@
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2319,32 +2325,16 @@
     <xf numFmtId="1" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2355,10 +2345,16 @@
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2370,14 +2366,30 @@
     <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Comma" xfId="7" builtinId="3"/>
@@ -2830,22 +2842,22 @@
   <sheetData>
     <row r="1" spans="2:45" s="9" customFormat="1"/>
     <row r="2" spans="2:45" s="9" customFormat="1" ht="33.75" customHeight="1" thickBot="1">
-      <c r="B2" s="113" t="s">
+      <c r="B2" s="111" t="s">
         <v>105</v>
       </c>
-      <c r="C2" s="113"/>
-      <c r="D2" s="113"/>
-      <c r="E2" s="113"/>
-      <c r="F2" s="113"/>
-      <c r="G2" s="113"/>
-      <c r="H2" s="113"/>
-      <c r="I2" s="113"/>
-      <c r="J2" s="113"/>
-      <c r="K2" s="113"/>
-      <c r="L2" s="113"/>
-      <c r="M2" s="113"/>
-      <c r="N2" s="113"/>
-      <c r="O2" s="113"/>
+      <c r="C2" s="111"/>
+      <c r="D2" s="111"/>
+      <c r="E2" s="111"/>
+      <c r="F2" s="111"/>
+      <c r="G2" s="111"/>
+      <c r="H2" s="111"/>
+      <c r="I2" s="111"/>
+      <c r="J2" s="111"/>
+      <c r="K2" s="111"/>
+      <c r="L2" s="111"/>
+      <c r="M2" s="111"/>
+      <c r="N2" s="111"/>
+      <c r="O2" s="111"/>
       <c r="Q2" s="57"/>
       <c r="R2" s="57"/>
       <c r="S2" s="57"/>
@@ -2895,59 +2907,59 @@
       <c r="M5" s="109"/>
       <c r="N5" s="109"/>
       <c r="O5" s="109"/>
-      <c r="Q5" s="117" t="s">
+      <c r="Q5" s="116" t="s">
         <v>173</v>
       </c>
-      <c r="R5" s="117"/>
-      <c r="S5" s="117"/>
-      <c r="T5" s="117"/>
-      <c r="U5" s="117"/>
-      <c r="V5" s="117"/>
-      <c r="W5" s="117"/>
-      <c r="X5" s="117"/>
-      <c r="Y5" s="117"/>
-      <c r="Z5" s="117"/>
-      <c r="AA5" s="117"/>
-      <c r="AB5" s="117"/>
-      <c r="AC5" s="117"/>
-      <c r="AD5" s="117"/>
+      <c r="R5" s="116"/>
+      <c r="S5" s="116"/>
+      <c r="T5" s="116"/>
+      <c r="U5" s="116"/>
+      <c r="V5" s="116"/>
+      <c r="W5" s="116"/>
+      <c r="X5" s="116"/>
+      <c r="Y5" s="116"/>
+      <c r="Z5" s="116"/>
+      <c r="AA5" s="116"/>
+      <c r="AB5" s="116"/>
+      <c r="AC5" s="116"/>
+      <c r="AD5" s="116"/>
       <c r="AQ5" s="9"/>
       <c r="AR5" s="9"/>
       <c r="AS5" s="9"/>
     </row>
     <row r="6" spans="2:45">
-      <c r="Q6" s="116" t="s">
+      <c r="Q6" s="115" t="s">
         <v>174</v>
       </c>
-      <c r="R6" s="116"/>
-      <c r="S6" s="116"/>
-      <c r="T6" s="116"/>
-      <c r="U6" s="116"/>
-      <c r="V6" s="116"/>
-      <c r="W6" s="116"/>
-      <c r="X6" s="116"/>
-      <c r="Y6" s="116"/>
-      <c r="Z6" s="116"/>
-      <c r="AA6" s="116"/>
-      <c r="AB6" s="116"/>
-      <c r="AC6" s="116"/>
-      <c r="AD6" s="116"/>
+      <c r="R6" s="115"/>
+      <c r="S6" s="115"/>
+      <c r="T6" s="115"/>
+      <c r="U6" s="115"/>
+      <c r="V6" s="115"/>
+      <c r="W6" s="115"/>
+      <c r="X6" s="115"/>
+      <c r="Y6" s="115"/>
+      <c r="Z6" s="115"/>
+      <c r="AA6" s="115"/>
+      <c r="AB6" s="115"/>
+      <c r="AC6" s="115"/>
+      <c r="AD6" s="115"/>
     </row>
     <row r="7" spans="2:45">
-      <c r="Q7" s="116"/>
-      <c r="R7" s="116"/>
-      <c r="S7" s="116"/>
-      <c r="T7" s="116"/>
-      <c r="U7" s="116"/>
-      <c r="V7" s="116"/>
-      <c r="W7" s="116"/>
-      <c r="X7" s="116"/>
-      <c r="Y7" s="116"/>
-      <c r="Z7" s="116"/>
-      <c r="AA7" s="116"/>
-      <c r="AB7" s="116"/>
-      <c r="AC7" s="116"/>
-      <c r="AD7" s="116"/>
+      <c r="Q7" s="115"/>
+      <c r="R7" s="115"/>
+      <c r="S7" s="115"/>
+      <c r="T7" s="115"/>
+      <c r="U7" s="115"/>
+      <c r="V7" s="115"/>
+      <c r="W7" s="115"/>
+      <c r="X7" s="115"/>
+      <c r="Y7" s="115"/>
+      <c r="Z7" s="115"/>
+      <c r="AA7" s="115"/>
+      <c r="AB7" s="115"/>
+      <c r="AC7" s="115"/>
+      <c r="AD7" s="115"/>
     </row>
     <row r="8" spans="2:45" ht="15" customHeight="1">
       <c r="B8" s="109" t="s">
@@ -2966,20 +2978,20 @@
       <c r="M8" s="109"/>
       <c r="N8" s="109"/>
       <c r="O8" s="109"/>
-      <c r="Q8" s="116"/>
-      <c r="R8" s="116"/>
-      <c r="S8" s="116"/>
-      <c r="T8" s="116"/>
-      <c r="U8" s="116"/>
-      <c r="V8" s="116"/>
-      <c r="W8" s="116"/>
-      <c r="X8" s="116"/>
-      <c r="Y8" s="116"/>
-      <c r="Z8" s="116"/>
-      <c r="AA8" s="116"/>
-      <c r="AB8" s="116"/>
-      <c r="AC8" s="116"/>
-      <c r="AD8" s="116"/>
+      <c r="Q8" s="115"/>
+      <c r="R8" s="115"/>
+      <c r="S8" s="115"/>
+      <c r="T8" s="115"/>
+      <c r="U8" s="115"/>
+      <c r="V8" s="115"/>
+      <c r="W8" s="115"/>
+      <c r="X8" s="115"/>
+      <c r="Y8" s="115"/>
+      <c r="Z8" s="115"/>
+      <c r="AA8" s="115"/>
+      <c r="AB8" s="115"/>
+      <c r="AC8" s="115"/>
+      <c r="AD8" s="115"/>
     </row>
     <row r="9" spans="2:45" ht="17.25" customHeight="1">
       <c r="B9" s="109"/>
@@ -3002,72 +3014,72 @@
         <v>96</v>
       </c>
       <c r="H12" s="17"/>
-      <c r="I12" s="114" t="s">
+      <c r="I12" s="112" t="s">
         <v>100</v>
       </c>
-      <c r="J12" s="115"/>
-      <c r="K12" s="115"/>
-      <c r="L12" s="115"/>
-      <c r="M12" s="115"/>
+      <c r="J12" s="113"/>
+      <c r="K12" s="113"/>
+      <c r="L12" s="113"/>
+      <c r="M12" s="113"/>
     </row>
     <row r="13" spans="2:45" ht="17.25">
       <c r="D13" s="11" t="s">
         <v>104</v>
       </c>
       <c r="H13" s="17"/>
-      <c r="I13" s="114"/>
-      <c r="J13" s="115"/>
-      <c r="K13" s="115"/>
-      <c r="L13" s="115"/>
-      <c r="M13" s="115"/>
+      <c r="I13" s="112"/>
+      <c r="J13" s="113"/>
+      <c r="K13" s="113"/>
+      <c r="L13" s="113"/>
+      <c r="M13" s="113"/>
     </row>
     <row r="14" spans="2:45" ht="17.25">
       <c r="D14" s="13" t="s">
         <v>97</v>
       </c>
       <c r="H14" s="17"/>
-      <c r="I14" s="114"/>
-      <c r="J14" s="115"/>
-      <c r="K14" s="115"/>
-      <c r="L14" s="115"/>
-      <c r="M14" s="115"/>
+      <c r="I14" s="112"/>
+      <c r="J14" s="113"/>
+      <c r="K14" s="113"/>
+      <c r="L14" s="113"/>
+      <c r="M14" s="113"/>
     </row>
     <row r="15" spans="2:45" ht="17.25" customHeight="1">
       <c r="D15" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="I15" s="114"/>
-      <c r="J15" s="115"/>
-      <c r="K15" s="115"/>
-      <c r="L15" s="115"/>
-      <c r="M15" s="115"/>
+      <c r="I15" s="112"/>
+      <c r="J15" s="113"/>
+      <c r="K15" s="113"/>
+      <c r="L15" s="113"/>
+      <c r="M15" s="113"/>
     </row>
     <row r="17" spans="2:43" ht="17.25" customHeight="1">
       <c r="G17" s="18"/>
-      <c r="I17" s="114" t="s">
+      <c r="I17" s="112" t="s">
         <v>102</v>
       </c>
-      <c r="J17" s="115"/>
-      <c r="K17" s="115"/>
-      <c r="L17" s="115"/>
-      <c r="M17" s="115"/>
+      <c r="J17" s="113"/>
+      <c r="K17" s="113"/>
+      <c r="L17" s="113"/>
+      <c r="M17" s="113"/>
     </row>
     <row r="18" spans="2:43" ht="17.25">
       <c r="D18" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="I18" s="114"/>
-      <c r="J18" s="115"/>
-      <c r="K18" s="115"/>
-      <c r="L18" s="115"/>
-      <c r="M18" s="115"/>
+      <c r="I18" s="112"/>
+      <c r="J18" s="113"/>
+      <c r="K18" s="113"/>
+      <c r="L18" s="113"/>
+      <c r="M18" s="113"/>
     </row>
     <row r="19" spans="2:43" ht="15" customHeight="1">
-      <c r="I19" s="114"/>
-      <c r="J19" s="115"/>
-      <c r="K19" s="115"/>
-      <c r="L19" s="115"/>
-      <c r="M19" s="115"/>
+      <c r="I19" s="112"/>
+      <c r="J19" s="113"/>
+      <c r="K19" s="113"/>
+      <c r="L19" s="113"/>
+      <c r="M19" s="113"/>
     </row>
     <row r="22" spans="2:43">
       <c r="B22" s="118" t="s">
@@ -3089,22 +3101,22 @@
     </row>
     <row r="23" spans="2:43" ht="15" customHeight="1"/>
     <row r="24" spans="2:43" ht="17.25">
-      <c r="B24" s="104" t="s">
+      <c r="B24" s="117" t="s">
         <v>96</v>
       </c>
-      <c r="C24" s="104"/>
-      <c r="D24" s="104"/>
-      <c r="E24" s="104"/>
-      <c r="F24" s="104"/>
-      <c r="G24" s="104"/>
-      <c r="H24" s="104"/>
-      <c r="I24" s="104"/>
-      <c r="J24" s="104"/>
-      <c r="K24" s="104"/>
-      <c r="L24" s="104"/>
-      <c r="M24" s="104"/>
-      <c r="N24" s="104"/>
-      <c r="O24" s="104"/>
+      <c r="C24" s="117"/>
+      <c r="D24" s="117"/>
+      <c r="E24" s="117"/>
+      <c r="F24" s="117"/>
+      <c r="G24" s="117"/>
+      <c r="H24" s="117"/>
+      <c r="I24" s="117"/>
+      <c r="J24" s="117"/>
+      <c r="K24" s="117"/>
+      <c r="L24" s="117"/>
+      <c r="M24" s="117"/>
+      <c r="N24" s="117"/>
+      <c r="O24" s="117"/>
     </row>
     <row r="25" spans="2:43">
       <c r="R25" s="23"/>
@@ -3125,18 +3137,18 @@
         <v>96</v>
       </c>
       <c r="R26" s="26"/>
-      <c r="S26" s="121" t="s">
+      <c r="S26" s="122" t="s">
         <v>106</v>
       </c>
-      <c r="T26" s="121"/>
-      <c r="U26" s="121"/>
-      <c r="V26" s="121"/>
-      <c r="W26" s="121"/>
-      <c r="X26" s="121"/>
-      <c r="Y26" s="121"/>
-      <c r="Z26" s="121"/>
-      <c r="AA26" s="121"/>
-      <c r="AB26" s="121"/>
+      <c r="T26" s="122"/>
+      <c r="U26" s="122"/>
+      <c r="V26" s="122"/>
+      <c r="W26" s="122"/>
+      <c r="X26" s="122"/>
+      <c r="Y26" s="122"/>
+      <c r="Z26" s="122"/>
+      <c r="AA26" s="122"/>
+      <c r="AB26" s="122"/>
       <c r="AC26" s="27"/>
     </row>
     <row r="27" spans="2:43" ht="15" customHeight="1">
@@ -3213,18 +3225,18 @@
       <c r="N29" s="109"/>
       <c r="O29" s="109"/>
       <c r="R29" s="26"/>
-      <c r="S29" s="112" t="s">
+      <c r="S29" s="121" t="s">
         <v>107</v>
       </c>
-      <c r="T29" s="112"/>
-      <c r="U29" s="112"/>
-      <c r="V29" s="112"/>
-      <c r="W29" s="112"/>
-      <c r="X29" s="112"/>
-      <c r="Y29" s="112"/>
-      <c r="Z29" s="112"/>
-      <c r="AA29" s="112"/>
-      <c r="AB29" s="112"/>
+      <c r="T29" s="121"/>
+      <c r="U29" s="121"/>
+      <c r="V29" s="121"/>
+      <c r="W29" s="121"/>
+      <c r="X29" s="121"/>
+      <c r="Y29" s="121"/>
+      <c r="Z29" s="121"/>
+      <c r="AA29" s="121"/>
+      <c r="AB29" s="121"/>
       <c r="AC29" s="27"/>
     </row>
     <row r="30" spans="2:43">
@@ -3318,18 +3330,18 @@
       <c r="M33" s="109"/>
       <c r="N33" s="109"/>
       <c r="R33" s="26"/>
-      <c r="S33" s="110" t="s">
+      <c r="S33" s="123" t="s">
         <v>108</v>
       </c>
-      <c r="T33" s="110"/>
-      <c r="U33" s="110"/>
-      <c r="V33" s="110"/>
-      <c r="W33" s="110"/>
-      <c r="X33" s="110"/>
-      <c r="Y33" s="110"/>
-      <c r="Z33" s="110"/>
-      <c r="AA33" s="110"/>
-      <c r="AB33" s="110"/>
+      <c r="T33" s="123"/>
+      <c r="U33" s="123"/>
+      <c r="V33" s="123"/>
+      <c r="W33" s="123"/>
+      <c r="X33" s="123"/>
+      <c r="Y33" s="123"/>
+      <c r="Z33" s="123"/>
+      <c r="AA33" s="123"/>
+      <c r="AB33" s="123"/>
       <c r="AC33" s="27"/>
     </row>
     <row r="34" spans="2:32" ht="17.25" customHeight="1">
@@ -3347,16 +3359,16 @@
       <c r="M34" s="109"/>
       <c r="N34" s="109"/>
       <c r="R34" s="26"/>
-      <c r="S34" s="110"/>
-      <c r="T34" s="110"/>
-      <c r="U34" s="110"/>
-      <c r="V34" s="110"/>
-      <c r="W34" s="110"/>
-      <c r="X34" s="110"/>
-      <c r="Y34" s="110"/>
-      <c r="Z34" s="110"/>
-      <c r="AA34" s="110"/>
-      <c r="AB34" s="110"/>
+      <c r="S34" s="123"/>
+      <c r="T34" s="123"/>
+      <c r="U34" s="123"/>
+      <c r="V34" s="123"/>
+      <c r="W34" s="123"/>
+      <c r="X34" s="123"/>
+      <c r="Y34" s="123"/>
+      <c r="Z34" s="123"/>
+      <c r="AA34" s="123"/>
+      <c r="AB34" s="123"/>
       <c r="AC34" s="27"/>
     </row>
     <row r="35" spans="2:32">
@@ -3394,18 +3406,18 @@
     </row>
     <row r="37" spans="2:32">
       <c r="R37" s="26"/>
-      <c r="S37" s="111" t="s">
+      <c r="S37" s="124" t="s">
         <v>111</v>
       </c>
-      <c r="T37" s="111"/>
-      <c r="U37" s="111"/>
-      <c r="V37" s="111"/>
-      <c r="W37" s="111"/>
-      <c r="X37" s="111"/>
-      <c r="Y37" s="111"/>
-      <c r="Z37" s="111"/>
-      <c r="AA37" s="111"/>
-      <c r="AB37" s="111"/>
+      <c r="T37" s="124"/>
+      <c r="U37" s="124"/>
+      <c r="V37" s="124"/>
+      <c r="W37" s="124"/>
+      <c r="X37" s="124"/>
+      <c r="Y37" s="124"/>
+      <c r="Z37" s="124"/>
+      <c r="AA37" s="124"/>
+      <c r="AB37" s="124"/>
       <c r="AC37" s="27"/>
       <c r="AF37" s="9"/>
     </row>
@@ -3427,16 +3439,16 @@
       <c r="N38" s="109"/>
       <c r="O38" s="109"/>
       <c r="R38" s="26"/>
-      <c r="S38" s="111"/>
-      <c r="T38" s="111"/>
-      <c r="U38" s="111"/>
-      <c r="V38" s="111"/>
-      <c r="W38" s="111"/>
-      <c r="X38" s="111"/>
-      <c r="Y38" s="111"/>
-      <c r="Z38" s="111"/>
-      <c r="AA38" s="111"/>
-      <c r="AB38" s="111"/>
+      <c r="S38" s="124"/>
+      <c r="T38" s="124"/>
+      <c r="U38" s="124"/>
+      <c r="V38" s="124"/>
+      <c r="W38" s="124"/>
+      <c r="X38" s="124"/>
+      <c r="Y38" s="124"/>
+      <c r="Z38" s="124"/>
+      <c r="AA38" s="124"/>
+      <c r="AB38" s="124"/>
       <c r="AC38" s="27"/>
       <c r="AF38" s="9"/>
     </row>
@@ -3486,22 +3498,22 @@
       <c r="AC40" s="27"/>
     </row>
     <row r="41" spans="2:32" ht="17.25">
-      <c r="B41" s="104" t="s">
+      <c r="B41" s="117" t="s">
         <v>104</v>
       </c>
-      <c r="C41" s="104"/>
-      <c r="D41" s="104"/>
-      <c r="E41" s="104"/>
-      <c r="F41" s="104"/>
-      <c r="G41" s="104"/>
-      <c r="H41" s="104"/>
-      <c r="I41" s="104"/>
-      <c r="J41" s="104"/>
-      <c r="K41" s="104"/>
-      <c r="L41" s="104"/>
-      <c r="M41" s="104"/>
-      <c r="N41" s="104"/>
-      <c r="O41" s="104"/>
+      <c r="C41" s="117"/>
+      <c r="D41" s="117"/>
+      <c r="E41" s="117"/>
+      <c r="F41" s="117"/>
+      <c r="G41" s="117"/>
+      <c r="H41" s="117"/>
+      <c r="I41" s="117"/>
+      <c r="J41" s="117"/>
+      <c r="K41" s="117"/>
+      <c r="L41" s="117"/>
+      <c r="M41" s="117"/>
+      <c r="N41" s="117"/>
+      <c r="O41" s="117"/>
       <c r="R41" s="26"/>
       <c r="S41" s="18"/>
       <c r="T41" s="18"/>
@@ -3517,18 +3529,18 @@
     </row>
     <row r="42" spans="2:32" ht="17.25">
       <c r="R42" s="26"/>
-      <c r="S42" s="112" t="s">
+      <c r="S42" s="121" t="s">
         <v>112</v>
       </c>
-      <c r="T42" s="112"/>
-      <c r="U42" s="112"/>
-      <c r="V42" s="112"/>
-      <c r="W42" s="112"/>
-      <c r="X42" s="112"/>
-      <c r="Y42" s="112"/>
-      <c r="Z42" s="112"/>
-      <c r="AA42" s="112"/>
-      <c r="AB42" s="112"/>
+      <c r="T42" s="121"/>
+      <c r="U42" s="121"/>
+      <c r="V42" s="121"/>
+      <c r="W42" s="121"/>
+      <c r="X42" s="121"/>
+      <c r="Y42" s="121"/>
+      <c r="Z42" s="121"/>
+      <c r="AA42" s="121"/>
+      <c r="AB42" s="121"/>
       <c r="AC42" s="27"/>
     </row>
     <row r="43" spans="2:32" ht="17.25">
@@ -3580,18 +3592,18 @@
       <c r="N45" s="109"/>
       <c r="O45" s="109"/>
       <c r="R45" s="26"/>
-      <c r="S45" s="110" t="s">
+      <c r="S45" s="123" t="s">
         <v>113</v>
       </c>
-      <c r="T45" s="110"/>
-      <c r="U45" s="110"/>
-      <c r="V45" s="110"/>
-      <c r="W45" s="110"/>
-      <c r="X45" s="110"/>
-      <c r="Y45" s="110"/>
-      <c r="Z45" s="110"/>
-      <c r="AA45" s="110"/>
-      <c r="AB45" s="110"/>
+      <c r="T45" s="123"/>
+      <c r="U45" s="123"/>
+      <c r="V45" s="123"/>
+      <c r="W45" s="123"/>
+      <c r="X45" s="123"/>
+      <c r="Y45" s="123"/>
+      <c r="Z45" s="123"/>
+      <c r="AA45" s="123"/>
+      <c r="AB45" s="123"/>
       <c r="AC45" s="27"/>
     </row>
     <row r="46" spans="2:32" ht="15" customHeight="1">
@@ -3610,16 +3622,16 @@
       <c r="N46" s="109"/>
       <c r="O46" s="109"/>
       <c r="R46" s="26"/>
-      <c r="S46" s="110"/>
-      <c r="T46" s="110"/>
-      <c r="U46" s="110"/>
-      <c r="V46" s="110"/>
-      <c r="W46" s="110"/>
-      <c r="X46" s="110"/>
-      <c r="Y46" s="110"/>
-      <c r="Z46" s="110"/>
-      <c r="AA46" s="110"/>
-      <c r="AB46" s="110"/>
+      <c r="S46" s="123"/>
+      <c r="T46" s="123"/>
+      <c r="U46" s="123"/>
+      <c r="V46" s="123"/>
+      <c r="W46" s="123"/>
+      <c r="X46" s="123"/>
+      <c r="Y46" s="123"/>
+      <c r="Z46" s="123"/>
+      <c r="AA46" s="123"/>
+      <c r="AB46" s="123"/>
       <c r="AC46" s="27"/>
     </row>
     <row r="47" spans="2:32" ht="15" customHeight="1">
@@ -3644,13 +3656,13 @@
       <c r="S48" s="18"/>
       <c r="T48" s="18"/>
       <c r="U48" s="18"/>
-      <c r="V48" s="107" t="s">
+      <c r="V48" s="126" t="s">
         <v>114</v>
       </c>
-      <c r="W48" s="107"/>
-      <c r="X48" s="107"/>
-      <c r="Y48" s="107"/>
-      <c r="Z48" s="107"/>
+      <c r="W48" s="126"/>
+      <c r="X48" s="126"/>
+      <c r="Y48" s="126"/>
+      <c r="Z48" s="126"/>
       <c r="AA48" s="18"/>
       <c r="AB48" s="18"/>
       <c r="AC48" s="27"/>
@@ -3687,18 +3699,18 @@
       <c r="N50" s="109"/>
       <c r="O50" s="109"/>
       <c r="R50" s="26"/>
-      <c r="S50" s="108" t="s">
+      <c r="S50" s="114" t="s">
         <v>115</v>
       </c>
-      <c r="T50" s="108"/>
-      <c r="U50" s="108"/>
-      <c r="V50" s="108"/>
-      <c r="W50" s="108"/>
-      <c r="X50" s="108"/>
-      <c r="Y50" s="108"/>
-      <c r="Z50" s="108"/>
-      <c r="AA50" s="108"/>
-      <c r="AB50" s="108"/>
+      <c r="T50" s="114"/>
+      <c r="U50" s="114"/>
+      <c r="V50" s="114"/>
+      <c r="W50" s="114"/>
+      <c r="X50" s="114"/>
+      <c r="Y50" s="114"/>
+      <c r="Z50" s="114"/>
+      <c r="AA50" s="114"/>
+      <c r="AB50" s="114"/>
       <c r="AC50" s="27"/>
     </row>
     <row r="51" spans="2:43" ht="15" customHeight="1">
@@ -3731,18 +3743,18 @@
     </row>
     <row r="52" spans="2:43">
       <c r="R52" s="26"/>
-      <c r="S52" s="108" t="s">
+      <c r="S52" s="114" t="s">
         <v>116</v>
       </c>
-      <c r="T52" s="108"/>
-      <c r="U52" s="108"/>
-      <c r="V52" s="108"/>
-      <c r="W52" s="108"/>
-      <c r="X52" s="108"/>
-      <c r="Y52" s="108"/>
-      <c r="Z52" s="108"/>
-      <c r="AA52" s="108"/>
-      <c r="AB52" s="108"/>
+      <c r="T52" s="114"/>
+      <c r="U52" s="114"/>
+      <c r="V52" s="114"/>
+      <c r="W52" s="114"/>
+      <c r="X52" s="114"/>
+      <c r="Y52" s="114"/>
+      <c r="Z52" s="114"/>
+      <c r="AA52" s="114"/>
+      <c r="AB52" s="114"/>
       <c r="AC52" s="27"/>
     </row>
     <row r="53" spans="2:43" ht="15.75" customHeight="1">
@@ -3750,16 +3762,16 @@
         <v>147</v>
       </c>
       <c r="R53" s="26"/>
-      <c r="S53" s="108"/>
-      <c r="T53" s="108"/>
-      <c r="U53" s="108"/>
-      <c r="V53" s="108"/>
-      <c r="W53" s="108"/>
-      <c r="X53" s="108"/>
-      <c r="Y53" s="108"/>
-      <c r="Z53" s="108"/>
-      <c r="AA53" s="108"/>
-      <c r="AB53" s="108"/>
+      <c r="S53" s="114"/>
+      <c r="T53" s="114"/>
+      <c r="U53" s="114"/>
+      <c r="V53" s="114"/>
+      <c r="W53" s="114"/>
+      <c r="X53" s="114"/>
+      <c r="Y53" s="114"/>
+      <c r="Z53" s="114"/>
+      <c r="AA53" s="114"/>
+      <c r="AB53" s="114"/>
       <c r="AC53" s="27"/>
       <c r="AH53" s="22"/>
       <c r="AI53" s="22"/>
@@ -3833,75 +3845,75 @@
       <c r="O56" s="109"/>
     </row>
     <row r="58" spans="2:43" ht="17.25">
-      <c r="B58" s="104" t="s">
+      <c r="B58" s="117" t="s">
         <v>97</v>
       </c>
-      <c r="C58" s="104"/>
-      <c r="D58" s="104"/>
-      <c r="E58" s="104"/>
-      <c r="F58" s="104"/>
-      <c r="G58" s="104"/>
-      <c r="H58" s="104"/>
-      <c r="I58" s="104"/>
-      <c r="J58" s="104"/>
-      <c r="K58" s="104"/>
-      <c r="L58" s="104"/>
-      <c r="M58" s="104"/>
-      <c r="N58" s="104"/>
-      <c r="O58" s="104"/>
-      <c r="Q58" s="105" t="s">
+      <c r="C58" s="117"/>
+      <c r="D58" s="117"/>
+      <c r="E58" s="117"/>
+      <c r="F58" s="117"/>
+      <c r="G58" s="117"/>
+      <c r="H58" s="117"/>
+      <c r="I58" s="117"/>
+      <c r="J58" s="117"/>
+      <c r="K58" s="117"/>
+      <c r="L58" s="117"/>
+      <c r="M58" s="117"/>
+      <c r="N58" s="117"/>
+      <c r="O58" s="117"/>
+      <c r="Q58" s="125" t="s">
         <v>169</v>
       </c>
-      <c r="R58" s="105"/>
-      <c r="S58" s="105"/>
-      <c r="T58" s="105"/>
-      <c r="U58" s="105"/>
-      <c r="V58" s="105"/>
-      <c r="W58" s="105"/>
-      <c r="X58" s="105"/>
-      <c r="Y58" s="105"/>
-      <c r="Z58" s="105"/>
-      <c r="AA58" s="105"/>
-      <c r="AB58" s="105"/>
-      <c r="AC58" s="105"/>
-      <c r="AD58" s="105"/>
+      <c r="R58" s="125"/>
+      <c r="S58" s="125"/>
+      <c r="T58" s="125"/>
+      <c r="U58" s="125"/>
+      <c r="V58" s="125"/>
+      <c r="W58" s="125"/>
+      <c r="X58" s="125"/>
+      <c r="Y58" s="125"/>
+      <c r="Z58" s="125"/>
+      <c r="AA58" s="125"/>
+      <c r="AB58" s="125"/>
+      <c r="AC58" s="125"/>
+      <c r="AD58" s="125"/>
     </row>
     <row r="60" spans="2:43" ht="17.25">
-      <c r="B60" s="106" t="s">
+      <c r="B60" s="110" t="s">
         <v>198</v>
       </c>
-      <c r="C60" s="106"/>
-      <c r="D60" s="106"/>
-      <c r="E60" s="106"/>
-      <c r="F60" s="106"/>
-      <c r="G60" s="106"/>
-      <c r="H60" s="106"/>
-      <c r="I60" s="106"/>
-      <c r="J60" s="106"/>
-      <c r="K60" s="106"/>
-      <c r="L60" s="106"/>
-      <c r="M60" s="106"/>
-      <c r="N60" s="106"/>
-      <c r="O60" s="106"/>
+      <c r="C60" s="110"/>
+      <c r="D60" s="110"/>
+      <c r="E60" s="110"/>
+      <c r="F60" s="110"/>
+      <c r="G60" s="110"/>
+      <c r="H60" s="110"/>
+      <c r="I60" s="110"/>
+      <c r="J60" s="110"/>
+      <c r="K60" s="110"/>
+      <c r="L60" s="110"/>
+      <c r="M60" s="110"/>
+      <c r="N60" s="110"/>
+      <c r="O60" s="110"/>
       <c r="Q60" s="20" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="61" spans="2:43">
-      <c r="B61" s="106"/>
-      <c r="C61" s="106"/>
-      <c r="D61" s="106"/>
-      <c r="E61" s="106"/>
-      <c r="F61" s="106"/>
-      <c r="G61" s="106"/>
-      <c r="H61" s="106"/>
-      <c r="I61" s="106"/>
-      <c r="J61" s="106"/>
-      <c r="K61" s="106"/>
-      <c r="L61" s="106"/>
-      <c r="M61" s="106"/>
-      <c r="N61" s="106"/>
-      <c r="O61" s="106"/>
+      <c r="B61" s="110"/>
+      <c r="C61" s="110"/>
+      <c r="D61" s="110"/>
+      <c r="E61" s="110"/>
+      <c r="F61" s="110"/>
+      <c r="G61" s="110"/>
+      <c r="H61" s="110"/>
+      <c r="I61" s="110"/>
+      <c r="J61" s="110"/>
+      <c r="K61" s="110"/>
+      <c r="L61" s="110"/>
+      <c r="M61" s="110"/>
+      <c r="N61" s="110"/>
+      <c r="O61" s="110"/>
     </row>
     <row r="62" spans="2:43">
       <c r="Q62" s="109" t="s">
@@ -3922,22 +3934,22 @@
       <c r="AD62" s="109"/>
     </row>
     <row r="63" spans="2:43" ht="15" customHeight="1">
-      <c r="B63" s="106" t="s">
+      <c r="B63" s="110" t="s">
         <v>213</v>
       </c>
-      <c r="C63" s="106"/>
-      <c r="D63" s="106"/>
-      <c r="E63" s="106"/>
-      <c r="F63" s="106"/>
-      <c r="G63" s="106"/>
-      <c r="H63" s="106"/>
-      <c r="I63" s="106"/>
-      <c r="J63" s="106"/>
-      <c r="K63" s="106"/>
-      <c r="L63" s="106"/>
-      <c r="M63" s="106"/>
-      <c r="N63" s="106"/>
-      <c r="O63" s="106"/>
+      <c r="C63" s="110"/>
+      <c r="D63" s="110"/>
+      <c r="E63" s="110"/>
+      <c r="F63" s="110"/>
+      <c r="G63" s="110"/>
+      <c r="H63" s="110"/>
+      <c r="I63" s="110"/>
+      <c r="J63" s="110"/>
+      <c r="K63" s="110"/>
+      <c r="L63" s="110"/>
+      <c r="M63" s="110"/>
+      <c r="N63" s="110"/>
+      <c r="O63" s="110"/>
       <c r="Q63" s="109"/>
       <c r="R63" s="109"/>
       <c r="S63" s="109"/>
@@ -3954,55 +3966,55 @@
       <c r="AD63" s="109"/>
     </row>
     <row r="64" spans="2:43">
-      <c r="B64" s="106"/>
-      <c r="C64" s="106"/>
-      <c r="D64" s="106"/>
-      <c r="E64" s="106"/>
-      <c r="F64" s="106"/>
-      <c r="G64" s="106"/>
-      <c r="H64" s="106"/>
-      <c r="I64" s="106"/>
-      <c r="J64" s="106"/>
-      <c r="K64" s="106"/>
-      <c r="L64" s="106"/>
-      <c r="M64" s="106"/>
-      <c r="N64" s="106"/>
-      <c r="O64" s="106"/>
+      <c r="B64" s="110"/>
+      <c r="C64" s="110"/>
+      <c r="D64" s="110"/>
+      <c r="E64" s="110"/>
+      <c r="F64" s="110"/>
+      <c r="G64" s="110"/>
+      <c r="H64" s="110"/>
+      <c r="I64" s="110"/>
+      <c r="J64" s="110"/>
+      <c r="K64" s="110"/>
+      <c r="L64" s="110"/>
+      <c r="M64" s="110"/>
+      <c r="N64" s="110"/>
+      <c r="O64" s="110"/>
     </row>
     <row r="65" spans="2:30" ht="17.25">
-      <c r="B65" s="106"/>
-      <c r="C65" s="106"/>
-      <c r="D65" s="106"/>
-      <c r="E65" s="106"/>
-      <c r="F65" s="106"/>
-      <c r="G65" s="106"/>
-      <c r="H65" s="106"/>
-      <c r="I65" s="106"/>
-      <c r="J65" s="106"/>
-      <c r="K65" s="106"/>
-      <c r="L65" s="106"/>
-      <c r="M65" s="106"/>
-      <c r="N65" s="106"/>
-      <c r="O65" s="106"/>
+      <c r="B65" s="110"/>
+      <c r="C65" s="110"/>
+      <c r="D65" s="110"/>
+      <c r="E65" s="110"/>
+      <c r="F65" s="110"/>
+      <c r="G65" s="110"/>
+      <c r="H65" s="110"/>
+      <c r="I65" s="110"/>
+      <c r="J65" s="110"/>
+      <c r="K65" s="110"/>
+      <c r="L65" s="110"/>
+      <c r="M65" s="110"/>
+      <c r="N65" s="110"/>
+      <c r="O65" s="110"/>
       <c r="Q65" s="20" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="66" spans="2:30">
-      <c r="B66" s="106"/>
-      <c r="C66" s="106"/>
-      <c r="D66" s="106"/>
-      <c r="E66" s="106"/>
-      <c r="F66" s="106"/>
-      <c r="G66" s="106"/>
-      <c r="H66" s="106"/>
-      <c r="I66" s="106"/>
-      <c r="J66" s="106"/>
-      <c r="K66" s="106"/>
-      <c r="L66" s="106"/>
-      <c r="M66" s="106"/>
-      <c r="N66" s="106"/>
-      <c r="O66" s="106"/>
+      <c r="B66" s="110"/>
+      <c r="C66" s="110"/>
+      <c r="D66" s="110"/>
+      <c r="E66" s="110"/>
+      <c r="F66" s="110"/>
+      <c r="G66" s="110"/>
+      <c r="H66" s="110"/>
+      <c r="I66" s="110"/>
+      <c r="J66" s="110"/>
+      <c r="K66" s="110"/>
+      <c r="L66" s="110"/>
+      <c r="M66" s="110"/>
+      <c r="N66" s="110"/>
+      <c r="O66" s="110"/>
     </row>
     <row r="67" spans="2:30" ht="15" customHeight="1">
       <c r="B67" s="109" t="s">
@@ -4095,104 +4107,104 @@
       </c>
     </row>
     <row r="73" spans="2:30">
-      <c r="Q73" s="106" t="s">
+      <c r="Q73" s="110" t="s">
         <v>203</v>
       </c>
-      <c r="R73" s="106"/>
-      <c r="S73" s="106"/>
-      <c r="T73" s="106"/>
-      <c r="U73" s="106"/>
-      <c r="V73" s="106"/>
-      <c r="W73" s="106"/>
-      <c r="X73" s="106"/>
-      <c r="Y73" s="106"/>
-      <c r="Z73" s="106"/>
-      <c r="AA73" s="106"/>
-      <c r="AB73" s="106"/>
-      <c r="AC73" s="106"/>
-      <c r="AD73" s="106"/>
+      <c r="R73" s="110"/>
+      <c r="S73" s="110"/>
+      <c r="T73" s="110"/>
+      <c r="U73" s="110"/>
+      <c r="V73" s="110"/>
+      <c r="W73" s="110"/>
+      <c r="X73" s="110"/>
+      <c r="Y73" s="110"/>
+      <c r="Z73" s="110"/>
+      <c r="AA73" s="110"/>
+      <c r="AB73" s="110"/>
+      <c r="AC73" s="110"/>
+      <c r="AD73" s="110"/>
     </row>
     <row r="74" spans="2:30">
-      <c r="Q74" s="106"/>
-      <c r="R74" s="106"/>
-      <c r="S74" s="106"/>
-      <c r="T74" s="106"/>
-      <c r="U74" s="106"/>
-      <c r="V74" s="106"/>
-      <c r="W74" s="106"/>
-      <c r="X74" s="106"/>
-      <c r="Y74" s="106"/>
-      <c r="Z74" s="106"/>
-      <c r="AA74" s="106"/>
-      <c r="AB74" s="106"/>
-      <c r="AC74" s="106"/>
-      <c r="AD74" s="106"/>
+      <c r="Q74" s="110"/>
+      <c r="R74" s="110"/>
+      <c r="S74" s="110"/>
+      <c r="T74" s="110"/>
+      <c r="U74" s="110"/>
+      <c r="V74" s="110"/>
+      <c r="W74" s="110"/>
+      <c r="X74" s="110"/>
+      <c r="Y74" s="110"/>
+      <c r="Z74" s="110"/>
+      <c r="AA74" s="110"/>
+      <c r="AB74" s="110"/>
+      <c r="AC74" s="110"/>
+      <c r="AD74" s="110"/>
     </row>
     <row r="75" spans="2:30" ht="15" customHeight="1">
-      <c r="Q75" s="106"/>
-      <c r="R75" s="106"/>
-      <c r="S75" s="106"/>
-      <c r="T75" s="106"/>
-      <c r="U75" s="106"/>
-      <c r="V75" s="106"/>
-      <c r="W75" s="106"/>
-      <c r="X75" s="106"/>
-      <c r="Y75" s="106"/>
-      <c r="Z75" s="106"/>
-      <c r="AA75" s="106"/>
-      <c r="AB75" s="106"/>
-      <c r="AC75" s="106"/>
-      <c r="AD75" s="106"/>
+      <c r="Q75" s="110"/>
+      <c r="R75" s="110"/>
+      <c r="S75" s="110"/>
+      <c r="T75" s="110"/>
+      <c r="U75" s="110"/>
+      <c r="V75" s="110"/>
+      <c r="W75" s="110"/>
+      <c r="X75" s="110"/>
+      <c r="Y75" s="110"/>
+      <c r="Z75" s="110"/>
+      <c r="AA75" s="110"/>
+      <c r="AB75" s="110"/>
+      <c r="AC75" s="110"/>
+      <c r="AD75" s="110"/>
     </row>
     <row r="76" spans="2:30">
-      <c r="Q76" s="106"/>
-      <c r="R76" s="106"/>
-      <c r="S76" s="106"/>
-      <c r="T76" s="106"/>
-      <c r="U76" s="106"/>
-      <c r="V76" s="106"/>
-      <c r="W76" s="106"/>
-      <c r="X76" s="106"/>
-      <c r="Y76" s="106"/>
-      <c r="Z76" s="106"/>
-      <c r="AA76" s="106"/>
-      <c r="AB76" s="106"/>
-      <c r="AC76" s="106"/>
-      <c r="AD76" s="106"/>
+      <c r="Q76" s="110"/>
+      <c r="R76" s="110"/>
+      <c r="S76" s="110"/>
+      <c r="T76" s="110"/>
+      <c r="U76" s="110"/>
+      <c r="V76" s="110"/>
+      <c r="W76" s="110"/>
+      <c r="X76" s="110"/>
+      <c r="Y76" s="110"/>
+      <c r="Z76" s="110"/>
+      <c r="AA76" s="110"/>
+      <c r="AB76" s="110"/>
+      <c r="AC76" s="110"/>
+      <c r="AD76" s="110"/>
     </row>
     <row r="77" spans="2:30">
-      <c r="Q77" s="106"/>
-      <c r="R77" s="106"/>
-      <c r="S77" s="106"/>
-      <c r="T77" s="106"/>
-      <c r="U77" s="106"/>
-      <c r="V77" s="106"/>
-      <c r="W77" s="106"/>
-      <c r="X77" s="106"/>
-      <c r="Y77" s="106"/>
-      <c r="Z77" s="106"/>
-      <c r="AA77" s="106"/>
-      <c r="AB77" s="106"/>
-      <c r="AC77" s="106"/>
-      <c r="AD77" s="106"/>
+      <c r="Q77" s="110"/>
+      <c r="R77" s="110"/>
+      <c r="S77" s="110"/>
+      <c r="T77" s="110"/>
+      <c r="U77" s="110"/>
+      <c r="V77" s="110"/>
+      <c r="W77" s="110"/>
+      <c r="X77" s="110"/>
+      <c r="Y77" s="110"/>
+      <c r="Z77" s="110"/>
+      <c r="AA77" s="110"/>
+      <c r="AB77" s="110"/>
+      <c r="AC77" s="110"/>
+      <c r="AD77" s="110"/>
     </row>
     <row r="79" spans="2:30" ht="17.25">
-      <c r="B79" s="104" t="s">
+      <c r="B79" s="117" t="s">
         <v>101</v>
       </c>
-      <c r="C79" s="104"/>
-      <c r="D79" s="104"/>
-      <c r="E79" s="104"/>
-      <c r="F79" s="104"/>
-      <c r="G79" s="104"/>
-      <c r="H79" s="104"/>
-      <c r="I79" s="104"/>
-      <c r="J79" s="104"/>
-      <c r="K79" s="104"/>
-      <c r="L79" s="104"/>
-      <c r="M79" s="104"/>
-      <c r="N79" s="104"/>
-      <c r="O79" s="104"/>
+      <c r="C79" s="117"/>
+      <c r="D79" s="117"/>
+      <c r="E79" s="117"/>
+      <c r="F79" s="117"/>
+      <c r="G79" s="117"/>
+      <c r="H79" s="117"/>
+      <c r="I79" s="117"/>
+      <c r="J79" s="117"/>
+      <c r="K79" s="117"/>
+      <c r="L79" s="117"/>
+      <c r="M79" s="117"/>
+      <c r="N79" s="117"/>
+      <c r="O79" s="117"/>
       <c r="Q79" s="20" t="s">
         <v>196</v>
       </c>
@@ -4214,22 +4226,22 @@
       <c r="M81" s="109"/>
       <c r="N81" s="109"/>
       <c r="O81" s="109"/>
-      <c r="Q81" s="106" t="s">
+      <c r="Q81" s="110" t="s">
         <v>202</v>
       </c>
-      <c r="R81" s="106"/>
-      <c r="S81" s="106"/>
-      <c r="T81" s="106"/>
-      <c r="U81" s="106"/>
-      <c r="V81" s="106"/>
-      <c r="W81" s="106"/>
-      <c r="X81" s="106"/>
-      <c r="Y81" s="106"/>
-      <c r="Z81" s="106"/>
-      <c r="AA81" s="106"/>
-      <c r="AB81" s="106"/>
-      <c r="AC81" s="106"/>
-      <c r="AD81" s="106"/>
+      <c r="R81" s="110"/>
+      <c r="S81" s="110"/>
+      <c r="T81" s="110"/>
+      <c r="U81" s="110"/>
+      <c r="V81" s="110"/>
+      <c r="W81" s="110"/>
+      <c r="X81" s="110"/>
+      <c r="Y81" s="110"/>
+      <c r="Z81" s="110"/>
+      <c r="AA81" s="110"/>
+      <c r="AB81" s="110"/>
+      <c r="AC81" s="110"/>
+      <c r="AD81" s="110"/>
     </row>
     <row r="82" spans="2:30">
       <c r="B82" s="109"/>
@@ -4246,45 +4258,56 @@
       <c r="M82" s="109"/>
       <c r="N82" s="109"/>
       <c r="O82" s="109"/>
-      <c r="Q82" s="106"/>
-      <c r="R82" s="106"/>
-      <c r="S82" s="106"/>
-      <c r="T82" s="106"/>
-      <c r="U82" s="106"/>
-      <c r="V82" s="106"/>
-      <c r="W82" s="106"/>
-      <c r="X82" s="106"/>
-      <c r="Y82" s="106"/>
-      <c r="Z82" s="106"/>
-      <c r="AA82" s="106"/>
-      <c r="AB82" s="106"/>
-      <c r="AC82" s="106"/>
-      <c r="AD82" s="106"/>
+      <c r="Q82" s="110"/>
+      <c r="R82" s="110"/>
+      <c r="S82" s="110"/>
+      <c r="T82" s="110"/>
+      <c r="U82" s="110"/>
+      <c r="V82" s="110"/>
+      <c r="W82" s="110"/>
+      <c r="X82" s="110"/>
+      <c r="Y82" s="110"/>
+      <c r="Z82" s="110"/>
+      <c r="AA82" s="110"/>
+      <c r="AB82" s="110"/>
+      <c r="AC82" s="110"/>
+      <c r="AD82" s="110"/>
     </row>
     <row r="83" spans="2:30">
-      <c r="Q83" s="106"/>
-      <c r="R83" s="106"/>
-      <c r="S83" s="106"/>
-      <c r="T83" s="106"/>
-      <c r="U83" s="106"/>
-      <c r="V83" s="106"/>
-      <c r="W83" s="106"/>
-      <c r="X83" s="106"/>
-      <c r="Y83" s="106"/>
-      <c r="Z83" s="106"/>
-      <c r="AA83" s="106"/>
-      <c r="AB83" s="106"/>
-      <c r="AC83" s="106"/>
-      <c r="AD83" s="106"/>
+      <c r="Q83" s="110"/>
+      <c r="R83" s="110"/>
+      <c r="S83" s="110"/>
+      <c r="T83" s="110"/>
+      <c r="U83" s="110"/>
+      <c r="V83" s="110"/>
+      <c r="W83" s="110"/>
+      <c r="X83" s="110"/>
+      <c r="Y83" s="110"/>
+      <c r="Z83" s="110"/>
+      <c r="AA83" s="110"/>
+      <c r="AB83" s="110"/>
+      <c r="AC83" s="110"/>
+      <c r="AD83" s="110"/>
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="B81:O82"/>
-    <mergeCell ref="Q62:AD63"/>
-    <mergeCell ref="B63:O66"/>
-    <mergeCell ref="B67:O68"/>
-    <mergeCell ref="Q73:AD77"/>
-    <mergeCell ref="Q81:AD83"/>
+    <mergeCell ref="B58:O58"/>
+    <mergeCell ref="B79:O79"/>
+    <mergeCell ref="Q58:AD58"/>
+    <mergeCell ref="B60:O61"/>
+    <mergeCell ref="V48:Z48"/>
+    <mergeCell ref="S50:AB50"/>
+    <mergeCell ref="Q67:AD69"/>
+    <mergeCell ref="B50:O51"/>
+    <mergeCell ref="S33:AB34"/>
+    <mergeCell ref="S37:AB38"/>
+    <mergeCell ref="S42:AB42"/>
+    <mergeCell ref="S45:AB46"/>
+    <mergeCell ref="B55:O56"/>
+    <mergeCell ref="B33:N34"/>
+    <mergeCell ref="B38:O39"/>
+    <mergeCell ref="B41:O41"/>
+    <mergeCell ref="B45:O46"/>
     <mergeCell ref="B2:O2"/>
     <mergeCell ref="B4:O5"/>
     <mergeCell ref="B8:O9"/>
@@ -4301,23 +4324,12 @@
     <mergeCell ref="V40:Z40"/>
     <mergeCell ref="S29:AB29"/>
     <mergeCell ref="S26:AB26"/>
-    <mergeCell ref="S33:AB34"/>
-    <mergeCell ref="S37:AB38"/>
-    <mergeCell ref="S42:AB42"/>
-    <mergeCell ref="S45:AB46"/>
-    <mergeCell ref="B55:O56"/>
-    <mergeCell ref="B33:N34"/>
-    <mergeCell ref="B38:O39"/>
-    <mergeCell ref="B41:O41"/>
-    <mergeCell ref="B45:O46"/>
-    <mergeCell ref="B58:O58"/>
-    <mergeCell ref="B79:O79"/>
-    <mergeCell ref="Q58:AD58"/>
-    <mergeCell ref="B60:O61"/>
-    <mergeCell ref="V48:Z48"/>
-    <mergeCell ref="S50:AB50"/>
-    <mergeCell ref="Q67:AD69"/>
-    <mergeCell ref="B50:O51"/>
+    <mergeCell ref="B81:O82"/>
+    <mergeCell ref="Q62:AD63"/>
+    <mergeCell ref="B63:O66"/>
+    <mergeCell ref="B67:O68"/>
+    <mergeCell ref="Q73:AD77"/>
+    <mergeCell ref="Q81:AD83"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -72461,8 +72473,8 @@
   </sheetPr>
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -72504,14 +72516,14 @@
         <f>Regiones!B2</f>
         <v>Interior de Buenos Aires</v>
       </c>
-      <c r="C2" s="35">
+      <c r="C2" s="127">
         <v>31049</v>
       </c>
-      <c r="D2" s="35">
+      <c r="D2" s="127">
         <v>1226</v>
       </c>
-      <c r="E2" s="35">
-        <v>1000</v>
+      <c r="E2" s="127">
+        <v>886</v>
       </c>
       <c r="G2" s="41">
         <v>2000</v>
@@ -72526,14 +72538,14 @@
         <f>Regiones!B3</f>
         <v>24 Partidos del Gran Buenos Aires</v>
       </c>
-      <c r="C3" s="35">
+      <c r="C3" s="127">
         <v>53940</v>
       </c>
-      <c r="D3" s="35">
+      <c r="D3" s="127">
         <v>2130</v>
       </c>
-      <c r="E3" s="35">
-        <v>1000</v>
+      <c r="E3" s="128">
+        <v>1539</v>
       </c>
       <c r="G3" s="41">
         <v>2000</v>
@@ -72548,14 +72560,14 @@
         <f>Regiones!B4</f>
         <v>Córdoba</v>
       </c>
-      <c r="C4" s="35">
+      <c r="C4" s="127">
         <v>17998</v>
       </c>
-      <c r="D4" s="35">
+      <c r="D4" s="127">
         <v>710</v>
       </c>
-      <c r="E4" s="35">
-        <v>500</v>
+      <c r="E4" s="127">
+        <v>513</v>
       </c>
       <c r="G4" s="41">
         <v>2000</v>
@@ -72570,14 +72582,14 @@
         <f>Regiones!B5</f>
         <v>Santa Fe</v>
       </c>
-      <c r="C5" s="35">
+      <c r="C5" s="127">
         <v>17376</v>
       </c>
-      <c r="D5" s="35">
+      <c r="D5" s="127">
         <v>686</v>
       </c>
-      <c r="E5" s="35">
-        <v>500</v>
+      <c r="E5" s="127">
+        <v>496</v>
       </c>
       <c r="G5" s="41">
         <v>2000</v>
@@ -72592,14 +72604,14 @@
         <f>Regiones!B6</f>
         <v>Ciudad de Buenos Aires</v>
       </c>
-      <c r="C6" s="35">
+      <c r="C6" s="127">
         <v>15720</v>
       </c>
-      <c r="D6" s="35">
+      <c r="D6" s="127">
         <v>620</v>
       </c>
-      <c r="E6" s="35">
-        <v>500</v>
+      <c r="E6" s="127">
+        <v>448</v>
       </c>
       <c r="G6" s="41">
         <v>2000</v>
@@ -72614,14 +72626,14 @@
         <f>Regiones!B7</f>
         <v>Mendoza</v>
       </c>
-      <c r="C7" s="35">
+      <c r="C7" s="127">
         <v>5557</v>
       </c>
-      <c r="D7" s="35">
+      <c r="D7" s="127">
         <v>228</v>
       </c>
-      <c r="E7" s="35">
-        <v>10</v>
+      <c r="E7" s="127">
+        <v>165</v>
       </c>
       <c r="G7" s="41">
         <v>2000</v>
@@ -72636,14 +72648,14 @@
         <f>Regiones!B8</f>
         <v>Tucumán</v>
       </c>
-      <c r="C8" s="35">
+      <c r="C8" s="127">
         <v>4494</v>
       </c>
-      <c r="D8" s="35">
+      <c r="D8" s="127">
         <v>334</v>
       </c>
-      <c r="E8" s="35">
-        <v>10</v>
+      <c r="E8" s="127">
+        <v>242</v>
       </c>
       <c r="G8" s="41">
         <v>2000</v>
@@ -72658,14 +72670,14 @@
         <f>Regiones!B9</f>
         <v>Entre Ríos</v>
       </c>
-      <c r="C9" s="35">
+      <c r="C9" s="127">
         <v>6723</v>
       </c>
-      <c r="D9" s="35">
+      <c r="D9" s="127">
         <v>265</v>
       </c>
-      <c r="E9" s="35">
-        <v>10</v>
+      <c r="E9" s="127">
+        <v>192</v>
       </c>
       <c r="G9" s="41">
         <v>2000</v>
@@ -72680,14 +72692,14 @@
         <f>Regiones!B10</f>
         <v>Salta</v>
       </c>
-      <c r="C10" s="35">
+      <c r="C10" s="127">
         <v>3769</v>
       </c>
-      <c r="D10" s="35">
+      <c r="D10" s="127">
         <v>280</v>
       </c>
-      <c r="E10" s="35">
-        <v>10</v>
+      <c r="E10" s="127">
+        <v>203</v>
       </c>
       <c r="G10" s="41">
         <v>2000</v>
@@ -72702,14 +72714,14 @@
         <f>Regiones!B11</f>
         <v>Misiones</v>
       </c>
-      <c r="C11" s="35">
+      <c r="C11" s="127">
         <v>3315</v>
       </c>
-      <c r="D11" s="35">
+      <c r="D11" s="127">
         <v>215</v>
       </c>
-      <c r="E11" s="35">
-        <v>10</v>
+      <c r="E11" s="127">
+        <v>156</v>
       </c>
       <c r="G11" s="41">
         <v>2000</v>
@@ -72724,14 +72736,14 @@
         <f>Regiones!B12</f>
         <v>Chaco</v>
       </c>
-      <c r="C12" s="35">
+      <c r="C12" s="127">
         <v>3176</v>
       </c>
-      <c r="D12" s="35">
+      <c r="D12" s="127">
         <v>206</v>
       </c>
-      <c r="E12" s="35">
-        <v>10</v>
+      <c r="E12" s="127">
+        <v>149</v>
       </c>
       <c r="G12" s="41">
         <v>2000</v>
@@ -72746,14 +72758,14 @@
         <f>Regiones!B13</f>
         <v>Corrientes</v>
       </c>
-      <c r="C13" s="35">
+      <c r="C13" s="127">
         <v>2987</v>
       </c>
-      <c r="D13" s="35">
+      <c r="D13" s="127">
         <v>194</v>
       </c>
-      <c r="E13" s="35">
-        <v>10</v>
+      <c r="E13" s="127">
+        <v>141</v>
       </c>
       <c r="G13" s="41">
         <v>2000</v>
@@ -72768,14 +72780,14 @@
         <f>Regiones!B14</f>
         <v>Santiago del Estero</v>
       </c>
-      <c r="C14" s="35">
+      <c r="C14" s="127">
         <v>2712</v>
       </c>
-      <c r="D14" s="35">
+      <c r="D14" s="127">
         <v>201</v>
       </c>
-      <c r="E14" s="35">
-        <v>10</v>
+      <c r="E14" s="127">
+        <v>146</v>
       </c>
       <c r="G14" s="41">
         <v>2000</v>
@@ -72790,14 +72802,14 @@
         <f>Regiones!B15</f>
         <v>San Juan</v>
       </c>
-      <c r="C15" s="35">
+      <c r="C15" s="127">
         <v>2176</v>
       </c>
-      <c r="D15" s="35">
+      <c r="D15" s="127">
         <v>89</v>
       </c>
-      <c r="E15" s="35">
-        <v>10</v>
+      <c r="E15" s="127">
+        <v>65</v>
       </c>
       <c r="G15" s="41">
         <v>2000</v>
@@ -72812,14 +72824,14 @@
         <f>Regiones!B16</f>
         <v>Jujuy</v>
       </c>
-      <c r="C16" s="35">
+      <c r="C16" s="127">
         <v>2089</v>
       </c>
-      <c r="D16" s="35">
+      <c r="D16" s="127">
         <v>155</v>
       </c>
-      <c r="E16" s="35">
-        <v>5</v>
+      <c r="E16" s="127">
+        <v>112</v>
       </c>
       <c r="G16" s="41">
         <v>2000</v>
@@ -72834,14 +72846,14 @@
         <f>Regiones!B17</f>
         <v>Río Negro</v>
       </c>
-      <c r="C17" s="35">
+      <c r="C17" s="127">
         <v>1901</v>
       </c>
-      <c r="D17" s="35">
+      <c r="D17" s="127">
         <v>111</v>
       </c>
-      <c r="E17" s="35">
-        <v>5</v>
+      <c r="E17" s="127">
+        <v>81</v>
       </c>
       <c r="G17" s="41">
         <v>2000</v>
@@ -72856,14 +72868,14 @@
         <f>Regiones!B18</f>
         <v>Neuquén</v>
       </c>
-      <c r="C18" s="35">
+      <c r="C18" s="127">
         <v>1641</v>
       </c>
-      <c r="D18" s="35">
+      <c r="D18" s="127">
         <v>96</v>
       </c>
-      <c r="E18" s="35">
-        <v>5</v>
+      <c r="E18" s="127">
+        <v>70</v>
       </c>
       <c r="G18" s="41">
         <v>2000</v>
@@ -72878,14 +72890,14 @@
         <f>Regiones!B19</f>
         <v>Formosa</v>
       </c>
-      <c r="C19" s="35">
+      <c r="C19" s="127">
         <v>1595</v>
       </c>
-      <c r="D19" s="35">
+      <c r="D19" s="127">
         <v>103</v>
       </c>
-      <c r="E19" s="35">
-        <v>5</v>
+      <c r="E19" s="127">
+        <v>75</v>
       </c>
       <c r="G19" s="41">
         <v>2000</v>
@@ -72900,14 +72912,14 @@
         <f>Regiones!B20</f>
         <v>Chubut</v>
       </c>
-      <c r="C20" s="35">
+      <c r="C20" s="127">
         <v>1515</v>
       </c>
-      <c r="D20" s="35">
+      <c r="D20" s="127">
         <v>89</v>
       </c>
-      <c r="E20" s="35">
-        <v>5</v>
+      <c r="E20" s="127">
+        <v>65</v>
       </c>
       <c r="G20" s="41">
         <v>2000</v>
@@ -72922,14 +72934,14 @@
         <f>Regiones!B21</f>
         <v>San Luis</v>
       </c>
-      <c r="C21" s="35">
+      <c r="C21" s="127">
         <v>1381</v>
       </c>
-      <c r="D21" s="35">
+      <c r="D21" s="127">
         <v>56</v>
       </c>
-      <c r="E21" s="35">
-        <v>5</v>
+      <c r="E21" s="127">
+        <v>41</v>
       </c>
       <c r="G21" s="41">
         <v>2000</v>
@@ -72944,14 +72956,14 @@
         <f>Regiones!B22</f>
         <v>Catamarca</v>
       </c>
-      <c r="C22" s="35">
+      <c r="C22" s="127">
         <v>1141</v>
       </c>
-      <c r="D22" s="35">
+      <c r="D22" s="127">
         <v>84</v>
       </c>
-      <c r="E22" s="35">
-        <v>5</v>
+      <c r="E22" s="127">
+        <v>61</v>
       </c>
       <c r="G22" s="41">
         <v>2000</v>
@@ -72966,14 +72978,14 @@
         <f>Regiones!B23</f>
         <v>La Rioja</v>
       </c>
-      <c r="C23" s="35">
+      <c r="C23" s="127">
         <v>1035</v>
       </c>
-      <c r="D23" s="35">
+      <c r="D23" s="127">
         <v>77</v>
       </c>
-      <c r="E23" s="35">
-        <v>5</v>
+      <c r="E23" s="127">
+        <v>56</v>
       </c>
       <c r="G23" s="41">
         <v>2000</v>
@@ -72988,14 +73000,14 @@
         <f>Regiones!B24</f>
         <v>La Pampa</v>
       </c>
-      <c r="C24" s="35">
+      <c r="C24" s="127">
         <v>949</v>
       </c>
-      <c r="D24" s="35">
+      <c r="D24" s="127">
         <v>55</v>
       </c>
-      <c r="E24" s="35">
-        <v>5</v>
+      <c r="E24" s="127">
+        <v>40</v>
       </c>
       <c r="G24" s="41">
         <v>2000</v>
@@ -73010,14 +73022,14 @@
         <f>Regiones!B25</f>
         <v>Santa Cruz</v>
       </c>
-      <c r="C25" s="35">
+      <c r="C25" s="127">
         <v>815</v>
       </c>
-      <c r="D25" s="35">
+      <c r="D25" s="127">
         <v>48</v>
       </c>
-      <c r="E25" s="35">
-        <v>5</v>
+      <c r="E25" s="127">
+        <v>35</v>
       </c>
       <c r="G25" s="41">
         <v>2000</v>
@@ -73032,14 +73044,14 @@
         <f>Regiones!B26</f>
         <v>Tierra del Fuego</v>
       </c>
-      <c r="C26" s="35">
+      <c r="C26" s="127">
         <v>378</v>
       </c>
-      <c r="D26" s="35">
+      <c r="D26" s="127">
         <v>22</v>
       </c>
-      <c r="E26" s="35">
-        <v>5</v>
+      <c r="E26" s="127">
+        <v>16</v>
       </c>
       <c r="G26" s="41">
         <v>2000</v>
@@ -73058,8 +73070,8 @@
   </sheetPr>
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -73097,10 +73109,10 @@
       <c r="C2" s="35">
         <v>1</v>
       </c>
-      <c r="E2" s="124" t="s">
+      <c r="E2" s="106" t="s">
         <v>232</v>
       </c>
-      <c r="F2" s="125" t="str">
+      <c r="F2" s="107" t="str">
         <f>_xlfn.CONCAT(F4+1,RIGHT(F3,7))</f>
         <v>11/1/2020</v>
       </c>
@@ -73117,7 +73129,7 @@
       <c r="C3" s="35">
         <v>1</v>
       </c>
-      <c r="F3" s="126" t="str">
+      <c r="F3" s="108" t="str">
         <f>E2</f>
         <v>10/1/2020</v>
       </c>
@@ -73134,12 +73146,12 @@
       <c r="C4" s="35">
         <v>0</v>
       </c>
-      <c r="E4" s="123"/>
-      <c r="F4" s="125" t="str">
+      <c r="E4" s="105"/>
+      <c r="F4" s="107" t="str">
         <f>LEFT(F3,2)</f>
         <v>10</v>
       </c>
-      <c r="H4" s="122"/>
+      <c r="H4" s="104"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="43">
@@ -73153,7 +73165,7 @@
       <c r="C5" s="35">
         <v>0</v>
       </c>
-      <c r="I5" s="123"/>
+      <c r="I5" s="105"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="43">
@@ -73167,7 +73179,7 @@
       <c r="C6" s="35">
         <v>1</v>
       </c>
-      <c r="I6" s="123"/>
+      <c r="I6" s="105"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="43">
@@ -73220,7 +73232,7 @@
       <c r="C10" s="35">
         <v>0</v>
       </c>
-      <c r="E10" s="122"/>
+      <c r="E10" s="104"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="43">

</xml_diff>

<commit_message>
adds estimated NPI effects added better testing capacity per region
</commit_message>
<xml_diff>
--- a/COVID Simulator v 1.1/Input/Input_Simulador.xlsx
+++ b/COVID Simulator v 1.1/Input/Input_Simulador.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignacio.brottier\Documents\COVID 19\COVID-19-Simulation-Argentina\COVID Simulator v 1.1\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D1A796-2D43-460C-B58F-CF124B395C9B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD5CEC3-3131-48A0-9FF1-BE5CEC59A1A8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="5" activeTab="7" xr2:uid="{55AC4C4C-7526-4060-9BB2-10E89010456B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="7" activeTab="9" xr2:uid="{55AC4C4C-7526-4060-9BB2-10E89010456B}"/>
   </bookViews>
   <sheets>
     <sheet name="Información" sheetId="28" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="237">
   <si>
     <t>Santa Fe</t>
   </si>
@@ -1634,6 +1634,18 @@
   <si>
     <t>10/1/2020</t>
   </si>
+  <si>
+    <t>3. Comentario</t>
+  </si>
+  <si>
+    <t>Remoticidad</t>
+  </si>
+  <si>
+    <t>Dist Social</t>
+  </si>
+  <si>
+    <t>Viajes</t>
+  </si>
 </sst>
 </file>
 
@@ -1872,7 +1884,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1931,6 +1943,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB4C6E7"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -2084,7 +2102,7 @@
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2330,11 +2348,38 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2345,16 +2390,10 @@
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2366,30 +2405,11 @@
     <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Comma" xfId="7" builtinId="3"/>
@@ -2842,22 +2862,22 @@
   <sheetData>
     <row r="1" spans="2:45" s="9" customFormat="1"/>
     <row r="2" spans="2:45" s="9" customFormat="1" ht="33.75" customHeight="1" thickBot="1">
-      <c r="B2" s="111" t="s">
+      <c r="B2" s="120" t="s">
         <v>105</v>
       </c>
-      <c r="C2" s="111"/>
-      <c r="D2" s="111"/>
-      <c r="E2" s="111"/>
-      <c r="F2" s="111"/>
-      <c r="G2" s="111"/>
-      <c r="H2" s="111"/>
-      <c r="I2" s="111"/>
-      <c r="J2" s="111"/>
-      <c r="K2" s="111"/>
-      <c r="L2" s="111"/>
-      <c r="M2" s="111"/>
-      <c r="N2" s="111"/>
-      <c r="O2" s="111"/>
+      <c r="C2" s="120"/>
+      <c r="D2" s="120"/>
+      <c r="E2" s="120"/>
+      <c r="F2" s="120"/>
+      <c r="G2" s="120"/>
+      <c r="H2" s="120"/>
+      <c r="I2" s="120"/>
+      <c r="J2" s="120"/>
+      <c r="K2" s="120"/>
+      <c r="L2" s="120"/>
+      <c r="M2" s="120"/>
+      <c r="N2" s="120"/>
+      <c r="O2" s="120"/>
       <c r="Q2" s="57"/>
       <c r="R2" s="57"/>
       <c r="S2" s="57"/>
@@ -2875,248 +2895,248 @@
     </row>
     <row r="3" spans="2:45" ht="15.75" thickTop="1"/>
     <row r="4" spans="2:45" ht="15" customHeight="1">
-      <c r="B4" s="109" t="s">
+      <c r="B4" s="116" t="s">
         <v>99</v>
       </c>
-      <c r="C4" s="109"/>
-      <c r="D4" s="109"/>
-      <c r="E4" s="109"/>
-      <c r="F4" s="109"/>
-      <c r="G4" s="109"/>
-      <c r="H4" s="109"/>
-      <c r="I4" s="109"/>
-      <c r="J4" s="109"/>
-      <c r="K4" s="109"/>
-      <c r="L4" s="109"/>
-      <c r="M4" s="109"/>
-      <c r="N4" s="109"/>
-      <c r="O4" s="109"/>
+      <c r="C4" s="116"/>
+      <c r="D4" s="116"/>
+      <c r="E4" s="116"/>
+      <c r="F4" s="116"/>
+      <c r="G4" s="116"/>
+      <c r="H4" s="116"/>
+      <c r="I4" s="116"/>
+      <c r="J4" s="116"/>
+      <c r="K4" s="116"/>
+      <c r="L4" s="116"/>
+      <c r="M4" s="116"/>
+      <c r="N4" s="116"/>
+      <c r="O4" s="116"/>
     </row>
     <row r="5" spans="2:45" ht="22.5" customHeight="1">
-      <c r="B5" s="109"/>
-      <c r="C5" s="109"/>
-      <c r="D5" s="109"/>
-      <c r="E5" s="109"/>
-      <c r="F5" s="109"/>
-      <c r="G5" s="109"/>
-      <c r="H5" s="109"/>
-      <c r="I5" s="109"/>
-      <c r="J5" s="109"/>
-      <c r="K5" s="109"/>
-      <c r="L5" s="109"/>
-      <c r="M5" s="109"/>
-      <c r="N5" s="109"/>
-      <c r="O5" s="109"/>
-      <c r="Q5" s="116" t="s">
+      <c r="B5" s="116"/>
+      <c r="C5" s="116"/>
+      <c r="D5" s="116"/>
+      <c r="E5" s="116"/>
+      <c r="F5" s="116"/>
+      <c r="G5" s="116"/>
+      <c r="H5" s="116"/>
+      <c r="I5" s="116"/>
+      <c r="J5" s="116"/>
+      <c r="K5" s="116"/>
+      <c r="L5" s="116"/>
+      <c r="M5" s="116"/>
+      <c r="N5" s="116"/>
+      <c r="O5" s="116"/>
+      <c r="Q5" s="124" t="s">
         <v>173</v>
       </c>
-      <c r="R5" s="116"/>
-      <c r="S5" s="116"/>
-      <c r="T5" s="116"/>
-      <c r="U5" s="116"/>
-      <c r="V5" s="116"/>
-      <c r="W5" s="116"/>
-      <c r="X5" s="116"/>
-      <c r="Y5" s="116"/>
-      <c r="Z5" s="116"/>
-      <c r="AA5" s="116"/>
-      <c r="AB5" s="116"/>
-      <c r="AC5" s="116"/>
-      <c r="AD5" s="116"/>
+      <c r="R5" s="124"/>
+      <c r="S5" s="124"/>
+      <c r="T5" s="124"/>
+      <c r="U5" s="124"/>
+      <c r="V5" s="124"/>
+      <c r="W5" s="124"/>
+      <c r="X5" s="124"/>
+      <c r="Y5" s="124"/>
+      <c r="Z5" s="124"/>
+      <c r="AA5" s="124"/>
+      <c r="AB5" s="124"/>
+      <c r="AC5" s="124"/>
+      <c r="AD5" s="124"/>
       <c r="AQ5" s="9"/>
       <c r="AR5" s="9"/>
       <c r="AS5" s="9"/>
     </row>
     <row r="6" spans="2:45">
-      <c r="Q6" s="115" t="s">
+      <c r="Q6" s="123" t="s">
         <v>174</v>
       </c>
-      <c r="R6" s="115"/>
-      <c r="S6" s="115"/>
-      <c r="T6" s="115"/>
-      <c r="U6" s="115"/>
-      <c r="V6" s="115"/>
-      <c r="W6" s="115"/>
-      <c r="X6" s="115"/>
-      <c r="Y6" s="115"/>
-      <c r="Z6" s="115"/>
-      <c r="AA6" s="115"/>
-      <c r="AB6" s="115"/>
-      <c r="AC6" s="115"/>
-      <c r="AD6" s="115"/>
+      <c r="R6" s="123"/>
+      <c r="S6" s="123"/>
+      <c r="T6" s="123"/>
+      <c r="U6" s="123"/>
+      <c r="V6" s="123"/>
+      <c r="W6" s="123"/>
+      <c r="X6" s="123"/>
+      <c r="Y6" s="123"/>
+      <c r="Z6" s="123"/>
+      <c r="AA6" s="123"/>
+      <c r="AB6" s="123"/>
+      <c r="AC6" s="123"/>
+      <c r="AD6" s="123"/>
     </row>
     <row r="7" spans="2:45">
-      <c r="Q7" s="115"/>
-      <c r="R7" s="115"/>
-      <c r="S7" s="115"/>
-      <c r="T7" s="115"/>
-      <c r="U7" s="115"/>
-      <c r="V7" s="115"/>
-      <c r="W7" s="115"/>
-      <c r="X7" s="115"/>
-      <c r="Y7" s="115"/>
-      <c r="Z7" s="115"/>
-      <c r="AA7" s="115"/>
-      <c r="AB7" s="115"/>
-      <c r="AC7" s="115"/>
-      <c r="AD7" s="115"/>
+      <c r="Q7" s="123"/>
+      <c r="R7" s="123"/>
+      <c r="S7" s="123"/>
+      <c r="T7" s="123"/>
+      <c r="U7" s="123"/>
+      <c r="V7" s="123"/>
+      <c r="W7" s="123"/>
+      <c r="X7" s="123"/>
+      <c r="Y7" s="123"/>
+      <c r="Z7" s="123"/>
+      <c r="AA7" s="123"/>
+      <c r="AB7" s="123"/>
+      <c r="AC7" s="123"/>
+      <c r="AD7" s="123"/>
     </row>
     <row r="8" spans="2:45" ht="15" customHeight="1">
-      <c r="B8" s="109" t="s">
+      <c r="B8" s="116" t="s">
         <v>103</v>
       </c>
-      <c r="C8" s="109"/>
-      <c r="D8" s="109"/>
-      <c r="E8" s="109"/>
-      <c r="F8" s="109"/>
-      <c r="G8" s="109"/>
-      <c r="H8" s="109"/>
-      <c r="I8" s="109"/>
-      <c r="J8" s="109"/>
-      <c r="K8" s="109"/>
-      <c r="L8" s="109"/>
-      <c r="M8" s="109"/>
-      <c r="N8" s="109"/>
-      <c r="O8" s="109"/>
-      <c r="Q8" s="115"/>
-      <c r="R8" s="115"/>
-      <c r="S8" s="115"/>
-      <c r="T8" s="115"/>
-      <c r="U8" s="115"/>
-      <c r="V8" s="115"/>
-      <c r="W8" s="115"/>
-      <c r="X8" s="115"/>
-      <c r="Y8" s="115"/>
-      <c r="Z8" s="115"/>
-      <c r="AA8" s="115"/>
-      <c r="AB8" s="115"/>
-      <c r="AC8" s="115"/>
-      <c r="AD8" s="115"/>
+      <c r="C8" s="116"/>
+      <c r="D8" s="116"/>
+      <c r="E8" s="116"/>
+      <c r="F8" s="116"/>
+      <c r="G8" s="116"/>
+      <c r="H8" s="116"/>
+      <c r="I8" s="116"/>
+      <c r="J8" s="116"/>
+      <c r="K8" s="116"/>
+      <c r="L8" s="116"/>
+      <c r="M8" s="116"/>
+      <c r="N8" s="116"/>
+      <c r="O8" s="116"/>
+      <c r="Q8" s="123"/>
+      <c r="R8" s="123"/>
+      <c r="S8" s="123"/>
+      <c r="T8" s="123"/>
+      <c r="U8" s="123"/>
+      <c r="V8" s="123"/>
+      <c r="W8" s="123"/>
+      <c r="X8" s="123"/>
+      <c r="Y8" s="123"/>
+      <c r="Z8" s="123"/>
+      <c r="AA8" s="123"/>
+      <c r="AB8" s="123"/>
+      <c r="AC8" s="123"/>
+      <c r="AD8" s="123"/>
     </row>
     <row r="9" spans="2:45" ht="17.25" customHeight="1">
-      <c r="B9" s="109"/>
-      <c r="C9" s="109"/>
-      <c r="D9" s="109"/>
-      <c r="E9" s="109"/>
-      <c r="F9" s="109"/>
-      <c r="G9" s="109"/>
-      <c r="H9" s="109"/>
-      <c r="I9" s="109"/>
-      <c r="J9" s="109"/>
-      <c r="K9" s="109"/>
-      <c r="L9" s="109"/>
-      <c r="M9" s="109"/>
-      <c r="N9" s="109"/>
-      <c r="O9" s="109"/>
+      <c r="B9" s="116"/>
+      <c r="C9" s="116"/>
+      <c r="D9" s="116"/>
+      <c r="E9" s="116"/>
+      <c r="F9" s="116"/>
+      <c r="G9" s="116"/>
+      <c r="H9" s="116"/>
+      <c r="I9" s="116"/>
+      <c r="J9" s="116"/>
+      <c r="K9" s="116"/>
+      <c r="L9" s="116"/>
+      <c r="M9" s="116"/>
+      <c r="N9" s="116"/>
+      <c r="O9" s="116"/>
     </row>
     <row r="12" spans="2:45" ht="17.25" customHeight="1">
       <c r="D12" s="15" t="s">
         <v>96</v>
       </c>
       <c r="H12" s="17"/>
-      <c r="I12" s="112" t="s">
+      <c r="I12" s="121" t="s">
         <v>100</v>
       </c>
-      <c r="J12" s="113"/>
-      <c r="K12" s="113"/>
-      <c r="L12" s="113"/>
-      <c r="M12" s="113"/>
+      <c r="J12" s="122"/>
+      <c r="K12" s="122"/>
+      <c r="L12" s="122"/>
+      <c r="M12" s="122"/>
     </row>
     <row r="13" spans="2:45" ht="17.25">
       <c r="D13" s="11" t="s">
         <v>104</v>
       </c>
       <c r="H13" s="17"/>
-      <c r="I13" s="112"/>
-      <c r="J13" s="113"/>
-      <c r="K13" s="113"/>
-      <c r="L13" s="113"/>
-      <c r="M13" s="113"/>
+      <c r="I13" s="121"/>
+      <c r="J13" s="122"/>
+      <c r="K13" s="122"/>
+      <c r="L13" s="122"/>
+      <c r="M13" s="122"/>
     </row>
     <row r="14" spans="2:45" ht="17.25">
       <c r="D14" s="13" t="s">
         <v>97</v>
       </c>
       <c r="H14" s="17"/>
-      <c r="I14" s="112"/>
-      <c r="J14" s="113"/>
-      <c r="K14" s="113"/>
-      <c r="L14" s="113"/>
-      <c r="M14" s="113"/>
+      <c r="I14" s="121"/>
+      <c r="J14" s="122"/>
+      <c r="K14" s="122"/>
+      <c r="L14" s="122"/>
+      <c r="M14" s="122"/>
     </row>
     <row r="15" spans="2:45" ht="17.25" customHeight="1">
       <c r="D15" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="I15" s="112"/>
-      <c r="J15" s="113"/>
-      <c r="K15" s="113"/>
-      <c r="L15" s="113"/>
-      <c r="M15" s="113"/>
+      <c r="I15" s="121"/>
+      <c r="J15" s="122"/>
+      <c r="K15" s="122"/>
+      <c r="L15" s="122"/>
+      <c r="M15" s="122"/>
     </row>
     <row r="17" spans="2:43" ht="17.25" customHeight="1">
       <c r="G17" s="18"/>
-      <c r="I17" s="112" t="s">
+      <c r="I17" s="121" t="s">
         <v>102</v>
       </c>
-      <c r="J17" s="113"/>
-      <c r="K17" s="113"/>
-      <c r="L17" s="113"/>
-      <c r="M17" s="113"/>
+      <c r="J17" s="122"/>
+      <c r="K17" s="122"/>
+      <c r="L17" s="122"/>
+      <c r="M17" s="122"/>
     </row>
     <row r="18" spans="2:43" ht="17.25">
       <c r="D18" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="I18" s="112"/>
-      <c r="J18" s="113"/>
-      <c r="K18" s="113"/>
-      <c r="L18" s="113"/>
-      <c r="M18" s="113"/>
+      <c r="I18" s="121"/>
+      <c r="J18" s="122"/>
+      <c r="K18" s="122"/>
+      <c r="L18" s="122"/>
+      <c r="M18" s="122"/>
     </row>
     <row r="19" spans="2:43" ht="15" customHeight="1">
-      <c r="I19" s="112"/>
-      <c r="J19" s="113"/>
-      <c r="K19" s="113"/>
-      <c r="L19" s="113"/>
-      <c r="M19" s="113"/>
+      <c r="I19" s="121"/>
+      <c r="J19" s="122"/>
+      <c r="K19" s="122"/>
+      <c r="L19" s="122"/>
+      <c r="M19" s="122"/>
     </row>
     <row r="22" spans="2:43">
-      <c r="B22" s="118" t="s">
+      <c r="B22" s="125" t="s">
         <v>139</v>
       </c>
-      <c r="C22" s="118"/>
-      <c r="D22" s="118"/>
-      <c r="E22" s="118"/>
-      <c r="F22" s="118"/>
-      <c r="G22" s="118"/>
-      <c r="H22" s="118"/>
-      <c r="I22" s="118"/>
-      <c r="J22" s="118"/>
-      <c r="K22" s="118"/>
-      <c r="L22" s="118"/>
-      <c r="M22" s="118"/>
-      <c r="N22" s="118"/>
-      <c r="O22" s="118"/>
+      <c r="C22" s="125"/>
+      <c r="D22" s="125"/>
+      <c r="E22" s="125"/>
+      <c r="F22" s="125"/>
+      <c r="G22" s="125"/>
+      <c r="H22" s="125"/>
+      <c r="I22" s="125"/>
+      <c r="J22" s="125"/>
+      <c r="K22" s="125"/>
+      <c r="L22" s="125"/>
+      <c r="M22" s="125"/>
+      <c r="N22" s="125"/>
+      <c r="O22" s="125"/>
     </row>
     <row r="23" spans="2:43" ht="15" customHeight="1"/>
     <row r="24" spans="2:43" ht="17.25">
-      <c r="B24" s="117" t="s">
+      <c r="B24" s="111" t="s">
         <v>96</v>
       </c>
-      <c r="C24" s="117"/>
-      <c r="D24" s="117"/>
-      <c r="E24" s="117"/>
-      <c r="F24" s="117"/>
-      <c r="G24" s="117"/>
-      <c r="H24" s="117"/>
-      <c r="I24" s="117"/>
-      <c r="J24" s="117"/>
-      <c r="K24" s="117"/>
-      <c r="L24" s="117"/>
-      <c r="M24" s="117"/>
-      <c r="N24" s="117"/>
-      <c r="O24" s="117"/>
+      <c r="C24" s="111"/>
+      <c r="D24" s="111"/>
+      <c r="E24" s="111"/>
+      <c r="F24" s="111"/>
+      <c r="G24" s="111"/>
+      <c r="H24" s="111"/>
+      <c r="I24" s="111"/>
+      <c r="J24" s="111"/>
+      <c r="K24" s="111"/>
+      <c r="L24" s="111"/>
+      <c r="M24" s="111"/>
+      <c r="N24" s="111"/>
+      <c r="O24" s="111"/>
     </row>
     <row r="25" spans="2:43">
       <c r="R25" s="23"/>
@@ -3137,37 +3157,37 @@
         <v>96</v>
       </c>
       <c r="R26" s="26"/>
-      <c r="S26" s="122" t="s">
+      <c r="S26" s="128" t="s">
         <v>106</v>
       </c>
-      <c r="T26" s="122"/>
-      <c r="U26" s="122"/>
-      <c r="V26" s="122"/>
-      <c r="W26" s="122"/>
-      <c r="X26" s="122"/>
-      <c r="Y26" s="122"/>
-      <c r="Z26" s="122"/>
-      <c r="AA26" s="122"/>
-      <c r="AB26" s="122"/>
+      <c r="T26" s="128"/>
+      <c r="U26" s="128"/>
+      <c r="V26" s="128"/>
+      <c r="W26" s="128"/>
+      <c r="X26" s="128"/>
+      <c r="Y26" s="128"/>
+      <c r="Z26" s="128"/>
+      <c r="AA26" s="128"/>
+      <c r="AB26" s="128"/>
       <c r="AC26" s="27"/>
     </row>
     <row r="27" spans="2:43" ht="15" customHeight="1">
-      <c r="B27" s="109" t="s">
+      <c r="B27" s="116" t="s">
         <v>117</v>
       </c>
-      <c r="C27" s="109"/>
-      <c r="D27" s="109"/>
-      <c r="E27" s="109"/>
-      <c r="F27" s="109"/>
-      <c r="G27" s="109"/>
-      <c r="H27" s="109"/>
-      <c r="I27" s="109"/>
-      <c r="J27" s="109"/>
-      <c r="K27" s="109"/>
-      <c r="L27" s="109"/>
-      <c r="M27" s="109"/>
-      <c r="N27" s="109"/>
-      <c r="O27" s="109"/>
+      <c r="C27" s="116"/>
+      <c r="D27" s="116"/>
+      <c r="E27" s="116"/>
+      <c r="F27" s="116"/>
+      <c r="G27" s="116"/>
+      <c r="H27" s="116"/>
+      <c r="I27" s="116"/>
+      <c r="J27" s="116"/>
+      <c r="K27" s="116"/>
+      <c r="L27" s="116"/>
+      <c r="M27" s="116"/>
+      <c r="N27" s="116"/>
+      <c r="O27" s="116"/>
       <c r="R27" s="26"/>
       <c r="S27" s="24"/>
       <c r="T27" s="24"/>
@@ -3192,51 +3212,51 @@
       <c r="AQ27" s="18"/>
     </row>
     <row r="28" spans="2:43" ht="15" customHeight="1">
-      <c r="B28" s="109"/>
-      <c r="C28" s="109"/>
-      <c r="D28" s="109"/>
-      <c r="E28" s="109"/>
-      <c r="F28" s="109"/>
-      <c r="G28" s="109"/>
-      <c r="H28" s="109"/>
-      <c r="I28" s="109"/>
-      <c r="J28" s="109"/>
-      <c r="K28" s="109"/>
-      <c r="L28" s="109"/>
-      <c r="M28" s="109"/>
-      <c r="N28" s="109"/>
-      <c r="O28" s="109"/>
+      <c r="B28" s="116"/>
+      <c r="C28" s="116"/>
+      <c r="D28" s="116"/>
+      <c r="E28" s="116"/>
+      <c r="F28" s="116"/>
+      <c r="G28" s="116"/>
+      <c r="H28" s="116"/>
+      <c r="I28" s="116"/>
+      <c r="J28" s="116"/>
+      <c r="K28" s="116"/>
+      <c r="L28" s="116"/>
+      <c r="M28" s="116"/>
+      <c r="N28" s="116"/>
+      <c r="O28" s="116"/>
       <c r="R28" s="26"/>
       <c r="AC28" s="27"/>
     </row>
     <row r="29" spans="2:43" ht="17.25">
-      <c r="B29" s="109"/>
-      <c r="C29" s="109"/>
-      <c r="D29" s="109"/>
-      <c r="E29" s="109"/>
-      <c r="F29" s="109"/>
-      <c r="G29" s="109"/>
-      <c r="H29" s="109"/>
-      <c r="I29" s="109"/>
-      <c r="J29" s="109"/>
-      <c r="K29" s="109"/>
-      <c r="L29" s="109"/>
-      <c r="M29" s="109"/>
-      <c r="N29" s="109"/>
-      <c r="O29" s="109"/>
+      <c r="B29" s="116"/>
+      <c r="C29" s="116"/>
+      <c r="D29" s="116"/>
+      <c r="E29" s="116"/>
+      <c r="F29" s="116"/>
+      <c r="G29" s="116"/>
+      <c r="H29" s="116"/>
+      <c r="I29" s="116"/>
+      <c r="J29" s="116"/>
+      <c r="K29" s="116"/>
+      <c r="L29" s="116"/>
+      <c r="M29" s="116"/>
+      <c r="N29" s="116"/>
+      <c r="O29" s="116"/>
       <c r="R29" s="26"/>
-      <c r="S29" s="121" t="s">
+      <c r="S29" s="119" t="s">
         <v>107</v>
       </c>
-      <c r="T29" s="121"/>
-      <c r="U29" s="121"/>
-      <c r="V29" s="121"/>
-      <c r="W29" s="121"/>
-      <c r="X29" s="121"/>
-      <c r="Y29" s="121"/>
-      <c r="Z29" s="121"/>
-      <c r="AA29" s="121"/>
-      <c r="AB29" s="121"/>
+      <c r="T29" s="119"/>
+      <c r="U29" s="119"/>
+      <c r="V29" s="119"/>
+      <c r="W29" s="119"/>
+      <c r="X29" s="119"/>
+      <c r="Y29" s="119"/>
+      <c r="Z29" s="119"/>
+      <c r="AA29" s="119"/>
+      <c r="AB29" s="119"/>
       <c r="AC29" s="27"/>
     </row>
     <row r="30" spans="2:43">
@@ -3254,52 +3274,52 @@
       <c r="AC30" s="27"/>
     </row>
     <row r="31" spans="2:43" ht="17.25">
-      <c r="B31" s="109" t="s">
+      <c r="B31" s="116" t="s">
         <v>140</v>
       </c>
-      <c r="C31" s="109"/>
-      <c r="D31" s="109"/>
-      <c r="E31" s="109"/>
-      <c r="F31" s="109"/>
-      <c r="G31" s="109"/>
-      <c r="H31" s="109"/>
-      <c r="I31" s="109"/>
-      <c r="J31" s="109"/>
-      <c r="K31" s="109"/>
-      <c r="L31" s="109"/>
-      <c r="M31" s="109"/>
-      <c r="N31" s="109"/>
-      <c r="O31" s="109"/>
+      <c r="C31" s="116"/>
+      <c r="D31" s="116"/>
+      <c r="E31" s="116"/>
+      <c r="F31" s="116"/>
+      <c r="G31" s="116"/>
+      <c r="H31" s="116"/>
+      <c r="I31" s="116"/>
+      <c r="J31" s="116"/>
+      <c r="K31" s="116"/>
+      <c r="L31" s="116"/>
+      <c r="M31" s="116"/>
+      <c r="N31" s="116"/>
+      <c r="O31" s="116"/>
       <c r="R31" s="26"/>
       <c r="S31" s="18"/>
       <c r="T31" s="18"/>
       <c r="U31" s="18"/>
-      <c r="V31" s="119" t="s">
+      <c r="V31" s="126" t="s">
         <v>109</v>
       </c>
-      <c r="W31" s="119"/>
-      <c r="X31" s="119"/>
-      <c r="Y31" s="119"/>
-      <c r="Z31" s="119"/>
+      <c r="W31" s="126"/>
+      <c r="X31" s="126"/>
+      <c r="Y31" s="126"/>
+      <c r="Z31" s="126"/>
       <c r="AA31" s="18"/>
       <c r="AB31" s="18"/>
       <c r="AC31" s="27"/>
     </row>
     <row r="32" spans="2:43" ht="15" customHeight="1">
-      <c r="B32" s="109"/>
-      <c r="C32" s="109"/>
-      <c r="D32" s="109"/>
-      <c r="E32" s="109"/>
-      <c r="F32" s="109"/>
-      <c r="G32" s="109"/>
-      <c r="H32" s="109"/>
-      <c r="I32" s="109"/>
-      <c r="J32" s="109"/>
-      <c r="K32" s="109"/>
-      <c r="L32" s="109"/>
-      <c r="M32" s="109"/>
-      <c r="N32" s="109"/>
-      <c r="O32" s="109"/>
+      <c r="B32" s="116"/>
+      <c r="C32" s="116"/>
+      <c r="D32" s="116"/>
+      <c r="E32" s="116"/>
+      <c r="F32" s="116"/>
+      <c r="G32" s="116"/>
+      <c r="H32" s="116"/>
+      <c r="I32" s="116"/>
+      <c r="J32" s="116"/>
+      <c r="K32" s="116"/>
+      <c r="L32" s="116"/>
+      <c r="M32" s="116"/>
+      <c r="N32" s="116"/>
+      <c r="O32" s="116"/>
       <c r="R32" s="26"/>
       <c r="S32" s="18"/>
       <c r="T32" s="18"/>
@@ -3314,61 +3334,61 @@
       <c r="AC32" s="27"/>
     </row>
     <row r="33" spans="2:32" ht="17.25" customHeight="1">
-      <c r="B33" s="109" t="s">
+      <c r="B33" s="116" t="s">
         <v>172</v>
       </c>
-      <c r="C33" s="109"/>
-      <c r="D33" s="109"/>
-      <c r="E33" s="109"/>
-      <c r="F33" s="109"/>
-      <c r="G33" s="109"/>
-      <c r="H33" s="109"/>
-      <c r="I33" s="109"/>
-      <c r="J33" s="109"/>
-      <c r="K33" s="109"/>
-      <c r="L33" s="109"/>
-      <c r="M33" s="109"/>
-      <c r="N33" s="109"/>
+      <c r="C33" s="116"/>
+      <c r="D33" s="116"/>
+      <c r="E33" s="116"/>
+      <c r="F33" s="116"/>
+      <c r="G33" s="116"/>
+      <c r="H33" s="116"/>
+      <c r="I33" s="116"/>
+      <c r="J33" s="116"/>
+      <c r="K33" s="116"/>
+      <c r="L33" s="116"/>
+      <c r="M33" s="116"/>
+      <c r="N33" s="116"/>
       <c r="R33" s="26"/>
-      <c r="S33" s="123" t="s">
+      <c r="S33" s="117" t="s">
         <v>108</v>
       </c>
-      <c r="T33" s="123"/>
-      <c r="U33" s="123"/>
-      <c r="V33" s="123"/>
-      <c r="W33" s="123"/>
-      <c r="X33" s="123"/>
-      <c r="Y33" s="123"/>
-      <c r="Z33" s="123"/>
-      <c r="AA33" s="123"/>
-      <c r="AB33" s="123"/>
+      <c r="T33" s="117"/>
+      <c r="U33" s="117"/>
+      <c r="V33" s="117"/>
+      <c r="W33" s="117"/>
+      <c r="X33" s="117"/>
+      <c r="Y33" s="117"/>
+      <c r="Z33" s="117"/>
+      <c r="AA33" s="117"/>
+      <c r="AB33" s="117"/>
       <c r="AC33" s="27"/>
     </row>
     <row r="34" spans="2:32" ht="17.25" customHeight="1">
-      <c r="B34" s="109"/>
-      <c r="C34" s="109"/>
-      <c r="D34" s="109"/>
-      <c r="E34" s="109"/>
-      <c r="F34" s="109"/>
-      <c r="G34" s="109"/>
-      <c r="H34" s="109"/>
-      <c r="I34" s="109"/>
-      <c r="J34" s="109"/>
-      <c r="K34" s="109"/>
-      <c r="L34" s="109"/>
-      <c r="M34" s="109"/>
-      <c r="N34" s="109"/>
+      <c r="B34" s="116"/>
+      <c r="C34" s="116"/>
+      <c r="D34" s="116"/>
+      <c r="E34" s="116"/>
+      <c r="F34" s="116"/>
+      <c r="G34" s="116"/>
+      <c r="H34" s="116"/>
+      <c r="I34" s="116"/>
+      <c r="J34" s="116"/>
+      <c r="K34" s="116"/>
+      <c r="L34" s="116"/>
+      <c r="M34" s="116"/>
+      <c r="N34" s="116"/>
       <c r="R34" s="26"/>
-      <c r="S34" s="123"/>
-      <c r="T34" s="123"/>
-      <c r="U34" s="123"/>
-      <c r="V34" s="123"/>
-      <c r="W34" s="123"/>
-      <c r="X34" s="123"/>
-      <c r="Y34" s="123"/>
-      <c r="Z34" s="123"/>
-      <c r="AA34" s="123"/>
-      <c r="AB34" s="123"/>
+      <c r="S34" s="117"/>
+      <c r="T34" s="117"/>
+      <c r="U34" s="117"/>
+      <c r="V34" s="117"/>
+      <c r="W34" s="117"/>
+      <c r="X34" s="117"/>
+      <c r="Y34" s="117"/>
+      <c r="Z34" s="117"/>
+      <c r="AA34" s="117"/>
+      <c r="AB34" s="117"/>
       <c r="AC34" s="27"/>
     </row>
     <row r="35" spans="2:32">
@@ -3406,67 +3426,67 @@
     </row>
     <row r="37" spans="2:32">
       <c r="R37" s="26"/>
-      <c r="S37" s="124" t="s">
+      <c r="S37" s="118" t="s">
         <v>111</v>
       </c>
-      <c r="T37" s="124"/>
-      <c r="U37" s="124"/>
-      <c r="V37" s="124"/>
-      <c r="W37" s="124"/>
-      <c r="X37" s="124"/>
-      <c r="Y37" s="124"/>
-      <c r="Z37" s="124"/>
-      <c r="AA37" s="124"/>
-      <c r="AB37" s="124"/>
+      <c r="T37" s="118"/>
+      <c r="U37" s="118"/>
+      <c r="V37" s="118"/>
+      <c r="W37" s="118"/>
+      <c r="X37" s="118"/>
+      <c r="Y37" s="118"/>
+      <c r="Z37" s="118"/>
+      <c r="AA37" s="118"/>
+      <c r="AB37" s="118"/>
       <c r="AC37" s="27"/>
       <c r="AF37" s="9"/>
     </row>
     <row r="38" spans="2:32">
-      <c r="B38" s="109" t="s">
+      <c r="B38" s="116" t="s">
         <v>142</v>
       </c>
-      <c r="C38" s="109"/>
-      <c r="D38" s="109"/>
-      <c r="E38" s="109"/>
-      <c r="F38" s="109"/>
-      <c r="G38" s="109"/>
-      <c r="H38" s="109"/>
-      <c r="I38" s="109"/>
-      <c r="J38" s="109"/>
-      <c r="K38" s="109"/>
-      <c r="L38" s="109"/>
-      <c r="M38" s="109"/>
-      <c r="N38" s="109"/>
-      <c r="O38" s="109"/>
+      <c r="C38" s="116"/>
+      <c r="D38" s="116"/>
+      <c r="E38" s="116"/>
+      <c r="F38" s="116"/>
+      <c r="G38" s="116"/>
+      <c r="H38" s="116"/>
+      <c r="I38" s="116"/>
+      <c r="J38" s="116"/>
+      <c r="K38" s="116"/>
+      <c r="L38" s="116"/>
+      <c r="M38" s="116"/>
+      <c r="N38" s="116"/>
+      <c r="O38" s="116"/>
       <c r="R38" s="26"/>
-      <c r="S38" s="124"/>
-      <c r="T38" s="124"/>
-      <c r="U38" s="124"/>
-      <c r="V38" s="124"/>
-      <c r="W38" s="124"/>
-      <c r="X38" s="124"/>
-      <c r="Y38" s="124"/>
-      <c r="Z38" s="124"/>
-      <c r="AA38" s="124"/>
-      <c r="AB38" s="124"/>
+      <c r="S38" s="118"/>
+      <c r="T38" s="118"/>
+      <c r="U38" s="118"/>
+      <c r="V38" s="118"/>
+      <c r="W38" s="118"/>
+      <c r="X38" s="118"/>
+      <c r="Y38" s="118"/>
+      <c r="Z38" s="118"/>
+      <c r="AA38" s="118"/>
+      <c r="AB38" s="118"/>
       <c r="AC38" s="27"/>
       <c r="AF38" s="9"/>
     </row>
     <row r="39" spans="2:32">
-      <c r="B39" s="109"/>
-      <c r="C39" s="109"/>
-      <c r="D39" s="109"/>
-      <c r="E39" s="109"/>
-      <c r="F39" s="109"/>
-      <c r="G39" s="109"/>
-      <c r="H39" s="109"/>
-      <c r="I39" s="109"/>
-      <c r="J39" s="109"/>
-      <c r="K39" s="109"/>
-      <c r="L39" s="109"/>
-      <c r="M39" s="109"/>
-      <c r="N39" s="109"/>
-      <c r="O39" s="109"/>
+      <c r="B39" s="116"/>
+      <c r="C39" s="116"/>
+      <c r="D39" s="116"/>
+      <c r="E39" s="116"/>
+      <c r="F39" s="116"/>
+      <c r="G39" s="116"/>
+      <c r="H39" s="116"/>
+      <c r="I39" s="116"/>
+      <c r="J39" s="116"/>
+      <c r="K39" s="116"/>
+      <c r="L39" s="116"/>
+      <c r="M39" s="116"/>
+      <c r="N39" s="116"/>
+      <c r="O39" s="116"/>
       <c r="R39" s="26"/>
       <c r="S39" s="18"/>
       <c r="T39" s="19"/>
@@ -3486,34 +3506,34 @@
       <c r="S40" s="18"/>
       <c r="T40" s="19"/>
       <c r="U40" s="19"/>
-      <c r="V40" s="120" t="s">
+      <c r="V40" s="127" t="s">
         <v>110</v>
       </c>
-      <c r="W40" s="120"/>
-      <c r="X40" s="120"/>
-      <c r="Y40" s="120"/>
-      <c r="Z40" s="120"/>
+      <c r="W40" s="127"/>
+      <c r="X40" s="127"/>
+      <c r="Y40" s="127"/>
+      <c r="Z40" s="127"/>
       <c r="AA40" s="19"/>
       <c r="AB40" s="19"/>
       <c r="AC40" s="27"/>
     </row>
     <row r="41" spans="2:32" ht="17.25">
-      <c r="B41" s="117" t="s">
+      <c r="B41" s="111" t="s">
         <v>104</v>
       </c>
-      <c r="C41" s="117"/>
-      <c r="D41" s="117"/>
-      <c r="E41" s="117"/>
-      <c r="F41" s="117"/>
-      <c r="G41" s="117"/>
-      <c r="H41" s="117"/>
-      <c r="I41" s="117"/>
-      <c r="J41" s="117"/>
-      <c r="K41" s="117"/>
-      <c r="L41" s="117"/>
-      <c r="M41" s="117"/>
-      <c r="N41" s="117"/>
-      <c r="O41" s="117"/>
+      <c r="C41" s="111"/>
+      <c r="D41" s="111"/>
+      <c r="E41" s="111"/>
+      <c r="F41" s="111"/>
+      <c r="G41" s="111"/>
+      <c r="H41" s="111"/>
+      <c r="I41" s="111"/>
+      <c r="J41" s="111"/>
+      <c r="K41" s="111"/>
+      <c r="L41" s="111"/>
+      <c r="M41" s="111"/>
+      <c r="N41" s="111"/>
+      <c r="O41" s="111"/>
       <c r="R41" s="26"/>
       <c r="S41" s="18"/>
       <c r="T41" s="18"/>
@@ -3529,18 +3549,18 @@
     </row>
     <row r="42" spans="2:32" ht="17.25">
       <c r="R42" s="26"/>
-      <c r="S42" s="121" t="s">
+      <c r="S42" s="119" t="s">
         <v>112</v>
       </c>
-      <c r="T42" s="121"/>
-      <c r="U42" s="121"/>
-      <c r="V42" s="121"/>
-      <c r="W42" s="121"/>
-      <c r="X42" s="121"/>
-      <c r="Y42" s="121"/>
-      <c r="Z42" s="121"/>
-      <c r="AA42" s="121"/>
-      <c r="AB42" s="121"/>
+      <c r="T42" s="119"/>
+      <c r="U42" s="119"/>
+      <c r="V42" s="119"/>
+      <c r="W42" s="119"/>
+      <c r="X42" s="119"/>
+      <c r="Y42" s="119"/>
+      <c r="Z42" s="119"/>
+      <c r="AA42" s="119"/>
+      <c r="AB42" s="119"/>
       <c r="AC42" s="27"/>
     </row>
     <row r="43" spans="2:32" ht="17.25">
@@ -3575,63 +3595,63 @@
       <c r="AC44" s="27"/>
     </row>
     <row r="45" spans="2:32">
-      <c r="B45" s="109" t="s">
+      <c r="B45" s="116" t="s">
         <v>143</v>
       </c>
-      <c r="C45" s="109"/>
-      <c r="D45" s="109"/>
-      <c r="E45" s="109"/>
-      <c r="F45" s="109"/>
-      <c r="G45" s="109"/>
-      <c r="H45" s="109"/>
-      <c r="I45" s="109"/>
-      <c r="J45" s="109"/>
-      <c r="K45" s="109"/>
-      <c r="L45" s="109"/>
-      <c r="M45" s="109"/>
-      <c r="N45" s="109"/>
-      <c r="O45" s="109"/>
+      <c r="C45" s="116"/>
+      <c r="D45" s="116"/>
+      <c r="E45" s="116"/>
+      <c r="F45" s="116"/>
+      <c r="G45" s="116"/>
+      <c r="H45" s="116"/>
+      <c r="I45" s="116"/>
+      <c r="J45" s="116"/>
+      <c r="K45" s="116"/>
+      <c r="L45" s="116"/>
+      <c r="M45" s="116"/>
+      <c r="N45" s="116"/>
+      <c r="O45" s="116"/>
       <c r="R45" s="26"/>
-      <c r="S45" s="123" t="s">
+      <c r="S45" s="117" t="s">
         <v>113</v>
       </c>
-      <c r="T45" s="123"/>
-      <c r="U45" s="123"/>
-      <c r="V45" s="123"/>
-      <c r="W45" s="123"/>
-      <c r="X45" s="123"/>
-      <c r="Y45" s="123"/>
-      <c r="Z45" s="123"/>
-      <c r="AA45" s="123"/>
-      <c r="AB45" s="123"/>
+      <c r="T45" s="117"/>
+      <c r="U45" s="117"/>
+      <c r="V45" s="117"/>
+      <c r="W45" s="117"/>
+      <c r="X45" s="117"/>
+      <c r="Y45" s="117"/>
+      <c r="Z45" s="117"/>
+      <c r="AA45" s="117"/>
+      <c r="AB45" s="117"/>
       <c r="AC45" s="27"/>
     </row>
     <row r="46" spans="2:32" ht="15" customHeight="1">
-      <c r="B46" s="109"/>
-      <c r="C46" s="109"/>
-      <c r="D46" s="109"/>
-      <c r="E46" s="109"/>
-      <c r="F46" s="109"/>
-      <c r="G46" s="109"/>
-      <c r="H46" s="109"/>
-      <c r="I46" s="109"/>
-      <c r="J46" s="109"/>
-      <c r="K46" s="109"/>
-      <c r="L46" s="109"/>
-      <c r="M46" s="109"/>
-      <c r="N46" s="109"/>
-      <c r="O46" s="109"/>
+      <c r="B46" s="116"/>
+      <c r="C46" s="116"/>
+      <c r="D46" s="116"/>
+      <c r="E46" s="116"/>
+      <c r="F46" s="116"/>
+      <c r="G46" s="116"/>
+      <c r="H46" s="116"/>
+      <c r="I46" s="116"/>
+      <c r="J46" s="116"/>
+      <c r="K46" s="116"/>
+      <c r="L46" s="116"/>
+      <c r="M46" s="116"/>
+      <c r="N46" s="116"/>
+      <c r="O46" s="116"/>
       <c r="R46" s="26"/>
-      <c r="S46" s="123"/>
-      <c r="T46" s="123"/>
-      <c r="U46" s="123"/>
-      <c r="V46" s="123"/>
-      <c r="W46" s="123"/>
-      <c r="X46" s="123"/>
-      <c r="Y46" s="123"/>
-      <c r="Z46" s="123"/>
-      <c r="AA46" s="123"/>
-      <c r="AB46" s="123"/>
+      <c r="S46" s="117"/>
+      <c r="T46" s="117"/>
+      <c r="U46" s="117"/>
+      <c r="V46" s="117"/>
+      <c r="W46" s="117"/>
+      <c r="X46" s="117"/>
+      <c r="Y46" s="117"/>
+      <c r="Z46" s="117"/>
+      <c r="AA46" s="117"/>
+      <c r="AB46" s="117"/>
       <c r="AC46" s="27"/>
     </row>
     <row r="47" spans="2:32" ht="15" customHeight="1">
@@ -3656,13 +3676,13 @@
       <c r="S48" s="18"/>
       <c r="T48" s="18"/>
       <c r="U48" s="18"/>
-      <c r="V48" s="126" t="s">
+      <c r="V48" s="114" t="s">
         <v>114</v>
       </c>
-      <c r="W48" s="126"/>
-      <c r="X48" s="126"/>
-      <c r="Y48" s="126"/>
-      <c r="Z48" s="126"/>
+      <c r="W48" s="114"/>
+      <c r="X48" s="114"/>
+      <c r="Y48" s="114"/>
+      <c r="Z48" s="114"/>
       <c r="AA48" s="18"/>
       <c r="AB48" s="18"/>
       <c r="AC48" s="27"/>
@@ -3682,52 +3702,52 @@
       <c r="AC49" s="27"/>
     </row>
     <row r="50" spans="2:43">
-      <c r="B50" s="109" t="s">
+      <c r="B50" s="116" t="s">
         <v>145</v>
       </c>
-      <c r="C50" s="109"/>
-      <c r="D50" s="109"/>
-      <c r="E50" s="109"/>
-      <c r="F50" s="109"/>
-      <c r="G50" s="109"/>
-      <c r="H50" s="109"/>
-      <c r="I50" s="109"/>
-      <c r="J50" s="109"/>
-      <c r="K50" s="109"/>
-      <c r="L50" s="109"/>
-      <c r="M50" s="109"/>
-      <c r="N50" s="109"/>
-      <c r="O50" s="109"/>
+      <c r="C50" s="116"/>
+      <c r="D50" s="116"/>
+      <c r="E50" s="116"/>
+      <c r="F50" s="116"/>
+      <c r="G50" s="116"/>
+      <c r="H50" s="116"/>
+      <c r="I50" s="116"/>
+      <c r="J50" s="116"/>
+      <c r="K50" s="116"/>
+      <c r="L50" s="116"/>
+      <c r="M50" s="116"/>
+      <c r="N50" s="116"/>
+      <c r="O50" s="116"/>
       <c r="R50" s="26"/>
-      <c r="S50" s="114" t="s">
+      <c r="S50" s="115" t="s">
         <v>115</v>
       </c>
-      <c r="T50" s="114"/>
-      <c r="U50" s="114"/>
-      <c r="V50" s="114"/>
-      <c r="W50" s="114"/>
-      <c r="X50" s="114"/>
-      <c r="Y50" s="114"/>
-      <c r="Z50" s="114"/>
-      <c r="AA50" s="114"/>
-      <c r="AB50" s="114"/>
+      <c r="T50" s="115"/>
+      <c r="U50" s="115"/>
+      <c r="V50" s="115"/>
+      <c r="W50" s="115"/>
+      <c r="X50" s="115"/>
+      <c r="Y50" s="115"/>
+      <c r="Z50" s="115"/>
+      <c r="AA50" s="115"/>
+      <c r="AB50" s="115"/>
       <c r="AC50" s="27"/>
     </row>
     <row r="51" spans="2:43" ht="15" customHeight="1">
-      <c r="B51" s="109"/>
-      <c r="C51" s="109"/>
-      <c r="D51" s="109"/>
-      <c r="E51" s="109"/>
-      <c r="F51" s="109"/>
-      <c r="G51" s="109"/>
-      <c r="H51" s="109"/>
-      <c r="I51" s="109"/>
-      <c r="J51" s="109"/>
-      <c r="K51" s="109"/>
-      <c r="L51" s="109"/>
-      <c r="M51" s="109"/>
-      <c r="N51" s="109"/>
-      <c r="O51" s="109"/>
+      <c r="B51" s="116"/>
+      <c r="C51" s="116"/>
+      <c r="D51" s="116"/>
+      <c r="E51" s="116"/>
+      <c r="F51" s="116"/>
+      <c r="G51" s="116"/>
+      <c r="H51" s="116"/>
+      <c r="I51" s="116"/>
+      <c r="J51" s="116"/>
+      <c r="K51" s="116"/>
+      <c r="L51" s="116"/>
+      <c r="M51" s="116"/>
+      <c r="N51" s="116"/>
+      <c r="O51" s="116"/>
       <c r="R51" s="26"/>
       <c r="S51" s="18"/>
       <c r="T51" s="18"/>
@@ -3743,18 +3763,18 @@
     </row>
     <row r="52" spans="2:43">
       <c r="R52" s="26"/>
-      <c r="S52" s="114" t="s">
+      <c r="S52" s="115" t="s">
         <v>116</v>
       </c>
-      <c r="T52" s="114"/>
-      <c r="U52" s="114"/>
-      <c r="V52" s="114"/>
-      <c r="W52" s="114"/>
-      <c r="X52" s="114"/>
-      <c r="Y52" s="114"/>
-      <c r="Z52" s="114"/>
-      <c r="AA52" s="114"/>
-      <c r="AB52" s="114"/>
+      <c r="T52" s="115"/>
+      <c r="U52" s="115"/>
+      <c r="V52" s="115"/>
+      <c r="W52" s="115"/>
+      <c r="X52" s="115"/>
+      <c r="Y52" s="115"/>
+      <c r="Z52" s="115"/>
+      <c r="AA52" s="115"/>
+      <c r="AB52" s="115"/>
       <c r="AC52" s="27"/>
     </row>
     <row r="53" spans="2:43" ht="15.75" customHeight="1">
@@ -3762,16 +3782,16 @@
         <v>147</v>
       </c>
       <c r="R53" s="26"/>
-      <c r="S53" s="114"/>
-      <c r="T53" s="114"/>
-      <c r="U53" s="114"/>
-      <c r="V53" s="114"/>
-      <c r="W53" s="114"/>
-      <c r="X53" s="114"/>
-      <c r="Y53" s="114"/>
-      <c r="Z53" s="114"/>
-      <c r="AA53" s="114"/>
-      <c r="AB53" s="114"/>
+      <c r="S53" s="115"/>
+      <c r="T53" s="115"/>
+      <c r="U53" s="115"/>
+      <c r="V53" s="115"/>
+      <c r="W53" s="115"/>
+      <c r="X53" s="115"/>
+      <c r="Y53" s="115"/>
+      <c r="Z53" s="115"/>
+      <c r="AA53" s="115"/>
+      <c r="AB53" s="115"/>
       <c r="AC53" s="27"/>
       <c r="AH53" s="22"/>
       <c r="AI53" s="22"/>
@@ -3799,22 +3819,22 @@
       <c r="AC54" s="27"/>
     </row>
     <row r="55" spans="2:43">
-      <c r="B55" s="109" t="s">
+      <c r="B55" s="116" t="s">
         <v>154</v>
       </c>
-      <c r="C55" s="109"/>
-      <c r="D55" s="109"/>
-      <c r="E55" s="109"/>
-      <c r="F55" s="109"/>
-      <c r="G55" s="109"/>
-      <c r="H55" s="109"/>
-      <c r="I55" s="109"/>
-      <c r="J55" s="109"/>
-      <c r="K55" s="109"/>
-      <c r="L55" s="109"/>
-      <c r="M55" s="109"/>
-      <c r="N55" s="109"/>
-      <c r="O55" s="109"/>
+      <c r="C55" s="116"/>
+      <c r="D55" s="116"/>
+      <c r="E55" s="116"/>
+      <c r="F55" s="116"/>
+      <c r="G55" s="116"/>
+      <c r="H55" s="116"/>
+      <c r="I55" s="116"/>
+      <c r="J55" s="116"/>
+      <c r="K55" s="116"/>
+      <c r="L55" s="116"/>
+      <c r="M55" s="116"/>
+      <c r="N55" s="116"/>
+      <c r="O55" s="116"/>
       <c r="R55" s="28"/>
       <c r="S55" s="29"/>
       <c r="T55" s="29"/>
@@ -3829,272 +3849,272 @@
       <c r="AC55" s="30"/>
     </row>
     <row r="56" spans="2:43">
-      <c r="B56" s="109"/>
-      <c r="C56" s="109"/>
-      <c r="D56" s="109"/>
-      <c r="E56" s="109"/>
-      <c r="F56" s="109"/>
-      <c r="G56" s="109"/>
-      <c r="H56" s="109"/>
-      <c r="I56" s="109"/>
-      <c r="J56" s="109"/>
-      <c r="K56" s="109"/>
-      <c r="L56" s="109"/>
-      <c r="M56" s="109"/>
-      <c r="N56" s="109"/>
-      <c r="O56" s="109"/>
+      <c r="B56" s="116"/>
+      <c r="C56" s="116"/>
+      <c r="D56" s="116"/>
+      <c r="E56" s="116"/>
+      <c r="F56" s="116"/>
+      <c r="G56" s="116"/>
+      <c r="H56" s="116"/>
+      <c r="I56" s="116"/>
+      <c r="J56" s="116"/>
+      <c r="K56" s="116"/>
+      <c r="L56" s="116"/>
+      <c r="M56" s="116"/>
+      <c r="N56" s="116"/>
+      <c r="O56" s="116"/>
     </row>
     <row r="58" spans="2:43" ht="17.25">
-      <c r="B58" s="117" t="s">
+      <c r="B58" s="111" t="s">
         <v>97</v>
       </c>
-      <c r="C58" s="117"/>
-      <c r="D58" s="117"/>
-      <c r="E58" s="117"/>
-      <c r="F58" s="117"/>
-      <c r="G58" s="117"/>
-      <c r="H58" s="117"/>
-      <c r="I58" s="117"/>
-      <c r="J58" s="117"/>
-      <c r="K58" s="117"/>
-      <c r="L58" s="117"/>
-      <c r="M58" s="117"/>
-      <c r="N58" s="117"/>
-      <c r="O58" s="117"/>
-      <c r="Q58" s="125" t="s">
+      <c r="C58" s="111"/>
+      <c r="D58" s="111"/>
+      <c r="E58" s="111"/>
+      <c r="F58" s="111"/>
+      <c r="G58" s="111"/>
+      <c r="H58" s="111"/>
+      <c r="I58" s="111"/>
+      <c r="J58" s="111"/>
+      <c r="K58" s="111"/>
+      <c r="L58" s="111"/>
+      <c r="M58" s="111"/>
+      <c r="N58" s="111"/>
+      <c r="O58" s="111"/>
+      <c r="Q58" s="112" t="s">
         <v>169</v>
       </c>
-      <c r="R58" s="125"/>
-      <c r="S58" s="125"/>
-      <c r="T58" s="125"/>
-      <c r="U58" s="125"/>
-      <c r="V58" s="125"/>
-      <c r="W58" s="125"/>
-      <c r="X58" s="125"/>
-      <c r="Y58" s="125"/>
-      <c r="Z58" s="125"/>
-      <c r="AA58" s="125"/>
-      <c r="AB58" s="125"/>
-      <c r="AC58" s="125"/>
-      <c r="AD58" s="125"/>
+      <c r="R58" s="112"/>
+      <c r="S58" s="112"/>
+      <c r="T58" s="112"/>
+      <c r="U58" s="112"/>
+      <c r="V58" s="112"/>
+      <c r="W58" s="112"/>
+      <c r="X58" s="112"/>
+      <c r="Y58" s="112"/>
+      <c r="Z58" s="112"/>
+      <c r="AA58" s="112"/>
+      <c r="AB58" s="112"/>
+      <c r="AC58" s="112"/>
+      <c r="AD58" s="112"/>
     </row>
     <row r="60" spans="2:43" ht="17.25">
-      <c r="B60" s="110" t="s">
+      <c r="B60" s="113" t="s">
         <v>198</v>
       </c>
-      <c r="C60" s="110"/>
-      <c r="D60" s="110"/>
-      <c r="E60" s="110"/>
-      <c r="F60" s="110"/>
-      <c r="G60" s="110"/>
-      <c r="H60" s="110"/>
-      <c r="I60" s="110"/>
-      <c r="J60" s="110"/>
-      <c r="K60" s="110"/>
-      <c r="L60" s="110"/>
-      <c r="M60" s="110"/>
-      <c r="N60" s="110"/>
-      <c r="O60" s="110"/>
+      <c r="C60" s="113"/>
+      <c r="D60" s="113"/>
+      <c r="E60" s="113"/>
+      <c r="F60" s="113"/>
+      <c r="G60" s="113"/>
+      <c r="H60" s="113"/>
+      <c r="I60" s="113"/>
+      <c r="J60" s="113"/>
+      <c r="K60" s="113"/>
+      <c r="L60" s="113"/>
+      <c r="M60" s="113"/>
+      <c r="N60" s="113"/>
+      <c r="O60" s="113"/>
       <c r="Q60" s="20" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="61" spans="2:43">
-      <c r="B61" s="110"/>
-      <c r="C61" s="110"/>
-      <c r="D61" s="110"/>
-      <c r="E61" s="110"/>
-      <c r="F61" s="110"/>
-      <c r="G61" s="110"/>
-      <c r="H61" s="110"/>
-      <c r="I61" s="110"/>
-      <c r="J61" s="110"/>
-      <c r="K61" s="110"/>
-      <c r="L61" s="110"/>
-      <c r="M61" s="110"/>
-      <c r="N61" s="110"/>
-      <c r="O61" s="110"/>
+      <c r="B61" s="113"/>
+      <c r="C61" s="113"/>
+      <c r="D61" s="113"/>
+      <c r="E61" s="113"/>
+      <c r="F61" s="113"/>
+      <c r="G61" s="113"/>
+      <c r="H61" s="113"/>
+      <c r="I61" s="113"/>
+      <c r="J61" s="113"/>
+      <c r="K61" s="113"/>
+      <c r="L61" s="113"/>
+      <c r="M61" s="113"/>
+      <c r="N61" s="113"/>
+      <c r="O61" s="113"/>
     </row>
     <row r="62" spans="2:43">
-      <c r="Q62" s="109" t="s">
+      <c r="Q62" s="116" t="s">
         <v>195</v>
       </c>
-      <c r="R62" s="109"/>
-      <c r="S62" s="109"/>
-      <c r="T62" s="109"/>
-      <c r="U62" s="109"/>
-      <c r="V62" s="109"/>
-      <c r="W62" s="109"/>
-      <c r="X62" s="109"/>
-      <c r="Y62" s="109"/>
-      <c r="Z62" s="109"/>
-      <c r="AA62" s="109"/>
-      <c r="AB62" s="109"/>
-      <c r="AC62" s="109"/>
-      <c r="AD62" s="109"/>
+      <c r="R62" s="116"/>
+      <c r="S62" s="116"/>
+      <c r="T62" s="116"/>
+      <c r="U62" s="116"/>
+      <c r="V62" s="116"/>
+      <c r="W62" s="116"/>
+      <c r="X62" s="116"/>
+      <c r="Y62" s="116"/>
+      <c r="Z62" s="116"/>
+      <c r="AA62" s="116"/>
+      <c r="AB62" s="116"/>
+      <c r="AC62" s="116"/>
+      <c r="AD62" s="116"/>
     </row>
     <row r="63" spans="2:43" ht="15" customHeight="1">
-      <c r="B63" s="110" t="s">
+      <c r="B63" s="113" t="s">
         <v>213</v>
       </c>
-      <c r="C63" s="110"/>
-      <c r="D63" s="110"/>
-      <c r="E63" s="110"/>
-      <c r="F63" s="110"/>
-      <c r="G63" s="110"/>
-      <c r="H63" s="110"/>
-      <c r="I63" s="110"/>
-      <c r="J63" s="110"/>
-      <c r="K63" s="110"/>
-      <c r="L63" s="110"/>
-      <c r="M63" s="110"/>
-      <c r="N63" s="110"/>
-      <c r="O63" s="110"/>
-      <c r="Q63" s="109"/>
-      <c r="R63" s="109"/>
-      <c r="S63" s="109"/>
-      <c r="T63" s="109"/>
-      <c r="U63" s="109"/>
-      <c r="V63" s="109"/>
-      <c r="W63" s="109"/>
-      <c r="X63" s="109"/>
-      <c r="Y63" s="109"/>
-      <c r="Z63" s="109"/>
-      <c r="AA63" s="109"/>
-      <c r="AB63" s="109"/>
-      <c r="AC63" s="109"/>
-      <c r="AD63" s="109"/>
+      <c r="C63" s="113"/>
+      <c r="D63" s="113"/>
+      <c r="E63" s="113"/>
+      <c r="F63" s="113"/>
+      <c r="G63" s="113"/>
+      <c r="H63" s="113"/>
+      <c r="I63" s="113"/>
+      <c r="J63" s="113"/>
+      <c r="K63" s="113"/>
+      <c r="L63" s="113"/>
+      <c r="M63" s="113"/>
+      <c r="N63" s="113"/>
+      <c r="O63" s="113"/>
+      <c r="Q63" s="116"/>
+      <c r="R63" s="116"/>
+      <c r="S63" s="116"/>
+      <c r="T63" s="116"/>
+      <c r="U63" s="116"/>
+      <c r="V63" s="116"/>
+      <c r="W63" s="116"/>
+      <c r="X63" s="116"/>
+      <c r="Y63" s="116"/>
+      <c r="Z63" s="116"/>
+      <c r="AA63" s="116"/>
+      <c r="AB63" s="116"/>
+      <c r="AC63" s="116"/>
+      <c r="AD63" s="116"/>
     </row>
     <row r="64" spans="2:43">
-      <c r="B64" s="110"/>
-      <c r="C64" s="110"/>
-      <c r="D64" s="110"/>
-      <c r="E64" s="110"/>
-      <c r="F64" s="110"/>
-      <c r="G64" s="110"/>
-      <c r="H64" s="110"/>
-      <c r="I64" s="110"/>
-      <c r="J64" s="110"/>
-      <c r="K64" s="110"/>
-      <c r="L64" s="110"/>
-      <c r="M64" s="110"/>
-      <c r="N64" s="110"/>
-      <c r="O64" s="110"/>
+      <c r="B64" s="113"/>
+      <c r="C64" s="113"/>
+      <c r="D64" s="113"/>
+      <c r="E64" s="113"/>
+      <c r="F64" s="113"/>
+      <c r="G64" s="113"/>
+      <c r="H64" s="113"/>
+      <c r="I64" s="113"/>
+      <c r="J64" s="113"/>
+      <c r="K64" s="113"/>
+      <c r="L64" s="113"/>
+      <c r="M64" s="113"/>
+      <c r="N64" s="113"/>
+      <c r="O64" s="113"/>
     </row>
     <row r="65" spans="2:30" ht="17.25">
-      <c r="B65" s="110"/>
-      <c r="C65" s="110"/>
-      <c r="D65" s="110"/>
-      <c r="E65" s="110"/>
-      <c r="F65" s="110"/>
-      <c r="G65" s="110"/>
-      <c r="H65" s="110"/>
-      <c r="I65" s="110"/>
-      <c r="J65" s="110"/>
-      <c r="K65" s="110"/>
-      <c r="L65" s="110"/>
-      <c r="M65" s="110"/>
-      <c r="N65" s="110"/>
-      <c r="O65" s="110"/>
+      <c r="B65" s="113"/>
+      <c r="C65" s="113"/>
+      <c r="D65" s="113"/>
+      <c r="E65" s="113"/>
+      <c r="F65" s="113"/>
+      <c r="G65" s="113"/>
+      <c r="H65" s="113"/>
+      <c r="I65" s="113"/>
+      <c r="J65" s="113"/>
+      <c r="K65" s="113"/>
+      <c r="L65" s="113"/>
+      <c r="M65" s="113"/>
+      <c r="N65" s="113"/>
+      <c r="O65" s="113"/>
       <c r="Q65" s="20" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="66" spans="2:30">
-      <c r="B66" s="110"/>
-      <c r="C66" s="110"/>
-      <c r="D66" s="110"/>
-      <c r="E66" s="110"/>
-      <c r="F66" s="110"/>
-      <c r="G66" s="110"/>
-      <c r="H66" s="110"/>
-      <c r="I66" s="110"/>
-      <c r="J66" s="110"/>
-      <c r="K66" s="110"/>
-      <c r="L66" s="110"/>
-      <c r="M66" s="110"/>
-      <c r="N66" s="110"/>
-      <c r="O66" s="110"/>
+      <c r="B66" s="113"/>
+      <c r="C66" s="113"/>
+      <c r="D66" s="113"/>
+      <c r="E66" s="113"/>
+      <c r="F66" s="113"/>
+      <c r="G66" s="113"/>
+      <c r="H66" s="113"/>
+      <c r="I66" s="113"/>
+      <c r="J66" s="113"/>
+      <c r="K66" s="113"/>
+      <c r="L66" s="113"/>
+      <c r="M66" s="113"/>
+      <c r="N66" s="113"/>
+      <c r="O66" s="113"/>
     </row>
     <row r="67" spans="2:30" ht="15" customHeight="1">
-      <c r="B67" s="109" t="s">
+      <c r="B67" s="116" t="s">
         <v>200</v>
       </c>
-      <c r="C67" s="109"/>
-      <c r="D67" s="109"/>
-      <c r="E67" s="109"/>
-      <c r="F67" s="109"/>
-      <c r="G67" s="109"/>
-      <c r="H67" s="109"/>
-      <c r="I67" s="109"/>
-      <c r="J67" s="109"/>
-      <c r="K67" s="109"/>
-      <c r="L67" s="109"/>
-      <c r="M67" s="109"/>
-      <c r="N67" s="109"/>
-      <c r="O67" s="109"/>
-      <c r="Q67" s="109" t="s">
+      <c r="C67" s="116"/>
+      <c r="D67" s="116"/>
+      <c r="E67" s="116"/>
+      <c r="F67" s="116"/>
+      <c r="G67" s="116"/>
+      <c r="H67" s="116"/>
+      <c r="I67" s="116"/>
+      <c r="J67" s="116"/>
+      <c r="K67" s="116"/>
+      <c r="L67" s="116"/>
+      <c r="M67" s="116"/>
+      <c r="N67" s="116"/>
+      <c r="O67" s="116"/>
+      <c r="Q67" s="116" t="s">
         <v>209</v>
       </c>
-      <c r="R67" s="109"/>
-      <c r="S67" s="109"/>
-      <c r="T67" s="109"/>
-      <c r="U67" s="109"/>
-      <c r="V67" s="109"/>
-      <c r="W67" s="109"/>
-      <c r="X67" s="109"/>
-      <c r="Y67" s="109"/>
-      <c r="Z67" s="109"/>
-      <c r="AA67" s="109"/>
-      <c r="AB67" s="109"/>
-      <c r="AC67" s="109"/>
-      <c r="AD67" s="109"/>
+      <c r="R67" s="116"/>
+      <c r="S67" s="116"/>
+      <c r="T67" s="116"/>
+      <c r="U67" s="116"/>
+      <c r="V67" s="116"/>
+      <c r="W67" s="116"/>
+      <c r="X67" s="116"/>
+      <c r="Y67" s="116"/>
+      <c r="Z67" s="116"/>
+      <c r="AA67" s="116"/>
+      <c r="AB67" s="116"/>
+      <c r="AC67" s="116"/>
+      <c r="AD67" s="116"/>
     </row>
     <row r="68" spans="2:30">
-      <c r="B68" s="109"/>
-      <c r="C68" s="109"/>
-      <c r="D68" s="109"/>
-      <c r="E68" s="109"/>
-      <c r="F68" s="109"/>
-      <c r="G68" s="109"/>
-      <c r="H68" s="109"/>
-      <c r="I68" s="109"/>
-      <c r="J68" s="109"/>
-      <c r="K68" s="109"/>
-      <c r="L68" s="109"/>
-      <c r="M68" s="109"/>
-      <c r="N68" s="109"/>
-      <c r="O68" s="109"/>
-      <c r="Q68" s="109"/>
-      <c r="R68" s="109"/>
-      <c r="S68" s="109"/>
-      <c r="T68" s="109"/>
-      <c r="U68" s="109"/>
-      <c r="V68" s="109"/>
-      <c r="W68" s="109"/>
-      <c r="X68" s="109"/>
-      <c r="Y68" s="109"/>
-      <c r="Z68" s="109"/>
-      <c r="AA68" s="109"/>
-      <c r="AB68" s="109"/>
-      <c r="AC68" s="109"/>
-      <c r="AD68" s="109"/>
+      <c r="B68" s="116"/>
+      <c r="C68" s="116"/>
+      <c r="D68" s="116"/>
+      <c r="E68" s="116"/>
+      <c r="F68" s="116"/>
+      <c r="G68" s="116"/>
+      <c r="H68" s="116"/>
+      <c r="I68" s="116"/>
+      <c r="J68" s="116"/>
+      <c r="K68" s="116"/>
+      <c r="L68" s="116"/>
+      <c r="M68" s="116"/>
+      <c r="N68" s="116"/>
+      <c r="O68" s="116"/>
+      <c r="Q68" s="116"/>
+      <c r="R68" s="116"/>
+      <c r="S68" s="116"/>
+      <c r="T68" s="116"/>
+      <c r="U68" s="116"/>
+      <c r="V68" s="116"/>
+      <c r="W68" s="116"/>
+      <c r="X68" s="116"/>
+      <c r="Y68" s="116"/>
+      <c r="Z68" s="116"/>
+      <c r="AA68" s="116"/>
+      <c r="AB68" s="116"/>
+      <c r="AC68" s="116"/>
+      <c r="AD68" s="116"/>
     </row>
     <row r="69" spans="2:30">
-      <c r="Q69" s="109"/>
-      <c r="R69" s="109"/>
-      <c r="S69" s="109"/>
-      <c r="T69" s="109"/>
-      <c r="U69" s="109"/>
-      <c r="V69" s="109"/>
-      <c r="W69" s="109"/>
-      <c r="X69" s="109"/>
-      <c r="Y69" s="109"/>
-      <c r="Z69" s="109"/>
-      <c r="AA69" s="109"/>
-      <c r="AB69" s="109"/>
-      <c r="AC69" s="109"/>
-      <c r="AD69" s="109"/>
+      <c r="Q69" s="116"/>
+      <c r="R69" s="116"/>
+      <c r="S69" s="116"/>
+      <c r="T69" s="116"/>
+      <c r="U69" s="116"/>
+      <c r="V69" s="116"/>
+      <c r="W69" s="116"/>
+      <c r="X69" s="116"/>
+      <c r="Y69" s="116"/>
+      <c r="Z69" s="116"/>
+      <c r="AA69" s="116"/>
+      <c r="AB69" s="116"/>
+      <c r="AC69" s="116"/>
+      <c r="AD69" s="116"/>
     </row>
     <row r="70" spans="2:30" ht="17.25">
       <c r="B70" s="10" t="s">
@@ -4107,207 +4127,196 @@
       </c>
     </row>
     <row r="73" spans="2:30">
-      <c r="Q73" s="110" t="s">
+      <c r="Q73" s="113" t="s">
         <v>203</v>
       </c>
-      <c r="R73" s="110"/>
-      <c r="S73" s="110"/>
-      <c r="T73" s="110"/>
-      <c r="U73" s="110"/>
-      <c r="V73" s="110"/>
-      <c r="W73" s="110"/>
-      <c r="X73" s="110"/>
-      <c r="Y73" s="110"/>
-      <c r="Z73" s="110"/>
-      <c r="AA73" s="110"/>
-      <c r="AB73" s="110"/>
-      <c r="AC73" s="110"/>
-      <c r="AD73" s="110"/>
+      <c r="R73" s="113"/>
+      <c r="S73" s="113"/>
+      <c r="T73" s="113"/>
+      <c r="U73" s="113"/>
+      <c r="V73" s="113"/>
+      <c r="W73" s="113"/>
+      <c r="X73" s="113"/>
+      <c r="Y73" s="113"/>
+      <c r="Z73" s="113"/>
+      <c r="AA73" s="113"/>
+      <c r="AB73" s="113"/>
+      <c r="AC73" s="113"/>
+      <c r="AD73" s="113"/>
     </row>
     <row r="74" spans="2:30">
-      <c r="Q74" s="110"/>
-      <c r="R74" s="110"/>
-      <c r="S74" s="110"/>
-      <c r="T74" s="110"/>
-      <c r="U74" s="110"/>
-      <c r="V74" s="110"/>
-      <c r="W74" s="110"/>
-      <c r="X74" s="110"/>
-      <c r="Y74" s="110"/>
-      <c r="Z74" s="110"/>
-      <c r="AA74" s="110"/>
-      <c r="AB74" s="110"/>
-      <c r="AC74" s="110"/>
-      <c r="AD74" s="110"/>
+      <c r="Q74" s="113"/>
+      <c r="R74" s="113"/>
+      <c r="S74" s="113"/>
+      <c r="T74" s="113"/>
+      <c r="U74" s="113"/>
+      <c r="V74" s="113"/>
+      <c r="W74" s="113"/>
+      <c r="X74" s="113"/>
+      <c r="Y74" s="113"/>
+      <c r="Z74" s="113"/>
+      <c r="AA74" s="113"/>
+      <c r="AB74" s="113"/>
+      <c r="AC74" s="113"/>
+      <c r="AD74" s="113"/>
     </row>
     <row r="75" spans="2:30" ht="15" customHeight="1">
-      <c r="Q75" s="110"/>
-      <c r="R75" s="110"/>
-      <c r="S75" s="110"/>
-      <c r="T75" s="110"/>
-      <c r="U75" s="110"/>
-      <c r="V75" s="110"/>
-      <c r="W75" s="110"/>
-      <c r="X75" s="110"/>
-      <c r="Y75" s="110"/>
-      <c r="Z75" s="110"/>
-      <c r="AA75" s="110"/>
-      <c r="AB75" s="110"/>
-      <c r="AC75" s="110"/>
-      <c r="AD75" s="110"/>
+      <c r="Q75" s="113"/>
+      <c r="R75" s="113"/>
+      <c r="S75" s="113"/>
+      <c r="T75" s="113"/>
+      <c r="U75" s="113"/>
+      <c r="V75" s="113"/>
+      <c r="W75" s="113"/>
+      <c r="X75" s="113"/>
+      <c r="Y75" s="113"/>
+      <c r="Z75" s="113"/>
+      <c r="AA75" s="113"/>
+      <c r="AB75" s="113"/>
+      <c r="AC75" s="113"/>
+      <c r="AD75" s="113"/>
     </row>
     <row r="76" spans="2:30">
-      <c r="Q76" s="110"/>
-      <c r="R76" s="110"/>
-      <c r="S76" s="110"/>
-      <c r="T76" s="110"/>
-      <c r="U76" s="110"/>
-      <c r="V76" s="110"/>
-      <c r="W76" s="110"/>
-      <c r="X76" s="110"/>
-      <c r="Y76" s="110"/>
-      <c r="Z76" s="110"/>
-      <c r="AA76" s="110"/>
-      <c r="AB76" s="110"/>
-      <c r="AC76" s="110"/>
-      <c r="AD76" s="110"/>
+      <c r="Q76" s="113"/>
+      <c r="R76" s="113"/>
+      <c r="S76" s="113"/>
+      <c r="T76" s="113"/>
+      <c r="U76" s="113"/>
+      <c r="V76" s="113"/>
+      <c r="W76" s="113"/>
+      <c r="X76" s="113"/>
+      <c r="Y76" s="113"/>
+      <c r="Z76" s="113"/>
+      <c r="AA76" s="113"/>
+      <c r="AB76" s="113"/>
+      <c r="AC76" s="113"/>
+      <c r="AD76" s="113"/>
     </row>
     <row r="77" spans="2:30">
-      <c r="Q77" s="110"/>
-      <c r="R77" s="110"/>
-      <c r="S77" s="110"/>
-      <c r="T77" s="110"/>
-      <c r="U77" s="110"/>
-      <c r="V77" s="110"/>
-      <c r="W77" s="110"/>
-      <c r="X77" s="110"/>
-      <c r="Y77" s="110"/>
-      <c r="Z77" s="110"/>
-      <c r="AA77" s="110"/>
-      <c r="AB77" s="110"/>
-      <c r="AC77" s="110"/>
-      <c r="AD77" s="110"/>
+      <c r="Q77" s="113"/>
+      <c r="R77" s="113"/>
+      <c r="S77" s="113"/>
+      <c r="T77" s="113"/>
+      <c r="U77" s="113"/>
+      <c r="V77" s="113"/>
+      <c r="W77" s="113"/>
+      <c r="X77" s="113"/>
+      <c r="Y77" s="113"/>
+      <c r="Z77" s="113"/>
+      <c r="AA77" s="113"/>
+      <c r="AB77" s="113"/>
+      <c r="AC77" s="113"/>
+      <c r="AD77" s="113"/>
     </row>
     <row r="79" spans="2:30" ht="17.25">
-      <c r="B79" s="117" t="s">
+      <c r="B79" s="111" t="s">
         <v>101</v>
       </c>
-      <c r="C79" s="117"/>
-      <c r="D79" s="117"/>
-      <c r="E79" s="117"/>
-      <c r="F79" s="117"/>
-      <c r="G79" s="117"/>
-      <c r="H79" s="117"/>
-      <c r="I79" s="117"/>
-      <c r="J79" s="117"/>
-      <c r="K79" s="117"/>
-      <c r="L79" s="117"/>
-      <c r="M79" s="117"/>
-      <c r="N79" s="117"/>
-      <c r="O79" s="117"/>
+      <c r="C79" s="111"/>
+      <c r="D79" s="111"/>
+      <c r="E79" s="111"/>
+      <c r="F79" s="111"/>
+      <c r="G79" s="111"/>
+      <c r="H79" s="111"/>
+      <c r="I79" s="111"/>
+      <c r="J79" s="111"/>
+      <c r="K79" s="111"/>
+      <c r="L79" s="111"/>
+      <c r="M79" s="111"/>
+      <c r="N79" s="111"/>
+      <c r="O79" s="111"/>
       <c r="Q79" s="20" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="81" spans="2:30" ht="15" customHeight="1">
-      <c r="B81" s="109" t="s">
+      <c r="B81" s="116" t="s">
         <v>193</v>
       </c>
-      <c r="C81" s="109"/>
-      <c r="D81" s="109"/>
-      <c r="E81" s="109"/>
-      <c r="F81" s="109"/>
-      <c r="G81" s="109"/>
-      <c r="H81" s="109"/>
-      <c r="I81" s="109"/>
-      <c r="J81" s="109"/>
-      <c r="K81" s="109"/>
-      <c r="L81" s="109"/>
-      <c r="M81" s="109"/>
-      <c r="N81" s="109"/>
-      <c r="O81" s="109"/>
-      <c r="Q81" s="110" t="s">
+      <c r="C81" s="116"/>
+      <c r="D81" s="116"/>
+      <c r="E81" s="116"/>
+      <c r="F81" s="116"/>
+      <c r="G81" s="116"/>
+      <c r="H81" s="116"/>
+      <c r="I81" s="116"/>
+      <c r="J81" s="116"/>
+      <c r="K81" s="116"/>
+      <c r="L81" s="116"/>
+      <c r="M81" s="116"/>
+      <c r="N81" s="116"/>
+      <c r="O81" s="116"/>
+      <c r="Q81" s="113" t="s">
         <v>202</v>
       </c>
-      <c r="R81" s="110"/>
-      <c r="S81" s="110"/>
-      <c r="T81" s="110"/>
-      <c r="U81" s="110"/>
-      <c r="V81" s="110"/>
-      <c r="W81" s="110"/>
-      <c r="X81" s="110"/>
-      <c r="Y81" s="110"/>
-      <c r="Z81" s="110"/>
-      <c r="AA81" s="110"/>
-      <c r="AB81" s="110"/>
-      <c r="AC81" s="110"/>
-      <c r="AD81" s="110"/>
+      <c r="R81" s="113"/>
+      <c r="S81" s="113"/>
+      <c r="T81" s="113"/>
+      <c r="U81" s="113"/>
+      <c r="V81" s="113"/>
+      <c r="W81" s="113"/>
+      <c r="X81" s="113"/>
+      <c r="Y81" s="113"/>
+      <c r="Z81" s="113"/>
+      <c r="AA81" s="113"/>
+      <c r="AB81" s="113"/>
+      <c r="AC81" s="113"/>
+      <c r="AD81" s="113"/>
     </row>
     <row r="82" spans="2:30">
-      <c r="B82" s="109"/>
-      <c r="C82" s="109"/>
-      <c r="D82" s="109"/>
-      <c r="E82" s="109"/>
-      <c r="F82" s="109"/>
-      <c r="G82" s="109"/>
-      <c r="H82" s="109"/>
-      <c r="I82" s="109"/>
-      <c r="J82" s="109"/>
-      <c r="K82" s="109"/>
-      <c r="L82" s="109"/>
-      <c r="M82" s="109"/>
-      <c r="N82" s="109"/>
-      <c r="O82" s="109"/>
-      <c r="Q82" s="110"/>
-      <c r="R82" s="110"/>
-      <c r="S82" s="110"/>
-      <c r="T82" s="110"/>
-      <c r="U82" s="110"/>
-      <c r="V82" s="110"/>
-      <c r="W82" s="110"/>
-      <c r="X82" s="110"/>
-      <c r="Y82" s="110"/>
-      <c r="Z82" s="110"/>
-      <c r="AA82" s="110"/>
-      <c r="AB82" s="110"/>
-      <c r="AC82" s="110"/>
-      <c r="AD82" s="110"/>
+      <c r="B82" s="116"/>
+      <c r="C82" s="116"/>
+      <c r="D82" s="116"/>
+      <c r="E82" s="116"/>
+      <c r="F82" s="116"/>
+      <c r="G82" s="116"/>
+      <c r="H82" s="116"/>
+      <c r="I82" s="116"/>
+      <c r="J82" s="116"/>
+      <c r="K82" s="116"/>
+      <c r="L82" s="116"/>
+      <c r="M82" s="116"/>
+      <c r="N82" s="116"/>
+      <c r="O82" s="116"/>
+      <c r="Q82" s="113"/>
+      <c r="R82" s="113"/>
+      <c r="S82" s="113"/>
+      <c r="T82" s="113"/>
+      <c r="U82" s="113"/>
+      <c r="V82" s="113"/>
+      <c r="W82" s="113"/>
+      <c r="X82" s="113"/>
+      <c r="Y82" s="113"/>
+      <c r="Z82" s="113"/>
+      <c r="AA82" s="113"/>
+      <c r="AB82" s="113"/>
+      <c r="AC82" s="113"/>
+      <c r="AD82" s="113"/>
     </row>
     <row r="83" spans="2:30">
-      <c r="Q83" s="110"/>
-      <c r="R83" s="110"/>
-      <c r="S83" s="110"/>
-      <c r="T83" s="110"/>
-      <c r="U83" s="110"/>
-      <c r="V83" s="110"/>
-      <c r="W83" s="110"/>
-      <c r="X83" s="110"/>
-      <c r="Y83" s="110"/>
-      <c r="Z83" s="110"/>
-      <c r="AA83" s="110"/>
-      <c r="AB83" s="110"/>
-      <c r="AC83" s="110"/>
-      <c r="AD83" s="110"/>
+      <c r="Q83" s="113"/>
+      <c r="R83" s="113"/>
+      <c r="S83" s="113"/>
+      <c r="T83" s="113"/>
+      <c r="U83" s="113"/>
+      <c r="V83" s="113"/>
+      <c r="W83" s="113"/>
+      <c r="X83" s="113"/>
+      <c r="Y83" s="113"/>
+      <c r="Z83" s="113"/>
+      <c r="AA83" s="113"/>
+      <c r="AB83" s="113"/>
+      <c r="AC83" s="113"/>
+      <c r="AD83" s="113"/>
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="B58:O58"/>
-    <mergeCell ref="B79:O79"/>
-    <mergeCell ref="Q58:AD58"/>
-    <mergeCell ref="B60:O61"/>
-    <mergeCell ref="V48:Z48"/>
-    <mergeCell ref="S50:AB50"/>
-    <mergeCell ref="Q67:AD69"/>
-    <mergeCell ref="B50:O51"/>
-    <mergeCell ref="S33:AB34"/>
-    <mergeCell ref="S37:AB38"/>
-    <mergeCell ref="S42:AB42"/>
-    <mergeCell ref="S45:AB46"/>
-    <mergeCell ref="B55:O56"/>
-    <mergeCell ref="B33:N34"/>
-    <mergeCell ref="B38:O39"/>
-    <mergeCell ref="B41:O41"/>
-    <mergeCell ref="B45:O46"/>
+    <mergeCell ref="B81:O82"/>
+    <mergeCell ref="Q62:AD63"/>
+    <mergeCell ref="B63:O66"/>
+    <mergeCell ref="B67:O68"/>
+    <mergeCell ref="Q73:AD77"/>
+    <mergeCell ref="Q81:AD83"/>
     <mergeCell ref="B2:O2"/>
     <mergeCell ref="B4:O5"/>
     <mergeCell ref="B8:O9"/>
@@ -4324,12 +4333,23 @@
     <mergeCell ref="V40:Z40"/>
     <mergeCell ref="S29:AB29"/>
     <mergeCell ref="S26:AB26"/>
-    <mergeCell ref="B81:O82"/>
-    <mergeCell ref="Q62:AD63"/>
-    <mergeCell ref="B63:O66"/>
-    <mergeCell ref="B67:O68"/>
-    <mergeCell ref="Q73:AD77"/>
-    <mergeCell ref="Q81:AD83"/>
+    <mergeCell ref="S33:AB34"/>
+    <mergeCell ref="S37:AB38"/>
+    <mergeCell ref="S42:AB42"/>
+    <mergeCell ref="S45:AB46"/>
+    <mergeCell ref="B55:O56"/>
+    <mergeCell ref="B33:N34"/>
+    <mergeCell ref="B38:O39"/>
+    <mergeCell ref="B41:O41"/>
+    <mergeCell ref="B45:O46"/>
+    <mergeCell ref="B58:O58"/>
+    <mergeCell ref="B79:O79"/>
+    <mergeCell ref="Q58:AD58"/>
+    <mergeCell ref="B60:O61"/>
+    <mergeCell ref="V48:Z48"/>
+    <mergeCell ref="S50:AB50"/>
+    <mergeCell ref="Q67:AD69"/>
+    <mergeCell ref="B50:O51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4342,88 +4362,143 @@
   <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A4:B12"/>
+  <dimension ref="A4:C16"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:B21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:2" ht="15.75" thickBot="1">
+    <row r="4" spans="1:3" ht="15.75" thickBot="1">
       <c r="A4" s="101" t="s">
         <v>228</v>
       </c>
       <c r="B4" s="101" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.75" thickTop="1">
-      <c r="A5" t="s">
+      <c r="C4" s="101" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" thickTop="1">
+      <c r="A5" s="129" t="s">
         <v>220</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="130">
         <v>0.4521856341365087</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
+      <c r="C5" s="129" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="129" t="s">
         <v>221</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="130">
         <v>0.38308555478780298</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
+      <c r="C6" s="129" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="129" t="s">
         <v>222</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="130">
         <v>0.39666773771891822</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
+      <c r="C7" s="129" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="129" t="s">
         <v>223</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="130">
         <v>0.43517066185236231</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
+      <c r="C8" s="129" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="129" t="s">
         <v>224</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="130">
         <v>0.37190757391651003</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
+      <c r="C9" s="129" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="129" t="s">
         <v>225</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="130">
         <v>0.47216441970460488</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
+      <c r="C10" s="129" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="129" t="s">
         <v>226</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="130">
         <v>0.33605820330095793</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
+      <c r="C11" s="129" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="129" t="s">
         <v>227</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="130">
         <v>0.62986877068882074</v>
+      </c>
+      <c r="C12" s="129" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="129" t="s">
+        <v>234</v>
+      </c>
+      <c r="B14" s="129">
+        <f>AVERAGEIF($C$5:C12,A14,$B$5:B12)</f>
+        <v>0.4436781479944355</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="129" t="s">
+        <v>235</v>
+      </c>
+      <c r="B15" s="129">
+        <f>AVERAGEIF($C$5:C13,A15,$B$5:B13)</f>
+        <v>0.36368377733509033</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="129" t="s">
+        <v>236</v>
+      </c>
+      <c r="B16" s="129">
+        <f>AVERAGEIF($C$5:C14,A16,$B$5:B14)</f>
+        <v>0.49956697603744793</v>
       </c>
     </row>
   </sheetData>
@@ -72473,8 +72548,8 @@
   </sheetPr>
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -72516,17 +72591,17 @@
         <f>Regiones!B2</f>
         <v>Interior de Buenos Aires</v>
       </c>
-      <c r="C2" s="127">
+      <c r="C2" s="109">
         <v>31049</v>
       </c>
-      <c r="D2" s="127">
+      <c r="D2" s="109">
         <v>1226</v>
       </c>
-      <c r="E2" s="127">
+      <c r="E2" s="109">
         <v>886</v>
       </c>
-      <c r="G2" s="41">
-        <v>2000</v>
+      <c r="G2" s="109">
+        <v>299</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -72538,17 +72613,17 @@
         <f>Regiones!B3</f>
         <v>24 Partidos del Gran Buenos Aires</v>
       </c>
-      <c r="C3" s="127">
+      <c r="C3" s="109">
         <v>53940</v>
       </c>
-      <c r="D3" s="127">
+      <c r="D3" s="109">
         <v>2130</v>
       </c>
-      <c r="E3" s="128">
+      <c r="E3" s="110">
         <v>1539</v>
       </c>
-      <c r="G3" s="41">
-        <v>2000</v>
+      <c r="G3" s="109">
+        <v>520</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -72560,17 +72635,17 @@
         <f>Regiones!B4</f>
         <v>Córdoba</v>
       </c>
-      <c r="C4" s="127">
+      <c r="C4" s="109">
         <v>17998</v>
       </c>
-      <c r="D4" s="127">
+      <c r="D4" s="109">
         <v>710</v>
       </c>
-      <c r="E4" s="127">
+      <c r="E4" s="109">
         <v>513</v>
       </c>
-      <c r="G4" s="41">
-        <v>2000</v>
+      <c r="G4" s="109">
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -72582,17 +72657,17 @@
         <f>Regiones!B5</f>
         <v>Santa Fe</v>
       </c>
-      <c r="C5" s="127">
+      <c r="C5" s="109">
         <v>17376</v>
       </c>
-      <c r="D5" s="127">
+      <c r="D5" s="109">
         <v>686</v>
       </c>
-      <c r="E5" s="127">
+      <c r="E5" s="109">
         <v>496</v>
       </c>
-      <c r="G5" s="41">
-        <v>2000</v>
+      <c r="G5" s="109">
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -72604,17 +72679,17 @@
         <f>Regiones!B6</f>
         <v>Ciudad de Buenos Aires</v>
       </c>
-      <c r="C6" s="127">
+      <c r="C6" s="109">
         <v>15720</v>
       </c>
-      <c r="D6" s="127">
+      <c r="D6" s="109">
         <v>620</v>
       </c>
-      <c r="E6" s="127">
+      <c r="E6" s="109">
         <v>448</v>
       </c>
-      <c r="G6" s="41">
-        <v>2000</v>
+      <c r="G6" s="109">
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -72626,17 +72701,17 @@
         <f>Regiones!B7</f>
         <v>Mendoza</v>
       </c>
-      <c r="C7" s="127">
+      <c r="C7" s="109">
         <v>5557</v>
       </c>
-      <c r="D7" s="127">
+      <c r="D7" s="109">
         <v>228</v>
       </c>
-      <c r="E7" s="127">
+      <c r="E7" s="109">
         <v>165</v>
       </c>
-      <c r="G7" s="41">
-        <v>2000</v>
+      <c r="G7" s="109">
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -72648,17 +72723,17 @@
         <f>Regiones!B8</f>
         <v>Tucumán</v>
       </c>
-      <c r="C8" s="127">
+      <c r="C8" s="109">
         <v>4494</v>
       </c>
-      <c r="D8" s="127">
+      <c r="D8" s="109">
         <v>334</v>
       </c>
-      <c r="E8" s="127">
+      <c r="E8" s="109">
         <v>242</v>
       </c>
-      <c r="G8" s="41">
-        <v>2000</v>
+      <c r="G8" s="109">
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -72670,17 +72745,17 @@
         <f>Regiones!B9</f>
         <v>Entre Ríos</v>
       </c>
-      <c r="C9" s="127">
+      <c r="C9" s="109">
         <v>6723</v>
       </c>
-      <c r="D9" s="127">
+      <c r="D9" s="109">
         <v>265</v>
       </c>
-      <c r="E9" s="127">
+      <c r="E9" s="109">
         <v>192</v>
       </c>
-      <c r="G9" s="41">
-        <v>2000</v>
+      <c r="G9" s="109">
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -72692,17 +72767,17 @@
         <f>Regiones!B10</f>
         <v>Salta</v>
       </c>
-      <c r="C10" s="127">
+      <c r="C10" s="109">
         <v>3769</v>
       </c>
-      <c r="D10" s="127">
+      <c r="D10" s="109">
         <v>280</v>
       </c>
-      <c r="E10" s="127">
+      <c r="E10" s="109">
         <v>203</v>
       </c>
-      <c r="G10" s="41">
-        <v>2000</v>
+      <c r="G10" s="109">
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -72714,17 +72789,17 @@
         <f>Regiones!B11</f>
         <v>Misiones</v>
       </c>
-      <c r="C11" s="127">
+      <c r="C11" s="109">
         <v>3315</v>
       </c>
-      <c r="D11" s="127">
+      <c r="D11" s="109">
         <v>215</v>
       </c>
-      <c r="E11" s="127">
+      <c r="E11" s="109">
         <v>156</v>
       </c>
-      <c r="G11" s="41">
-        <v>2000</v>
+      <c r="G11" s="109">
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -72736,17 +72811,17 @@
         <f>Regiones!B12</f>
         <v>Chaco</v>
       </c>
-      <c r="C12" s="127">
+      <c r="C12" s="109">
         <v>3176</v>
       </c>
-      <c r="D12" s="127">
+      <c r="D12" s="109">
         <v>206</v>
       </c>
-      <c r="E12" s="127">
+      <c r="E12" s="109">
         <v>149</v>
       </c>
-      <c r="G12" s="41">
-        <v>2000</v>
+      <c r="G12" s="109">
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -72758,17 +72833,17 @@
         <f>Regiones!B13</f>
         <v>Corrientes</v>
       </c>
-      <c r="C13" s="127">
+      <c r="C13" s="109">
         <v>2987</v>
       </c>
-      <c r="D13" s="127">
+      <c r="D13" s="109">
         <v>194</v>
       </c>
-      <c r="E13" s="127">
+      <c r="E13" s="109">
         <v>141</v>
       </c>
-      <c r="G13" s="41">
-        <v>2000</v>
+      <c r="G13" s="109">
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -72780,17 +72855,17 @@
         <f>Regiones!B14</f>
         <v>Santiago del Estero</v>
       </c>
-      <c r="C14" s="127">
+      <c r="C14" s="109">
         <v>2712</v>
       </c>
-      <c r="D14" s="127">
+      <c r="D14" s="109">
         <v>201</v>
       </c>
-      <c r="E14" s="127">
+      <c r="E14" s="109">
         <v>146</v>
       </c>
-      <c r="G14" s="41">
-        <v>2000</v>
+      <c r="G14" s="109">
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -72802,17 +72877,17 @@
         <f>Regiones!B15</f>
         <v>San Juan</v>
       </c>
-      <c r="C15" s="127">
+      <c r="C15" s="109">
         <v>2176</v>
       </c>
-      <c r="D15" s="127">
+      <c r="D15" s="109">
         <v>89</v>
       </c>
-      <c r="E15" s="127">
+      <c r="E15" s="109">
         <v>65</v>
       </c>
-      <c r="G15" s="41">
-        <v>2000</v>
+      <c r="G15" s="109">
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -72824,17 +72899,17 @@
         <f>Regiones!B16</f>
         <v>Jujuy</v>
       </c>
-      <c r="C16" s="127">
+      <c r="C16" s="109">
         <v>2089</v>
       </c>
-      <c r="D16" s="127">
+      <c r="D16" s="109">
         <v>155</v>
       </c>
-      <c r="E16" s="127">
+      <c r="E16" s="109">
         <v>112</v>
       </c>
-      <c r="G16" s="41">
-        <v>2000</v>
+      <c r="G16" s="109">
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -72846,17 +72921,17 @@
         <f>Regiones!B17</f>
         <v>Río Negro</v>
       </c>
-      <c r="C17" s="127">
+      <c r="C17" s="109">
         <v>1901</v>
       </c>
-      <c r="D17" s="127">
+      <c r="D17" s="109">
         <v>111</v>
       </c>
-      <c r="E17" s="127">
+      <c r="E17" s="109">
         <v>81</v>
       </c>
-      <c r="G17" s="41">
-        <v>2000</v>
+      <c r="G17" s="109">
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -72868,17 +72943,17 @@
         <f>Regiones!B18</f>
         <v>Neuquén</v>
       </c>
-      <c r="C18" s="127">
+      <c r="C18" s="109">
         <v>1641</v>
       </c>
-      <c r="D18" s="127">
+      <c r="D18" s="109">
         <v>96</v>
       </c>
-      <c r="E18" s="127">
+      <c r="E18" s="109">
         <v>70</v>
       </c>
-      <c r="G18" s="41">
-        <v>2000</v>
+      <c r="G18" s="109">
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -72890,17 +72965,17 @@
         <f>Regiones!B19</f>
         <v>Formosa</v>
       </c>
-      <c r="C19" s="127">
+      <c r="C19" s="109">
         <v>1595</v>
       </c>
-      <c r="D19" s="127">
+      <c r="D19" s="109">
         <v>103</v>
       </c>
-      <c r="E19" s="127">
+      <c r="E19" s="109">
         <v>75</v>
       </c>
-      <c r="G19" s="41">
-        <v>2000</v>
+      <c r="G19" s="109">
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -72912,17 +72987,17 @@
         <f>Regiones!B20</f>
         <v>Chubut</v>
       </c>
-      <c r="C20" s="127">
+      <c r="C20" s="109">
         <v>1515</v>
       </c>
-      <c r="D20" s="127">
+      <c r="D20" s="109">
         <v>89</v>
       </c>
-      <c r="E20" s="127">
+      <c r="E20" s="109">
         <v>65</v>
       </c>
-      <c r="G20" s="41">
-        <v>2000</v>
+      <c r="G20" s="109">
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -72934,17 +73009,17 @@
         <f>Regiones!B21</f>
         <v>San Luis</v>
       </c>
-      <c r="C21" s="127">
+      <c r="C21" s="109">
         <v>1381</v>
       </c>
-      <c r="D21" s="127">
+      <c r="D21" s="109">
         <v>56</v>
       </c>
-      <c r="E21" s="127">
+      <c r="E21" s="109">
         <v>41</v>
       </c>
-      <c r="G21" s="41">
-        <v>2000</v>
+      <c r="G21" s="109">
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -72956,17 +73031,17 @@
         <f>Regiones!B22</f>
         <v>Catamarca</v>
       </c>
-      <c r="C22" s="127">
+      <c r="C22" s="109">
         <v>1141</v>
       </c>
-      <c r="D22" s="127">
+      <c r="D22" s="109">
         <v>84</v>
       </c>
-      <c r="E22" s="127">
+      <c r="E22" s="109">
         <v>61</v>
       </c>
-      <c r="G22" s="41">
-        <v>2000</v>
+      <c r="G22" s="109">
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -72978,17 +73053,17 @@
         <f>Regiones!B23</f>
         <v>La Rioja</v>
       </c>
-      <c r="C23" s="127">
+      <c r="C23" s="109">
         <v>1035</v>
       </c>
-      <c r="D23" s="127">
+      <c r="D23" s="109">
         <v>77</v>
       </c>
-      <c r="E23" s="127">
+      <c r="E23" s="109">
         <v>56</v>
       </c>
-      <c r="G23" s="41">
-        <v>2000</v>
+      <c r="G23" s="109">
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -73000,17 +73075,17 @@
         <f>Regiones!B24</f>
         <v>La Pampa</v>
       </c>
-      <c r="C24" s="127">
+      <c r="C24" s="109">
         <v>949</v>
       </c>
-      <c r="D24" s="127">
+      <c r="D24" s="109">
         <v>55</v>
       </c>
-      <c r="E24" s="127">
+      <c r="E24" s="109">
         <v>40</v>
       </c>
-      <c r="G24" s="41">
-        <v>2000</v>
+      <c r="G24" s="109">
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -73022,17 +73097,17 @@
         <f>Regiones!B25</f>
         <v>Santa Cruz</v>
       </c>
-      <c r="C25" s="127">
+      <c r="C25" s="109">
         <v>815</v>
       </c>
-      <c r="D25" s="127">
+      <c r="D25" s="109">
         <v>48</v>
       </c>
-      <c r="E25" s="127">
+      <c r="E25" s="109">
         <v>35</v>
       </c>
-      <c r="G25" s="41">
-        <v>2000</v>
+      <c r="G25" s="109">
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -73044,17 +73119,17 @@
         <f>Regiones!B26</f>
         <v>Tierra del Fuego</v>
       </c>
-      <c r="C26" s="127">
+      <c r="C26" s="109">
         <v>378</v>
       </c>
-      <c r="D26" s="127">
+      <c r="D26" s="109">
         <v>22</v>
       </c>
-      <c r="E26" s="127">
+      <c r="E26" s="109">
         <v>16</v>
       </c>
-      <c r="G26" s="41">
-        <v>2000</v>
+      <c r="G26" s="109">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>